<commit_message>
work logs so far
more to come.
</commit_message>
<xml_diff>
--- a/Documents/WorkLogs/JoshuaFord_workLog.xlsx
+++ b/Documents/WorkLogs/JoshuaFord_workLog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Ford\Documents\GitHub\tune_squad\tune_squad\Documents\WorkLogs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Ford\Documents\GitHub\tune_squad\Documents\WorkLogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>Worked to apply plan B to the compression algorithm.</t>
+  </si>
+  <si>
+    <t>decided on positions and talked about meeting times.</t>
+  </si>
+  <si>
+    <t>descussed the method of team communication, repo, and team names.</t>
+  </si>
+  <si>
+    <t>formulated questions for customer.</t>
+  </si>
+  <si>
+    <t>worked on a development model, learned folder structure, schedule customer meeting.</t>
+  </si>
+  <si>
+    <t>finish question list, choose a method to use</t>
   </si>
 </sst>
 </file>
@@ -634,7 +649,7 @@
   <dimension ref="A1:I1995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -703,7 +718,7 @@
       </c>
       <c r="I4" s="11">
         <f>SUM(G4:G2000)</f>
-        <v>34.25</v>
+        <v>39.25</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
@@ -842,132 +857,172 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
+      <c r="A14" s="9">
+        <v>42024</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
+      <c r="G14" s="6">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
+      <c r="A15" s="9">
+        <v>42025</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
+      <c r="G15" s="6">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="12"/>
+      <c r="A16" s="9">
+        <v>42032</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
+      <c r="G16" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>42034</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="9">
+        <v>42037</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -14717,1980 +14772,6 @@
     </row>
   </sheetData>
   <mergeCells count="1995">
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B109:F109"/>
-    <mergeCell ref="B110:F110"/>
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="B105:F105"/>
-    <mergeCell ref="B106:F106"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B127:F127"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B121:F121"/>
-    <mergeCell ref="B122:F122"/>
-    <mergeCell ref="B123:F123"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B151:F151"/>
-    <mergeCell ref="B152:F152"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B154:F154"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B156:F156"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B150:F150"/>
-    <mergeCell ref="B139:F139"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B169:F169"/>
-    <mergeCell ref="B170:F170"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B173:F173"/>
-    <mergeCell ref="B174:F174"/>
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B165:F165"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B168:F168"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B160:F160"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B187:F187"/>
-    <mergeCell ref="B188:F188"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B190:F190"/>
-    <mergeCell ref="B191:F191"/>
-    <mergeCell ref="B192:F192"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B175:F175"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B178:F178"/>
-    <mergeCell ref="B179:F179"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B209:F209"/>
-    <mergeCell ref="B210:F210"/>
-    <mergeCell ref="B199:F199"/>
-    <mergeCell ref="B200:F200"/>
-    <mergeCell ref="B201:F201"/>
-    <mergeCell ref="B202:F202"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B204:F204"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B194:F194"/>
-    <mergeCell ref="B195:F195"/>
-    <mergeCell ref="B196:F196"/>
-    <mergeCell ref="B197:F197"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B224:F224"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="B226:F226"/>
-    <mergeCell ref="B227:F227"/>
-    <mergeCell ref="B228:F228"/>
-    <mergeCell ref="B217:F217"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B219:F219"/>
-    <mergeCell ref="B220:F220"/>
-    <mergeCell ref="B221:F221"/>
-    <mergeCell ref="B222:F222"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B212:F212"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B214:F214"/>
-    <mergeCell ref="B215:F215"/>
-    <mergeCell ref="B216:F216"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B246:F246"/>
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B236:F236"/>
-    <mergeCell ref="B237:F237"/>
-    <mergeCell ref="B238:F238"/>
-    <mergeCell ref="B239:F239"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="B230:F230"/>
-    <mergeCell ref="B231:F231"/>
-    <mergeCell ref="B232:F232"/>
-    <mergeCell ref="B233:F233"/>
-    <mergeCell ref="B234:F234"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B264:F264"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B247:F247"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B282:F282"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="B275:F275"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="B265:F265"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B296:F296"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B299:F299"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="B289:F289"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B292:F292"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="B288:F288"/>
-    <mergeCell ref="B313:F313"/>
-    <mergeCell ref="B314:F314"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="B311:F311"/>
-    <mergeCell ref="B312:F312"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B306:F306"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B335:F335"/>
-    <mergeCell ref="B336:F336"/>
-    <mergeCell ref="B325:F325"/>
-    <mergeCell ref="B326:F326"/>
-    <mergeCell ref="B327:F327"/>
-    <mergeCell ref="B328:F328"/>
-    <mergeCell ref="B329:F329"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B320:F320"/>
-    <mergeCell ref="B321:F321"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="B323:F323"/>
-    <mergeCell ref="B324:F324"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="B350:F350"/>
-    <mergeCell ref="B351:F351"/>
-    <mergeCell ref="B352:F352"/>
-    <mergeCell ref="B353:F353"/>
-    <mergeCell ref="B354:F354"/>
-    <mergeCell ref="B343:F343"/>
-    <mergeCell ref="B344:F344"/>
-    <mergeCell ref="B345:F345"/>
-    <mergeCell ref="B346:F346"/>
-    <mergeCell ref="B347:F347"/>
-    <mergeCell ref="B348:F348"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B339:F339"/>
-    <mergeCell ref="B340:F340"/>
-    <mergeCell ref="B341:F341"/>
-    <mergeCell ref="B342:F342"/>
-    <mergeCell ref="B367:F367"/>
-    <mergeCell ref="B368:F368"/>
-    <mergeCell ref="B369:F369"/>
-    <mergeCell ref="B370:F370"/>
-    <mergeCell ref="B371:F371"/>
-    <mergeCell ref="B372:F372"/>
-    <mergeCell ref="B361:F361"/>
-    <mergeCell ref="B362:F362"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="B364:F364"/>
-    <mergeCell ref="B365:F365"/>
-    <mergeCell ref="B366:F366"/>
-    <mergeCell ref="B355:F355"/>
-    <mergeCell ref="B356:F356"/>
-    <mergeCell ref="B357:F357"/>
-    <mergeCell ref="B358:F358"/>
-    <mergeCell ref="B359:F359"/>
-    <mergeCell ref="B360:F360"/>
-    <mergeCell ref="B385:F385"/>
-    <mergeCell ref="B386:F386"/>
-    <mergeCell ref="B387:F387"/>
-    <mergeCell ref="B388:F388"/>
-    <mergeCell ref="B389:F389"/>
-    <mergeCell ref="B390:F390"/>
-    <mergeCell ref="B379:F379"/>
-    <mergeCell ref="B380:F380"/>
-    <mergeCell ref="B381:F381"/>
-    <mergeCell ref="B382:F382"/>
-    <mergeCell ref="B383:F383"/>
-    <mergeCell ref="B384:F384"/>
-    <mergeCell ref="B373:F373"/>
-    <mergeCell ref="B374:F374"/>
-    <mergeCell ref="B375:F375"/>
-    <mergeCell ref="B376:F376"/>
-    <mergeCell ref="B377:F377"/>
-    <mergeCell ref="B378:F378"/>
-    <mergeCell ref="B403:F403"/>
-    <mergeCell ref="B404:F404"/>
-    <mergeCell ref="B405:F405"/>
-    <mergeCell ref="B406:F406"/>
-    <mergeCell ref="B407:F407"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="B397:F397"/>
-    <mergeCell ref="B398:F398"/>
-    <mergeCell ref="B399:F399"/>
-    <mergeCell ref="B400:F400"/>
-    <mergeCell ref="B401:F401"/>
-    <mergeCell ref="B402:F402"/>
-    <mergeCell ref="B391:F391"/>
-    <mergeCell ref="B392:F392"/>
-    <mergeCell ref="B393:F393"/>
-    <mergeCell ref="B394:F394"/>
-    <mergeCell ref="B395:F395"/>
-    <mergeCell ref="B396:F396"/>
-    <mergeCell ref="B421:F421"/>
-    <mergeCell ref="B422:F422"/>
-    <mergeCell ref="B423:F423"/>
-    <mergeCell ref="B424:F424"/>
-    <mergeCell ref="B425:F425"/>
-    <mergeCell ref="B426:F426"/>
-    <mergeCell ref="B415:F415"/>
-    <mergeCell ref="B416:F416"/>
-    <mergeCell ref="B417:F417"/>
-    <mergeCell ref="B418:F418"/>
-    <mergeCell ref="B419:F419"/>
-    <mergeCell ref="B420:F420"/>
-    <mergeCell ref="B409:F409"/>
-    <mergeCell ref="B410:F410"/>
-    <mergeCell ref="B411:F411"/>
-    <mergeCell ref="B412:F412"/>
-    <mergeCell ref="B413:F413"/>
-    <mergeCell ref="B414:F414"/>
-    <mergeCell ref="B439:F439"/>
-    <mergeCell ref="B440:F440"/>
-    <mergeCell ref="B441:F441"/>
-    <mergeCell ref="B442:F442"/>
-    <mergeCell ref="B443:F443"/>
-    <mergeCell ref="B444:F444"/>
-    <mergeCell ref="B433:F433"/>
-    <mergeCell ref="B434:F434"/>
-    <mergeCell ref="B435:F435"/>
-    <mergeCell ref="B436:F436"/>
-    <mergeCell ref="B437:F437"/>
-    <mergeCell ref="B438:F438"/>
-    <mergeCell ref="B427:F427"/>
-    <mergeCell ref="B428:F428"/>
-    <mergeCell ref="B429:F429"/>
-    <mergeCell ref="B430:F430"/>
-    <mergeCell ref="B431:F431"/>
-    <mergeCell ref="B432:F432"/>
-    <mergeCell ref="B457:F457"/>
-    <mergeCell ref="B458:F458"/>
-    <mergeCell ref="B459:F459"/>
-    <mergeCell ref="B460:F460"/>
-    <mergeCell ref="B461:F461"/>
-    <mergeCell ref="B462:F462"/>
-    <mergeCell ref="B451:F451"/>
-    <mergeCell ref="B452:F452"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="B454:F454"/>
-    <mergeCell ref="B455:F455"/>
-    <mergeCell ref="B456:F456"/>
-    <mergeCell ref="B445:F445"/>
-    <mergeCell ref="B446:F446"/>
-    <mergeCell ref="B447:F447"/>
-    <mergeCell ref="B448:F448"/>
-    <mergeCell ref="B449:F449"/>
-    <mergeCell ref="B450:F450"/>
-    <mergeCell ref="B475:F475"/>
-    <mergeCell ref="B476:F476"/>
-    <mergeCell ref="B477:F477"/>
-    <mergeCell ref="B478:F478"/>
-    <mergeCell ref="B479:F479"/>
-    <mergeCell ref="B480:F480"/>
-    <mergeCell ref="B469:F469"/>
-    <mergeCell ref="B470:F470"/>
-    <mergeCell ref="B471:F471"/>
-    <mergeCell ref="B472:F472"/>
-    <mergeCell ref="B473:F473"/>
-    <mergeCell ref="B474:F474"/>
-    <mergeCell ref="B463:F463"/>
-    <mergeCell ref="B464:F464"/>
-    <mergeCell ref="B465:F465"/>
-    <mergeCell ref="B466:F466"/>
-    <mergeCell ref="B467:F467"/>
-    <mergeCell ref="B468:F468"/>
-    <mergeCell ref="B493:F493"/>
-    <mergeCell ref="B494:F494"/>
-    <mergeCell ref="B495:F495"/>
-    <mergeCell ref="B496:F496"/>
-    <mergeCell ref="B497:F497"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="B487:F487"/>
-    <mergeCell ref="B488:F488"/>
-    <mergeCell ref="B489:F489"/>
-    <mergeCell ref="B490:F490"/>
-    <mergeCell ref="B491:F491"/>
-    <mergeCell ref="B492:F492"/>
-    <mergeCell ref="B481:F481"/>
-    <mergeCell ref="B482:F482"/>
-    <mergeCell ref="B483:F483"/>
-    <mergeCell ref="B484:F484"/>
-    <mergeCell ref="B485:F485"/>
-    <mergeCell ref="B486:F486"/>
-    <mergeCell ref="B511:F511"/>
-    <mergeCell ref="B512:F512"/>
-    <mergeCell ref="B513:F513"/>
-    <mergeCell ref="B514:F514"/>
-    <mergeCell ref="B515:F515"/>
-    <mergeCell ref="B516:F516"/>
-    <mergeCell ref="B505:F505"/>
-    <mergeCell ref="B506:F506"/>
-    <mergeCell ref="B507:F507"/>
-    <mergeCell ref="B508:F508"/>
-    <mergeCell ref="B509:F509"/>
-    <mergeCell ref="B510:F510"/>
-    <mergeCell ref="B499:F499"/>
-    <mergeCell ref="B500:F500"/>
-    <mergeCell ref="B501:F501"/>
-    <mergeCell ref="B502:F502"/>
-    <mergeCell ref="B503:F503"/>
-    <mergeCell ref="B504:F504"/>
-    <mergeCell ref="B529:F529"/>
-    <mergeCell ref="B530:F530"/>
-    <mergeCell ref="B531:F531"/>
-    <mergeCell ref="B532:F532"/>
-    <mergeCell ref="B533:F533"/>
-    <mergeCell ref="B534:F534"/>
-    <mergeCell ref="B523:F523"/>
-    <mergeCell ref="B524:F524"/>
-    <mergeCell ref="B525:F525"/>
-    <mergeCell ref="B526:F526"/>
-    <mergeCell ref="B527:F527"/>
-    <mergeCell ref="B528:F528"/>
-    <mergeCell ref="B517:F517"/>
-    <mergeCell ref="B518:F518"/>
-    <mergeCell ref="B519:F519"/>
-    <mergeCell ref="B520:F520"/>
-    <mergeCell ref="B521:F521"/>
-    <mergeCell ref="B522:F522"/>
-    <mergeCell ref="B547:F547"/>
-    <mergeCell ref="B548:F548"/>
-    <mergeCell ref="B549:F549"/>
-    <mergeCell ref="B550:F550"/>
-    <mergeCell ref="B551:F551"/>
-    <mergeCell ref="B552:F552"/>
-    <mergeCell ref="B541:F541"/>
-    <mergeCell ref="B542:F542"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="B544:F544"/>
-    <mergeCell ref="B545:F545"/>
-    <mergeCell ref="B546:F546"/>
-    <mergeCell ref="B535:F535"/>
-    <mergeCell ref="B536:F536"/>
-    <mergeCell ref="B537:F537"/>
-    <mergeCell ref="B538:F538"/>
-    <mergeCell ref="B539:F539"/>
-    <mergeCell ref="B540:F540"/>
-    <mergeCell ref="B565:F565"/>
-    <mergeCell ref="B566:F566"/>
-    <mergeCell ref="B567:F567"/>
-    <mergeCell ref="B568:F568"/>
-    <mergeCell ref="B569:F569"/>
-    <mergeCell ref="B570:F570"/>
-    <mergeCell ref="B559:F559"/>
-    <mergeCell ref="B560:F560"/>
-    <mergeCell ref="B561:F561"/>
-    <mergeCell ref="B562:F562"/>
-    <mergeCell ref="B563:F563"/>
-    <mergeCell ref="B564:F564"/>
-    <mergeCell ref="B553:F553"/>
-    <mergeCell ref="B554:F554"/>
-    <mergeCell ref="B555:F555"/>
-    <mergeCell ref="B556:F556"/>
-    <mergeCell ref="B557:F557"/>
-    <mergeCell ref="B558:F558"/>
-    <mergeCell ref="B583:F583"/>
-    <mergeCell ref="B584:F584"/>
-    <mergeCell ref="B585:F585"/>
-    <mergeCell ref="B586:F586"/>
-    <mergeCell ref="B587:F587"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="B577:F577"/>
-    <mergeCell ref="B578:F578"/>
-    <mergeCell ref="B579:F579"/>
-    <mergeCell ref="B580:F580"/>
-    <mergeCell ref="B581:F581"/>
-    <mergeCell ref="B582:F582"/>
-    <mergeCell ref="B571:F571"/>
-    <mergeCell ref="B572:F572"/>
-    <mergeCell ref="B573:F573"/>
-    <mergeCell ref="B574:F574"/>
-    <mergeCell ref="B575:F575"/>
-    <mergeCell ref="B576:F576"/>
-    <mergeCell ref="B601:F601"/>
-    <mergeCell ref="B602:F602"/>
-    <mergeCell ref="B603:F603"/>
-    <mergeCell ref="B604:F604"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="B606:F606"/>
-    <mergeCell ref="B595:F595"/>
-    <mergeCell ref="B596:F596"/>
-    <mergeCell ref="B597:F597"/>
-    <mergeCell ref="B598:F598"/>
-    <mergeCell ref="B599:F599"/>
-    <mergeCell ref="B600:F600"/>
-    <mergeCell ref="B589:F589"/>
-    <mergeCell ref="B590:F590"/>
-    <mergeCell ref="B591:F591"/>
-    <mergeCell ref="B592:F592"/>
-    <mergeCell ref="B593:F593"/>
-    <mergeCell ref="B594:F594"/>
-    <mergeCell ref="B619:F619"/>
-    <mergeCell ref="B620:F620"/>
-    <mergeCell ref="B621:F621"/>
-    <mergeCell ref="B622:F622"/>
-    <mergeCell ref="B623:F623"/>
-    <mergeCell ref="B624:F624"/>
-    <mergeCell ref="B613:F613"/>
-    <mergeCell ref="B614:F614"/>
-    <mergeCell ref="B615:F615"/>
-    <mergeCell ref="B616:F616"/>
-    <mergeCell ref="B617:F617"/>
-    <mergeCell ref="B618:F618"/>
-    <mergeCell ref="B607:F607"/>
-    <mergeCell ref="B608:F608"/>
-    <mergeCell ref="B609:F609"/>
-    <mergeCell ref="B610:F610"/>
-    <mergeCell ref="B611:F611"/>
-    <mergeCell ref="B612:F612"/>
-    <mergeCell ref="B637:F637"/>
-    <mergeCell ref="B638:F638"/>
-    <mergeCell ref="B639:F639"/>
-    <mergeCell ref="B640:F640"/>
-    <mergeCell ref="B641:F641"/>
-    <mergeCell ref="B642:F642"/>
-    <mergeCell ref="B631:F631"/>
-    <mergeCell ref="B632:F632"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="B634:F634"/>
-    <mergeCell ref="B635:F635"/>
-    <mergeCell ref="B636:F636"/>
-    <mergeCell ref="B625:F625"/>
-    <mergeCell ref="B626:F626"/>
-    <mergeCell ref="B627:F627"/>
-    <mergeCell ref="B628:F628"/>
-    <mergeCell ref="B629:F629"/>
-    <mergeCell ref="B630:F630"/>
-    <mergeCell ref="B655:F655"/>
-    <mergeCell ref="B656:F656"/>
-    <mergeCell ref="B657:F657"/>
-    <mergeCell ref="B658:F658"/>
-    <mergeCell ref="B659:F659"/>
-    <mergeCell ref="B660:F660"/>
-    <mergeCell ref="B649:F649"/>
-    <mergeCell ref="B650:F650"/>
-    <mergeCell ref="B651:F651"/>
-    <mergeCell ref="B652:F652"/>
-    <mergeCell ref="B653:F653"/>
-    <mergeCell ref="B654:F654"/>
-    <mergeCell ref="B643:F643"/>
-    <mergeCell ref="B644:F644"/>
-    <mergeCell ref="B645:F645"/>
-    <mergeCell ref="B646:F646"/>
-    <mergeCell ref="B647:F647"/>
-    <mergeCell ref="B648:F648"/>
-    <mergeCell ref="B673:F673"/>
-    <mergeCell ref="B674:F674"/>
-    <mergeCell ref="B675:F675"/>
-    <mergeCell ref="B676:F676"/>
-    <mergeCell ref="B677:F677"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="B667:F667"/>
-    <mergeCell ref="B668:F668"/>
-    <mergeCell ref="B669:F669"/>
-    <mergeCell ref="B670:F670"/>
-    <mergeCell ref="B671:F671"/>
-    <mergeCell ref="B672:F672"/>
-    <mergeCell ref="B661:F661"/>
-    <mergeCell ref="B662:F662"/>
-    <mergeCell ref="B663:F663"/>
-    <mergeCell ref="B664:F664"/>
-    <mergeCell ref="B665:F665"/>
-    <mergeCell ref="B666:F666"/>
-    <mergeCell ref="B691:F691"/>
-    <mergeCell ref="B692:F692"/>
-    <mergeCell ref="B693:F693"/>
-    <mergeCell ref="B694:F694"/>
-    <mergeCell ref="B695:F695"/>
-    <mergeCell ref="B696:F696"/>
-    <mergeCell ref="B685:F685"/>
-    <mergeCell ref="B686:F686"/>
-    <mergeCell ref="B687:F687"/>
-    <mergeCell ref="B688:F688"/>
-    <mergeCell ref="B689:F689"/>
-    <mergeCell ref="B690:F690"/>
-    <mergeCell ref="B679:F679"/>
-    <mergeCell ref="B680:F680"/>
-    <mergeCell ref="B681:F681"/>
-    <mergeCell ref="B682:F682"/>
-    <mergeCell ref="B683:F683"/>
-    <mergeCell ref="B684:F684"/>
-    <mergeCell ref="B709:F709"/>
-    <mergeCell ref="B710:F710"/>
-    <mergeCell ref="B711:F711"/>
-    <mergeCell ref="B712:F712"/>
-    <mergeCell ref="B713:F713"/>
-    <mergeCell ref="B714:F714"/>
-    <mergeCell ref="B703:F703"/>
-    <mergeCell ref="B704:F704"/>
-    <mergeCell ref="B705:F705"/>
-    <mergeCell ref="B706:F706"/>
-    <mergeCell ref="B707:F707"/>
-    <mergeCell ref="B708:F708"/>
-    <mergeCell ref="B697:F697"/>
-    <mergeCell ref="B698:F698"/>
-    <mergeCell ref="B699:F699"/>
-    <mergeCell ref="B700:F700"/>
-    <mergeCell ref="B701:F701"/>
-    <mergeCell ref="B702:F702"/>
-    <mergeCell ref="B727:F727"/>
-    <mergeCell ref="B728:F728"/>
-    <mergeCell ref="B729:F729"/>
-    <mergeCell ref="B730:F730"/>
-    <mergeCell ref="B731:F731"/>
-    <mergeCell ref="B732:F732"/>
-    <mergeCell ref="B721:F721"/>
-    <mergeCell ref="B722:F722"/>
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="B724:F724"/>
-    <mergeCell ref="B725:F725"/>
-    <mergeCell ref="B726:F726"/>
-    <mergeCell ref="B715:F715"/>
-    <mergeCell ref="B716:F716"/>
-    <mergeCell ref="B717:F717"/>
-    <mergeCell ref="B718:F718"/>
-    <mergeCell ref="B719:F719"/>
-    <mergeCell ref="B720:F720"/>
-    <mergeCell ref="B745:F745"/>
-    <mergeCell ref="B746:F746"/>
-    <mergeCell ref="B747:F747"/>
-    <mergeCell ref="B748:F748"/>
-    <mergeCell ref="B749:F749"/>
-    <mergeCell ref="B750:F750"/>
-    <mergeCell ref="B739:F739"/>
-    <mergeCell ref="B740:F740"/>
-    <mergeCell ref="B741:F741"/>
-    <mergeCell ref="B742:F742"/>
-    <mergeCell ref="B743:F743"/>
-    <mergeCell ref="B744:F744"/>
-    <mergeCell ref="B733:F733"/>
-    <mergeCell ref="B734:F734"/>
-    <mergeCell ref="B735:F735"/>
-    <mergeCell ref="B736:F736"/>
-    <mergeCell ref="B737:F737"/>
-    <mergeCell ref="B738:F738"/>
-    <mergeCell ref="B763:F763"/>
-    <mergeCell ref="B764:F764"/>
-    <mergeCell ref="B765:F765"/>
-    <mergeCell ref="B766:F766"/>
-    <mergeCell ref="B767:F767"/>
-    <mergeCell ref="B768:F768"/>
-    <mergeCell ref="B757:F757"/>
-    <mergeCell ref="B758:F758"/>
-    <mergeCell ref="B759:F759"/>
-    <mergeCell ref="B760:F760"/>
-    <mergeCell ref="B761:F761"/>
-    <mergeCell ref="B762:F762"/>
-    <mergeCell ref="B751:F751"/>
-    <mergeCell ref="B752:F752"/>
-    <mergeCell ref="B753:F753"/>
-    <mergeCell ref="B754:F754"/>
-    <mergeCell ref="B755:F755"/>
-    <mergeCell ref="B756:F756"/>
-    <mergeCell ref="B781:F781"/>
-    <mergeCell ref="B782:F782"/>
-    <mergeCell ref="B783:F783"/>
-    <mergeCell ref="B784:F784"/>
-    <mergeCell ref="B785:F785"/>
-    <mergeCell ref="B786:F786"/>
-    <mergeCell ref="B775:F775"/>
-    <mergeCell ref="B776:F776"/>
-    <mergeCell ref="B777:F777"/>
-    <mergeCell ref="B778:F778"/>
-    <mergeCell ref="B779:F779"/>
-    <mergeCell ref="B780:F780"/>
-    <mergeCell ref="B769:F769"/>
-    <mergeCell ref="B770:F770"/>
-    <mergeCell ref="B771:F771"/>
-    <mergeCell ref="B772:F772"/>
-    <mergeCell ref="B773:F773"/>
-    <mergeCell ref="B774:F774"/>
-    <mergeCell ref="B799:F799"/>
-    <mergeCell ref="B800:F800"/>
-    <mergeCell ref="B801:F801"/>
-    <mergeCell ref="B802:F802"/>
-    <mergeCell ref="B803:F803"/>
-    <mergeCell ref="B804:F804"/>
-    <mergeCell ref="B793:F793"/>
-    <mergeCell ref="B794:F794"/>
-    <mergeCell ref="B795:F795"/>
-    <mergeCell ref="B796:F796"/>
-    <mergeCell ref="B797:F797"/>
-    <mergeCell ref="B798:F798"/>
-    <mergeCell ref="B787:F787"/>
-    <mergeCell ref="B788:F788"/>
-    <mergeCell ref="B789:F789"/>
-    <mergeCell ref="B790:F790"/>
-    <mergeCell ref="B791:F791"/>
-    <mergeCell ref="B792:F792"/>
-    <mergeCell ref="B817:F817"/>
-    <mergeCell ref="B818:F818"/>
-    <mergeCell ref="B819:F819"/>
-    <mergeCell ref="B820:F820"/>
-    <mergeCell ref="B821:F821"/>
-    <mergeCell ref="B822:F822"/>
-    <mergeCell ref="B811:F811"/>
-    <mergeCell ref="B812:F812"/>
-    <mergeCell ref="B813:F813"/>
-    <mergeCell ref="B814:F814"/>
-    <mergeCell ref="B815:F815"/>
-    <mergeCell ref="B816:F816"/>
-    <mergeCell ref="B805:F805"/>
-    <mergeCell ref="B806:F806"/>
-    <mergeCell ref="B807:F807"/>
-    <mergeCell ref="B808:F808"/>
-    <mergeCell ref="B809:F809"/>
-    <mergeCell ref="B810:F810"/>
-    <mergeCell ref="B835:F835"/>
-    <mergeCell ref="B836:F836"/>
-    <mergeCell ref="B837:F837"/>
-    <mergeCell ref="B838:F838"/>
-    <mergeCell ref="B839:F839"/>
-    <mergeCell ref="B840:F840"/>
-    <mergeCell ref="B829:F829"/>
-    <mergeCell ref="B830:F830"/>
-    <mergeCell ref="B831:F831"/>
-    <mergeCell ref="B832:F832"/>
-    <mergeCell ref="B833:F833"/>
-    <mergeCell ref="B834:F834"/>
-    <mergeCell ref="B823:F823"/>
-    <mergeCell ref="B824:F824"/>
-    <mergeCell ref="B825:F825"/>
-    <mergeCell ref="B826:F826"/>
-    <mergeCell ref="B827:F827"/>
-    <mergeCell ref="B828:F828"/>
-    <mergeCell ref="B853:F853"/>
-    <mergeCell ref="B854:F854"/>
-    <mergeCell ref="B855:F855"/>
-    <mergeCell ref="B856:F856"/>
-    <mergeCell ref="B857:F857"/>
-    <mergeCell ref="B858:F858"/>
-    <mergeCell ref="B847:F847"/>
-    <mergeCell ref="B848:F848"/>
-    <mergeCell ref="B849:F849"/>
-    <mergeCell ref="B850:F850"/>
-    <mergeCell ref="B851:F851"/>
-    <mergeCell ref="B852:F852"/>
-    <mergeCell ref="B841:F841"/>
-    <mergeCell ref="B842:F842"/>
-    <mergeCell ref="B843:F843"/>
-    <mergeCell ref="B844:F844"/>
-    <mergeCell ref="B845:F845"/>
-    <mergeCell ref="B846:F846"/>
-    <mergeCell ref="B871:F871"/>
-    <mergeCell ref="B872:F872"/>
-    <mergeCell ref="B873:F873"/>
-    <mergeCell ref="B874:F874"/>
-    <mergeCell ref="B875:F875"/>
-    <mergeCell ref="B876:F876"/>
-    <mergeCell ref="B865:F865"/>
-    <mergeCell ref="B866:F866"/>
-    <mergeCell ref="B867:F867"/>
-    <mergeCell ref="B868:F868"/>
-    <mergeCell ref="B869:F869"/>
-    <mergeCell ref="B870:F870"/>
-    <mergeCell ref="B859:F859"/>
-    <mergeCell ref="B860:F860"/>
-    <mergeCell ref="B861:F861"/>
-    <mergeCell ref="B862:F862"/>
-    <mergeCell ref="B863:F863"/>
-    <mergeCell ref="B864:F864"/>
-    <mergeCell ref="B889:F889"/>
-    <mergeCell ref="B890:F890"/>
-    <mergeCell ref="B891:F891"/>
-    <mergeCell ref="B892:F892"/>
-    <mergeCell ref="B893:F893"/>
-    <mergeCell ref="B894:F894"/>
-    <mergeCell ref="B883:F883"/>
-    <mergeCell ref="B884:F884"/>
-    <mergeCell ref="B885:F885"/>
-    <mergeCell ref="B886:F886"/>
-    <mergeCell ref="B887:F887"/>
-    <mergeCell ref="B888:F888"/>
-    <mergeCell ref="B877:F877"/>
-    <mergeCell ref="B878:F878"/>
-    <mergeCell ref="B879:F879"/>
-    <mergeCell ref="B880:F880"/>
-    <mergeCell ref="B881:F881"/>
-    <mergeCell ref="B882:F882"/>
-    <mergeCell ref="B907:F907"/>
-    <mergeCell ref="B908:F908"/>
-    <mergeCell ref="B909:F909"/>
-    <mergeCell ref="B910:F910"/>
-    <mergeCell ref="B911:F911"/>
-    <mergeCell ref="B912:F912"/>
-    <mergeCell ref="B901:F901"/>
-    <mergeCell ref="B902:F902"/>
-    <mergeCell ref="B903:F903"/>
-    <mergeCell ref="B904:F904"/>
-    <mergeCell ref="B905:F905"/>
-    <mergeCell ref="B906:F906"/>
-    <mergeCell ref="B895:F895"/>
-    <mergeCell ref="B896:F896"/>
-    <mergeCell ref="B897:F897"/>
-    <mergeCell ref="B898:F898"/>
-    <mergeCell ref="B899:F899"/>
-    <mergeCell ref="B900:F900"/>
-    <mergeCell ref="B925:F925"/>
-    <mergeCell ref="B926:F926"/>
-    <mergeCell ref="B927:F927"/>
-    <mergeCell ref="B928:F928"/>
-    <mergeCell ref="B929:F929"/>
-    <mergeCell ref="B930:F930"/>
-    <mergeCell ref="B919:F919"/>
-    <mergeCell ref="B920:F920"/>
-    <mergeCell ref="B921:F921"/>
-    <mergeCell ref="B922:F922"/>
-    <mergeCell ref="B923:F923"/>
-    <mergeCell ref="B924:F924"/>
-    <mergeCell ref="B913:F913"/>
-    <mergeCell ref="B914:F914"/>
-    <mergeCell ref="B915:F915"/>
-    <mergeCell ref="B916:F916"/>
-    <mergeCell ref="B917:F917"/>
-    <mergeCell ref="B918:F918"/>
-    <mergeCell ref="B943:F943"/>
-    <mergeCell ref="B944:F944"/>
-    <mergeCell ref="B945:F945"/>
-    <mergeCell ref="B946:F946"/>
-    <mergeCell ref="B947:F947"/>
-    <mergeCell ref="B948:F948"/>
-    <mergeCell ref="B937:F937"/>
-    <mergeCell ref="B938:F938"/>
-    <mergeCell ref="B939:F939"/>
-    <mergeCell ref="B940:F940"/>
-    <mergeCell ref="B941:F941"/>
-    <mergeCell ref="B942:F942"/>
-    <mergeCell ref="B931:F931"/>
-    <mergeCell ref="B932:F932"/>
-    <mergeCell ref="B933:F933"/>
-    <mergeCell ref="B934:F934"/>
-    <mergeCell ref="B935:F935"/>
-    <mergeCell ref="B936:F936"/>
-    <mergeCell ref="B961:F961"/>
-    <mergeCell ref="B962:F962"/>
-    <mergeCell ref="B963:F963"/>
-    <mergeCell ref="B964:F964"/>
-    <mergeCell ref="B965:F965"/>
-    <mergeCell ref="B966:F966"/>
-    <mergeCell ref="B955:F955"/>
-    <mergeCell ref="B956:F956"/>
-    <mergeCell ref="B957:F957"/>
-    <mergeCell ref="B958:F958"/>
-    <mergeCell ref="B959:F959"/>
-    <mergeCell ref="B960:F960"/>
-    <mergeCell ref="B949:F949"/>
-    <mergeCell ref="B950:F950"/>
-    <mergeCell ref="B951:F951"/>
-    <mergeCell ref="B952:F952"/>
-    <mergeCell ref="B953:F953"/>
-    <mergeCell ref="B954:F954"/>
-    <mergeCell ref="B979:F979"/>
-    <mergeCell ref="B980:F980"/>
-    <mergeCell ref="B981:F981"/>
-    <mergeCell ref="B982:F982"/>
-    <mergeCell ref="B983:F983"/>
-    <mergeCell ref="B984:F984"/>
-    <mergeCell ref="B973:F973"/>
-    <mergeCell ref="B974:F974"/>
-    <mergeCell ref="B975:F975"/>
-    <mergeCell ref="B976:F976"/>
-    <mergeCell ref="B977:F977"/>
-    <mergeCell ref="B978:F978"/>
-    <mergeCell ref="B967:F967"/>
-    <mergeCell ref="B968:F968"/>
-    <mergeCell ref="B969:F969"/>
-    <mergeCell ref="B970:F970"/>
-    <mergeCell ref="B971:F971"/>
-    <mergeCell ref="B972:F972"/>
-    <mergeCell ref="B997:F997"/>
-    <mergeCell ref="B998:F998"/>
-    <mergeCell ref="B999:F999"/>
-    <mergeCell ref="B1000:F1000"/>
-    <mergeCell ref="B1001:F1001"/>
-    <mergeCell ref="B1002:F1002"/>
-    <mergeCell ref="B991:F991"/>
-    <mergeCell ref="B992:F992"/>
-    <mergeCell ref="B993:F993"/>
-    <mergeCell ref="B994:F994"/>
-    <mergeCell ref="B995:F995"/>
-    <mergeCell ref="B996:F996"/>
-    <mergeCell ref="B985:F985"/>
-    <mergeCell ref="B986:F986"/>
-    <mergeCell ref="B987:F987"/>
-    <mergeCell ref="B988:F988"/>
-    <mergeCell ref="B989:F989"/>
-    <mergeCell ref="B990:F990"/>
-    <mergeCell ref="B1015:F1015"/>
-    <mergeCell ref="B1016:F1016"/>
-    <mergeCell ref="B1017:F1017"/>
-    <mergeCell ref="B1018:F1018"/>
-    <mergeCell ref="B1019:F1019"/>
-    <mergeCell ref="B1020:F1020"/>
-    <mergeCell ref="B1009:F1009"/>
-    <mergeCell ref="B1010:F1010"/>
-    <mergeCell ref="B1011:F1011"/>
-    <mergeCell ref="B1012:F1012"/>
-    <mergeCell ref="B1013:F1013"/>
-    <mergeCell ref="B1014:F1014"/>
-    <mergeCell ref="B1003:F1003"/>
-    <mergeCell ref="B1004:F1004"/>
-    <mergeCell ref="B1005:F1005"/>
-    <mergeCell ref="B1006:F1006"/>
-    <mergeCell ref="B1007:F1007"/>
-    <mergeCell ref="B1008:F1008"/>
-    <mergeCell ref="B1033:F1033"/>
-    <mergeCell ref="B1034:F1034"/>
-    <mergeCell ref="B1035:F1035"/>
-    <mergeCell ref="B1036:F1036"/>
-    <mergeCell ref="B1037:F1037"/>
-    <mergeCell ref="B1038:F1038"/>
-    <mergeCell ref="B1027:F1027"/>
-    <mergeCell ref="B1028:F1028"/>
-    <mergeCell ref="B1029:F1029"/>
-    <mergeCell ref="B1030:F1030"/>
-    <mergeCell ref="B1031:F1031"/>
-    <mergeCell ref="B1032:F1032"/>
-    <mergeCell ref="B1021:F1021"/>
-    <mergeCell ref="B1022:F1022"/>
-    <mergeCell ref="B1023:F1023"/>
-    <mergeCell ref="B1024:F1024"/>
-    <mergeCell ref="B1025:F1025"/>
-    <mergeCell ref="B1026:F1026"/>
-    <mergeCell ref="B1051:F1051"/>
-    <mergeCell ref="B1052:F1052"/>
-    <mergeCell ref="B1053:F1053"/>
-    <mergeCell ref="B1054:F1054"/>
-    <mergeCell ref="B1055:F1055"/>
-    <mergeCell ref="B1056:F1056"/>
-    <mergeCell ref="B1045:F1045"/>
-    <mergeCell ref="B1046:F1046"/>
-    <mergeCell ref="B1047:F1047"/>
-    <mergeCell ref="B1048:F1048"/>
-    <mergeCell ref="B1049:F1049"/>
-    <mergeCell ref="B1050:F1050"/>
-    <mergeCell ref="B1039:F1039"/>
-    <mergeCell ref="B1040:F1040"/>
-    <mergeCell ref="B1041:F1041"/>
-    <mergeCell ref="B1042:F1042"/>
-    <mergeCell ref="B1043:F1043"/>
-    <mergeCell ref="B1044:F1044"/>
-    <mergeCell ref="B1069:F1069"/>
-    <mergeCell ref="B1070:F1070"/>
-    <mergeCell ref="B1071:F1071"/>
-    <mergeCell ref="B1072:F1072"/>
-    <mergeCell ref="B1073:F1073"/>
-    <mergeCell ref="B1074:F1074"/>
-    <mergeCell ref="B1063:F1063"/>
-    <mergeCell ref="B1064:F1064"/>
-    <mergeCell ref="B1065:F1065"/>
-    <mergeCell ref="B1066:F1066"/>
-    <mergeCell ref="B1067:F1067"/>
-    <mergeCell ref="B1068:F1068"/>
-    <mergeCell ref="B1057:F1057"/>
-    <mergeCell ref="B1058:F1058"/>
-    <mergeCell ref="B1059:F1059"/>
-    <mergeCell ref="B1060:F1060"/>
-    <mergeCell ref="B1061:F1061"/>
-    <mergeCell ref="B1062:F1062"/>
-    <mergeCell ref="B1087:F1087"/>
-    <mergeCell ref="B1088:F1088"/>
-    <mergeCell ref="B1089:F1089"/>
-    <mergeCell ref="B1090:F1090"/>
-    <mergeCell ref="B1091:F1091"/>
-    <mergeCell ref="B1092:F1092"/>
-    <mergeCell ref="B1081:F1081"/>
-    <mergeCell ref="B1082:F1082"/>
-    <mergeCell ref="B1083:F1083"/>
-    <mergeCell ref="B1084:F1084"/>
-    <mergeCell ref="B1085:F1085"/>
-    <mergeCell ref="B1086:F1086"/>
-    <mergeCell ref="B1075:F1075"/>
-    <mergeCell ref="B1076:F1076"/>
-    <mergeCell ref="B1077:F1077"/>
-    <mergeCell ref="B1078:F1078"/>
-    <mergeCell ref="B1079:F1079"/>
-    <mergeCell ref="B1080:F1080"/>
-    <mergeCell ref="B1105:F1105"/>
-    <mergeCell ref="B1106:F1106"/>
-    <mergeCell ref="B1107:F1107"/>
-    <mergeCell ref="B1108:F1108"/>
-    <mergeCell ref="B1109:F1109"/>
-    <mergeCell ref="B1110:F1110"/>
-    <mergeCell ref="B1099:F1099"/>
-    <mergeCell ref="B1100:F1100"/>
-    <mergeCell ref="B1101:F1101"/>
-    <mergeCell ref="B1102:F1102"/>
-    <mergeCell ref="B1103:F1103"/>
-    <mergeCell ref="B1104:F1104"/>
-    <mergeCell ref="B1093:F1093"/>
-    <mergeCell ref="B1094:F1094"/>
-    <mergeCell ref="B1095:F1095"/>
-    <mergeCell ref="B1096:F1096"/>
-    <mergeCell ref="B1097:F1097"/>
-    <mergeCell ref="B1098:F1098"/>
-    <mergeCell ref="B1123:F1123"/>
-    <mergeCell ref="B1124:F1124"/>
-    <mergeCell ref="B1125:F1125"/>
-    <mergeCell ref="B1126:F1126"/>
-    <mergeCell ref="B1127:F1127"/>
-    <mergeCell ref="B1128:F1128"/>
-    <mergeCell ref="B1117:F1117"/>
-    <mergeCell ref="B1118:F1118"/>
-    <mergeCell ref="B1119:F1119"/>
-    <mergeCell ref="B1120:F1120"/>
-    <mergeCell ref="B1121:F1121"/>
-    <mergeCell ref="B1122:F1122"/>
-    <mergeCell ref="B1111:F1111"/>
-    <mergeCell ref="B1112:F1112"/>
-    <mergeCell ref="B1113:F1113"/>
-    <mergeCell ref="B1114:F1114"/>
-    <mergeCell ref="B1115:F1115"/>
-    <mergeCell ref="B1116:F1116"/>
-    <mergeCell ref="B1141:F1141"/>
-    <mergeCell ref="B1142:F1142"/>
-    <mergeCell ref="B1143:F1143"/>
-    <mergeCell ref="B1144:F1144"/>
-    <mergeCell ref="B1145:F1145"/>
-    <mergeCell ref="B1146:F1146"/>
-    <mergeCell ref="B1135:F1135"/>
-    <mergeCell ref="B1136:F1136"/>
-    <mergeCell ref="B1137:F1137"/>
-    <mergeCell ref="B1138:F1138"/>
-    <mergeCell ref="B1139:F1139"/>
-    <mergeCell ref="B1140:F1140"/>
-    <mergeCell ref="B1129:F1129"/>
-    <mergeCell ref="B1130:F1130"/>
-    <mergeCell ref="B1131:F1131"/>
-    <mergeCell ref="B1132:F1132"/>
-    <mergeCell ref="B1133:F1133"/>
-    <mergeCell ref="B1134:F1134"/>
-    <mergeCell ref="B1159:F1159"/>
-    <mergeCell ref="B1160:F1160"/>
-    <mergeCell ref="B1161:F1161"/>
-    <mergeCell ref="B1162:F1162"/>
-    <mergeCell ref="B1163:F1163"/>
-    <mergeCell ref="B1164:F1164"/>
-    <mergeCell ref="B1153:F1153"/>
-    <mergeCell ref="B1154:F1154"/>
-    <mergeCell ref="B1155:F1155"/>
-    <mergeCell ref="B1156:F1156"/>
-    <mergeCell ref="B1157:F1157"/>
-    <mergeCell ref="B1158:F1158"/>
-    <mergeCell ref="B1147:F1147"/>
-    <mergeCell ref="B1148:F1148"/>
-    <mergeCell ref="B1149:F1149"/>
-    <mergeCell ref="B1150:F1150"/>
-    <mergeCell ref="B1151:F1151"/>
-    <mergeCell ref="B1152:F1152"/>
-    <mergeCell ref="B1177:F1177"/>
-    <mergeCell ref="B1178:F1178"/>
-    <mergeCell ref="B1179:F1179"/>
-    <mergeCell ref="B1180:F1180"/>
-    <mergeCell ref="B1181:F1181"/>
-    <mergeCell ref="B1182:F1182"/>
-    <mergeCell ref="B1171:F1171"/>
-    <mergeCell ref="B1172:F1172"/>
-    <mergeCell ref="B1173:F1173"/>
-    <mergeCell ref="B1174:F1174"/>
-    <mergeCell ref="B1175:F1175"/>
-    <mergeCell ref="B1176:F1176"/>
-    <mergeCell ref="B1165:F1165"/>
-    <mergeCell ref="B1166:F1166"/>
-    <mergeCell ref="B1167:F1167"/>
-    <mergeCell ref="B1168:F1168"/>
-    <mergeCell ref="B1169:F1169"/>
-    <mergeCell ref="B1170:F1170"/>
-    <mergeCell ref="B1195:F1195"/>
-    <mergeCell ref="B1196:F1196"/>
-    <mergeCell ref="B1197:F1197"/>
-    <mergeCell ref="B1198:F1198"/>
-    <mergeCell ref="B1199:F1199"/>
-    <mergeCell ref="B1200:F1200"/>
-    <mergeCell ref="B1189:F1189"/>
-    <mergeCell ref="B1190:F1190"/>
-    <mergeCell ref="B1191:F1191"/>
-    <mergeCell ref="B1192:F1192"/>
-    <mergeCell ref="B1193:F1193"/>
-    <mergeCell ref="B1194:F1194"/>
-    <mergeCell ref="B1183:F1183"/>
-    <mergeCell ref="B1184:F1184"/>
-    <mergeCell ref="B1185:F1185"/>
-    <mergeCell ref="B1186:F1186"/>
-    <mergeCell ref="B1187:F1187"/>
-    <mergeCell ref="B1188:F1188"/>
-    <mergeCell ref="B1213:F1213"/>
-    <mergeCell ref="B1214:F1214"/>
-    <mergeCell ref="B1215:F1215"/>
-    <mergeCell ref="B1216:F1216"/>
-    <mergeCell ref="B1217:F1217"/>
-    <mergeCell ref="B1218:F1218"/>
-    <mergeCell ref="B1207:F1207"/>
-    <mergeCell ref="B1208:F1208"/>
-    <mergeCell ref="B1209:F1209"/>
-    <mergeCell ref="B1210:F1210"/>
-    <mergeCell ref="B1211:F1211"/>
-    <mergeCell ref="B1212:F1212"/>
-    <mergeCell ref="B1201:F1201"/>
-    <mergeCell ref="B1202:F1202"/>
-    <mergeCell ref="B1203:F1203"/>
-    <mergeCell ref="B1204:F1204"/>
-    <mergeCell ref="B1205:F1205"/>
-    <mergeCell ref="B1206:F1206"/>
-    <mergeCell ref="B1231:F1231"/>
-    <mergeCell ref="B1232:F1232"/>
-    <mergeCell ref="B1233:F1233"/>
-    <mergeCell ref="B1234:F1234"/>
-    <mergeCell ref="B1235:F1235"/>
-    <mergeCell ref="B1236:F1236"/>
-    <mergeCell ref="B1225:F1225"/>
-    <mergeCell ref="B1226:F1226"/>
-    <mergeCell ref="B1227:F1227"/>
-    <mergeCell ref="B1228:F1228"/>
-    <mergeCell ref="B1229:F1229"/>
-    <mergeCell ref="B1230:F1230"/>
-    <mergeCell ref="B1219:F1219"/>
-    <mergeCell ref="B1220:F1220"/>
-    <mergeCell ref="B1221:F1221"/>
-    <mergeCell ref="B1222:F1222"/>
-    <mergeCell ref="B1223:F1223"/>
-    <mergeCell ref="B1224:F1224"/>
-    <mergeCell ref="B1249:F1249"/>
-    <mergeCell ref="B1250:F1250"/>
-    <mergeCell ref="B1251:F1251"/>
-    <mergeCell ref="B1252:F1252"/>
-    <mergeCell ref="B1253:F1253"/>
-    <mergeCell ref="B1254:F1254"/>
-    <mergeCell ref="B1243:F1243"/>
-    <mergeCell ref="B1244:F1244"/>
-    <mergeCell ref="B1245:F1245"/>
-    <mergeCell ref="B1246:F1246"/>
-    <mergeCell ref="B1247:F1247"/>
-    <mergeCell ref="B1248:F1248"/>
-    <mergeCell ref="B1237:F1237"/>
-    <mergeCell ref="B1238:F1238"/>
-    <mergeCell ref="B1239:F1239"/>
-    <mergeCell ref="B1240:F1240"/>
-    <mergeCell ref="B1241:F1241"/>
-    <mergeCell ref="B1242:F1242"/>
-    <mergeCell ref="B1267:F1267"/>
-    <mergeCell ref="B1268:F1268"/>
-    <mergeCell ref="B1269:F1269"/>
-    <mergeCell ref="B1270:F1270"/>
-    <mergeCell ref="B1271:F1271"/>
-    <mergeCell ref="B1272:F1272"/>
-    <mergeCell ref="B1261:F1261"/>
-    <mergeCell ref="B1262:F1262"/>
-    <mergeCell ref="B1263:F1263"/>
-    <mergeCell ref="B1264:F1264"/>
-    <mergeCell ref="B1265:F1265"/>
-    <mergeCell ref="B1266:F1266"/>
-    <mergeCell ref="B1255:F1255"/>
-    <mergeCell ref="B1256:F1256"/>
-    <mergeCell ref="B1257:F1257"/>
-    <mergeCell ref="B1258:F1258"/>
-    <mergeCell ref="B1259:F1259"/>
-    <mergeCell ref="B1260:F1260"/>
-    <mergeCell ref="B1285:F1285"/>
-    <mergeCell ref="B1286:F1286"/>
-    <mergeCell ref="B1287:F1287"/>
-    <mergeCell ref="B1288:F1288"/>
-    <mergeCell ref="B1289:F1289"/>
-    <mergeCell ref="B1290:F1290"/>
-    <mergeCell ref="B1279:F1279"/>
-    <mergeCell ref="B1280:F1280"/>
-    <mergeCell ref="B1281:F1281"/>
-    <mergeCell ref="B1282:F1282"/>
-    <mergeCell ref="B1283:F1283"/>
-    <mergeCell ref="B1284:F1284"/>
-    <mergeCell ref="B1273:F1273"/>
-    <mergeCell ref="B1274:F1274"/>
-    <mergeCell ref="B1275:F1275"/>
-    <mergeCell ref="B1276:F1276"/>
-    <mergeCell ref="B1277:F1277"/>
-    <mergeCell ref="B1278:F1278"/>
-    <mergeCell ref="B1303:F1303"/>
-    <mergeCell ref="B1304:F1304"/>
-    <mergeCell ref="B1305:F1305"/>
-    <mergeCell ref="B1306:F1306"/>
-    <mergeCell ref="B1307:F1307"/>
-    <mergeCell ref="B1308:F1308"/>
-    <mergeCell ref="B1297:F1297"/>
-    <mergeCell ref="B1298:F1298"/>
-    <mergeCell ref="B1299:F1299"/>
-    <mergeCell ref="B1300:F1300"/>
-    <mergeCell ref="B1301:F1301"/>
-    <mergeCell ref="B1302:F1302"/>
-    <mergeCell ref="B1291:F1291"/>
-    <mergeCell ref="B1292:F1292"/>
-    <mergeCell ref="B1293:F1293"/>
-    <mergeCell ref="B1294:F1294"/>
-    <mergeCell ref="B1295:F1295"/>
-    <mergeCell ref="B1296:F1296"/>
-    <mergeCell ref="B1321:F1321"/>
-    <mergeCell ref="B1322:F1322"/>
-    <mergeCell ref="B1323:F1323"/>
-    <mergeCell ref="B1324:F1324"/>
-    <mergeCell ref="B1325:F1325"/>
-    <mergeCell ref="B1326:F1326"/>
-    <mergeCell ref="B1315:F1315"/>
-    <mergeCell ref="B1316:F1316"/>
-    <mergeCell ref="B1317:F1317"/>
-    <mergeCell ref="B1318:F1318"/>
-    <mergeCell ref="B1319:F1319"/>
-    <mergeCell ref="B1320:F1320"/>
-    <mergeCell ref="B1309:F1309"/>
-    <mergeCell ref="B1310:F1310"/>
-    <mergeCell ref="B1311:F1311"/>
-    <mergeCell ref="B1312:F1312"/>
-    <mergeCell ref="B1313:F1313"/>
-    <mergeCell ref="B1314:F1314"/>
-    <mergeCell ref="B1339:F1339"/>
-    <mergeCell ref="B1340:F1340"/>
-    <mergeCell ref="B1341:F1341"/>
-    <mergeCell ref="B1342:F1342"/>
-    <mergeCell ref="B1343:F1343"/>
-    <mergeCell ref="B1344:F1344"/>
-    <mergeCell ref="B1333:F1333"/>
-    <mergeCell ref="B1334:F1334"/>
-    <mergeCell ref="B1335:F1335"/>
-    <mergeCell ref="B1336:F1336"/>
-    <mergeCell ref="B1337:F1337"/>
-    <mergeCell ref="B1338:F1338"/>
-    <mergeCell ref="B1327:F1327"/>
-    <mergeCell ref="B1328:F1328"/>
-    <mergeCell ref="B1329:F1329"/>
-    <mergeCell ref="B1330:F1330"/>
-    <mergeCell ref="B1331:F1331"/>
-    <mergeCell ref="B1332:F1332"/>
-    <mergeCell ref="B1357:F1357"/>
-    <mergeCell ref="B1358:F1358"/>
-    <mergeCell ref="B1359:F1359"/>
-    <mergeCell ref="B1360:F1360"/>
-    <mergeCell ref="B1361:F1361"/>
-    <mergeCell ref="B1362:F1362"/>
-    <mergeCell ref="B1351:F1351"/>
-    <mergeCell ref="B1352:F1352"/>
-    <mergeCell ref="B1353:F1353"/>
-    <mergeCell ref="B1354:F1354"/>
-    <mergeCell ref="B1355:F1355"/>
-    <mergeCell ref="B1356:F1356"/>
-    <mergeCell ref="B1345:F1345"/>
-    <mergeCell ref="B1346:F1346"/>
-    <mergeCell ref="B1347:F1347"/>
-    <mergeCell ref="B1348:F1348"/>
-    <mergeCell ref="B1349:F1349"/>
-    <mergeCell ref="B1350:F1350"/>
-    <mergeCell ref="B1375:F1375"/>
-    <mergeCell ref="B1376:F1376"/>
-    <mergeCell ref="B1377:F1377"/>
-    <mergeCell ref="B1378:F1378"/>
-    <mergeCell ref="B1379:F1379"/>
-    <mergeCell ref="B1380:F1380"/>
-    <mergeCell ref="B1369:F1369"/>
-    <mergeCell ref="B1370:F1370"/>
-    <mergeCell ref="B1371:F1371"/>
-    <mergeCell ref="B1372:F1372"/>
-    <mergeCell ref="B1373:F1373"/>
-    <mergeCell ref="B1374:F1374"/>
-    <mergeCell ref="B1363:F1363"/>
-    <mergeCell ref="B1364:F1364"/>
-    <mergeCell ref="B1365:F1365"/>
-    <mergeCell ref="B1366:F1366"/>
-    <mergeCell ref="B1367:F1367"/>
-    <mergeCell ref="B1368:F1368"/>
-    <mergeCell ref="B1393:F1393"/>
-    <mergeCell ref="B1394:F1394"/>
-    <mergeCell ref="B1395:F1395"/>
-    <mergeCell ref="B1396:F1396"/>
-    <mergeCell ref="B1397:F1397"/>
-    <mergeCell ref="B1398:F1398"/>
-    <mergeCell ref="B1387:F1387"/>
-    <mergeCell ref="B1388:F1388"/>
-    <mergeCell ref="B1389:F1389"/>
-    <mergeCell ref="B1390:F1390"/>
-    <mergeCell ref="B1391:F1391"/>
-    <mergeCell ref="B1392:F1392"/>
-    <mergeCell ref="B1381:F1381"/>
-    <mergeCell ref="B1382:F1382"/>
-    <mergeCell ref="B1383:F1383"/>
-    <mergeCell ref="B1384:F1384"/>
-    <mergeCell ref="B1385:F1385"/>
-    <mergeCell ref="B1386:F1386"/>
-    <mergeCell ref="B1411:F1411"/>
-    <mergeCell ref="B1412:F1412"/>
-    <mergeCell ref="B1413:F1413"/>
-    <mergeCell ref="B1414:F1414"/>
-    <mergeCell ref="B1415:F1415"/>
-    <mergeCell ref="B1416:F1416"/>
-    <mergeCell ref="B1405:F1405"/>
-    <mergeCell ref="B1406:F1406"/>
-    <mergeCell ref="B1407:F1407"/>
-    <mergeCell ref="B1408:F1408"/>
-    <mergeCell ref="B1409:F1409"/>
-    <mergeCell ref="B1410:F1410"/>
-    <mergeCell ref="B1399:F1399"/>
-    <mergeCell ref="B1400:F1400"/>
-    <mergeCell ref="B1401:F1401"/>
-    <mergeCell ref="B1402:F1402"/>
-    <mergeCell ref="B1403:F1403"/>
-    <mergeCell ref="B1404:F1404"/>
-    <mergeCell ref="B1429:F1429"/>
-    <mergeCell ref="B1430:F1430"/>
-    <mergeCell ref="B1431:F1431"/>
-    <mergeCell ref="B1432:F1432"/>
-    <mergeCell ref="B1433:F1433"/>
-    <mergeCell ref="B1434:F1434"/>
-    <mergeCell ref="B1423:F1423"/>
-    <mergeCell ref="B1424:F1424"/>
-    <mergeCell ref="B1425:F1425"/>
-    <mergeCell ref="B1426:F1426"/>
-    <mergeCell ref="B1427:F1427"/>
-    <mergeCell ref="B1428:F1428"/>
-    <mergeCell ref="B1417:F1417"/>
-    <mergeCell ref="B1418:F1418"/>
-    <mergeCell ref="B1419:F1419"/>
-    <mergeCell ref="B1420:F1420"/>
-    <mergeCell ref="B1421:F1421"/>
-    <mergeCell ref="B1422:F1422"/>
-    <mergeCell ref="B1447:F1447"/>
-    <mergeCell ref="B1448:F1448"/>
-    <mergeCell ref="B1449:F1449"/>
-    <mergeCell ref="B1450:F1450"/>
-    <mergeCell ref="B1451:F1451"/>
-    <mergeCell ref="B1452:F1452"/>
-    <mergeCell ref="B1441:F1441"/>
-    <mergeCell ref="B1442:F1442"/>
-    <mergeCell ref="B1443:F1443"/>
-    <mergeCell ref="B1444:F1444"/>
-    <mergeCell ref="B1445:F1445"/>
-    <mergeCell ref="B1446:F1446"/>
-    <mergeCell ref="B1435:F1435"/>
-    <mergeCell ref="B1436:F1436"/>
-    <mergeCell ref="B1437:F1437"/>
-    <mergeCell ref="B1438:F1438"/>
-    <mergeCell ref="B1439:F1439"/>
-    <mergeCell ref="B1440:F1440"/>
-    <mergeCell ref="B1465:F1465"/>
-    <mergeCell ref="B1466:F1466"/>
-    <mergeCell ref="B1467:F1467"/>
-    <mergeCell ref="B1468:F1468"/>
-    <mergeCell ref="B1469:F1469"/>
-    <mergeCell ref="B1470:F1470"/>
-    <mergeCell ref="B1459:F1459"/>
-    <mergeCell ref="B1460:F1460"/>
-    <mergeCell ref="B1461:F1461"/>
-    <mergeCell ref="B1462:F1462"/>
-    <mergeCell ref="B1463:F1463"/>
-    <mergeCell ref="B1464:F1464"/>
-    <mergeCell ref="B1453:F1453"/>
-    <mergeCell ref="B1454:F1454"/>
-    <mergeCell ref="B1455:F1455"/>
-    <mergeCell ref="B1456:F1456"/>
-    <mergeCell ref="B1457:F1457"/>
-    <mergeCell ref="B1458:F1458"/>
-    <mergeCell ref="B1483:F1483"/>
-    <mergeCell ref="B1484:F1484"/>
-    <mergeCell ref="B1485:F1485"/>
-    <mergeCell ref="B1486:F1486"/>
-    <mergeCell ref="B1487:F1487"/>
-    <mergeCell ref="B1488:F1488"/>
-    <mergeCell ref="B1477:F1477"/>
-    <mergeCell ref="B1478:F1478"/>
-    <mergeCell ref="B1479:F1479"/>
-    <mergeCell ref="B1480:F1480"/>
-    <mergeCell ref="B1481:F1481"/>
-    <mergeCell ref="B1482:F1482"/>
-    <mergeCell ref="B1471:F1471"/>
-    <mergeCell ref="B1472:F1472"/>
-    <mergeCell ref="B1473:F1473"/>
-    <mergeCell ref="B1474:F1474"/>
-    <mergeCell ref="B1475:F1475"/>
-    <mergeCell ref="B1476:F1476"/>
-    <mergeCell ref="B1501:F1501"/>
-    <mergeCell ref="B1502:F1502"/>
-    <mergeCell ref="B1503:F1503"/>
-    <mergeCell ref="B1504:F1504"/>
-    <mergeCell ref="B1505:F1505"/>
-    <mergeCell ref="B1506:F1506"/>
-    <mergeCell ref="B1495:F1495"/>
-    <mergeCell ref="B1496:F1496"/>
-    <mergeCell ref="B1497:F1497"/>
-    <mergeCell ref="B1498:F1498"/>
-    <mergeCell ref="B1499:F1499"/>
-    <mergeCell ref="B1500:F1500"/>
-    <mergeCell ref="B1489:F1489"/>
-    <mergeCell ref="B1490:F1490"/>
-    <mergeCell ref="B1491:F1491"/>
-    <mergeCell ref="B1492:F1492"/>
-    <mergeCell ref="B1493:F1493"/>
-    <mergeCell ref="B1494:F1494"/>
-    <mergeCell ref="B1519:F1519"/>
-    <mergeCell ref="B1520:F1520"/>
-    <mergeCell ref="B1521:F1521"/>
-    <mergeCell ref="B1522:F1522"/>
-    <mergeCell ref="B1523:F1523"/>
-    <mergeCell ref="B1524:F1524"/>
-    <mergeCell ref="B1513:F1513"/>
-    <mergeCell ref="B1514:F1514"/>
-    <mergeCell ref="B1515:F1515"/>
-    <mergeCell ref="B1516:F1516"/>
-    <mergeCell ref="B1517:F1517"/>
-    <mergeCell ref="B1518:F1518"/>
-    <mergeCell ref="B1507:F1507"/>
-    <mergeCell ref="B1508:F1508"/>
-    <mergeCell ref="B1509:F1509"/>
-    <mergeCell ref="B1510:F1510"/>
-    <mergeCell ref="B1511:F1511"/>
-    <mergeCell ref="B1512:F1512"/>
-    <mergeCell ref="B1537:F1537"/>
-    <mergeCell ref="B1538:F1538"/>
-    <mergeCell ref="B1539:F1539"/>
-    <mergeCell ref="B1540:F1540"/>
-    <mergeCell ref="B1541:F1541"/>
-    <mergeCell ref="B1542:F1542"/>
-    <mergeCell ref="B1531:F1531"/>
-    <mergeCell ref="B1532:F1532"/>
-    <mergeCell ref="B1533:F1533"/>
-    <mergeCell ref="B1534:F1534"/>
-    <mergeCell ref="B1535:F1535"/>
-    <mergeCell ref="B1536:F1536"/>
-    <mergeCell ref="B1525:F1525"/>
-    <mergeCell ref="B1526:F1526"/>
-    <mergeCell ref="B1527:F1527"/>
-    <mergeCell ref="B1528:F1528"/>
-    <mergeCell ref="B1529:F1529"/>
-    <mergeCell ref="B1530:F1530"/>
-    <mergeCell ref="B1555:F1555"/>
-    <mergeCell ref="B1556:F1556"/>
-    <mergeCell ref="B1557:F1557"/>
-    <mergeCell ref="B1558:F1558"/>
-    <mergeCell ref="B1559:F1559"/>
-    <mergeCell ref="B1560:F1560"/>
-    <mergeCell ref="B1549:F1549"/>
-    <mergeCell ref="B1550:F1550"/>
-    <mergeCell ref="B1551:F1551"/>
-    <mergeCell ref="B1552:F1552"/>
-    <mergeCell ref="B1553:F1553"/>
-    <mergeCell ref="B1554:F1554"/>
-    <mergeCell ref="B1543:F1543"/>
-    <mergeCell ref="B1544:F1544"/>
-    <mergeCell ref="B1545:F1545"/>
-    <mergeCell ref="B1546:F1546"/>
-    <mergeCell ref="B1547:F1547"/>
-    <mergeCell ref="B1548:F1548"/>
-    <mergeCell ref="B1573:F1573"/>
-    <mergeCell ref="B1574:F1574"/>
-    <mergeCell ref="B1575:F1575"/>
-    <mergeCell ref="B1576:F1576"/>
-    <mergeCell ref="B1577:F1577"/>
-    <mergeCell ref="B1578:F1578"/>
-    <mergeCell ref="B1567:F1567"/>
-    <mergeCell ref="B1568:F1568"/>
-    <mergeCell ref="B1569:F1569"/>
-    <mergeCell ref="B1570:F1570"/>
-    <mergeCell ref="B1571:F1571"/>
-    <mergeCell ref="B1572:F1572"/>
-    <mergeCell ref="B1561:F1561"/>
-    <mergeCell ref="B1562:F1562"/>
-    <mergeCell ref="B1563:F1563"/>
-    <mergeCell ref="B1564:F1564"/>
-    <mergeCell ref="B1565:F1565"/>
-    <mergeCell ref="B1566:F1566"/>
-    <mergeCell ref="B1591:F1591"/>
-    <mergeCell ref="B1592:F1592"/>
-    <mergeCell ref="B1593:F1593"/>
-    <mergeCell ref="B1594:F1594"/>
-    <mergeCell ref="B1595:F1595"/>
-    <mergeCell ref="B1596:F1596"/>
-    <mergeCell ref="B1585:F1585"/>
-    <mergeCell ref="B1586:F1586"/>
-    <mergeCell ref="B1587:F1587"/>
-    <mergeCell ref="B1588:F1588"/>
-    <mergeCell ref="B1589:F1589"/>
-    <mergeCell ref="B1590:F1590"/>
-    <mergeCell ref="B1579:F1579"/>
-    <mergeCell ref="B1580:F1580"/>
-    <mergeCell ref="B1581:F1581"/>
-    <mergeCell ref="B1582:F1582"/>
-    <mergeCell ref="B1583:F1583"/>
-    <mergeCell ref="B1584:F1584"/>
-    <mergeCell ref="B1609:F1609"/>
-    <mergeCell ref="B1610:F1610"/>
-    <mergeCell ref="B1611:F1611"/>
-    <mergeCell ref="B1612:F1612"/>
-    <mergeCell ref="B1613:F1613"/>
-    <mergeCell ref="B1614:F1614"/>
-    <mergeCell ref="B1603:F1603"/>
-    <mergeCell ref="B1604:F1604"/>
-    <mergeCell ref="B1605:F1605"/>
-    <mergeCell ref="B1606:F1606"/>
-    <mergeCell ref="B1607:F1607"/>
-    <mergeCell ref="B1608:F1608"/>
-    <mergeCell ref="B1597:F1597"/>
-    <mergeCell ref="B1598:F1598"/>
-    <mergeCell ref="B1599:F1599"/>
-    <mergeCell ref="B1600:F1600"/>
-    <mergeCell ref="B1601:F1601"/>
-    <mergeCell ref="B1602:F1602"/>
-    <mergeCell ref="B1627:F1627"/>
-    <mergeCell ref="B1628:F1628"/>
-    <mergeCell ref="B1629:F1629"/>
-    <mergeCell ref="B1630:F1630"/>
-    <mergeCell ref="B1631:F1631"/>
-    <mergeCell ref="B1632:F1632"/>
-    <mergeCell ref="B1621:F1621"/>
-    <mergeCell ref="B1622:F1622"/>
-    <mergeCell ref="B1623:F1623"/>
-    <mergeCell ref="B1624:F1624"/>
-    <mergeCell ref="B1625:F1625"/>
-    <mergeCell ref="B1626:F1626"/>
-    <mergeCell ref="B1615:F1615"/>
-    <mergeCell ref="B1616:F1616"/>
-    <mergeCell ref="B1617:F1617"/>
-    <mergeCell ref="B1618:F1618"/>
-    <mergeCell ref="B1619:F1619"/>
-    <mergeCell ref="B1620:F1620"/>
-    <mergeCell ref="B1645:F1645"/>
-    <mergeCell ref="B1646:F1646"/>
-    <mergeCell ref="B1647:F1647"/>
-    <mergeCell ref="B1648:F1648"/>
-    <mergeCell ref="B1649:F1649"/>
-    <mergeCell ref="B1650:F1650"/>
-    <mergeCell ref="B1639:F1639"/>
-    <mergeCell ref="B1640:F1640"/>
-    <mergeCell ref="B1641:F1641"/>
-    <mergeCell ref="B1642:F1642"/>
-    <mergeCell ref="B1643:F1643"/>
-    <mergeCell ref="B1644:F1644"/>
-    <mergeCell ref="B1633:F1633"/>
-    <mergeCell ref="B1634:F1634"/>
-    <mergeCell ref="B1635:F1635"/>
-    <mergeCell ref="B1636:F1636"/>
-    <mergeCell ref="B1637:F1637"/>
-    <mergeCell ref="B1638:F1638"/>
-    <mergeCell ref="B1663:F1663"/>
-    <mergeCell ref="B1664:F1664"/>
-    <mergeCell ref="B1665:F1665"/>
-    <mergeCell ref="B1666:F1666"/>
-    <mergeCell ref="B1667:F1667"/>
-    <mergeCell ref="B1668:F1668"/>
-    <mergeCell ref="B1657:F1657"/>
-    <mergeCell ref="B1658:F1658"/>
-    <mergeCell ref="B1659:F1659"/>
-    <mergeCell ref="B1660:F1660"/>
-    <mergeCell ref="B1661:F1661"/>
-    <mergeCell ref="B1662:F1662"/>
-    <mergeCell ref="B1651:F1651"/>
-    <mergeCell ref="B1652:F1652"/>
-    <mergeCell ref="B1653:F1653"/>
-    <mergeCell ref="B1654:F1654"/>
-    <mergeCell ref="B1655:F1655"/>
-    <mergeCell ref="B1656:F1656"/>
-    <mergeCell ref="B1681:F1681"/>
-    <mergeCell ref="B1682:F1682"/>
-    <mergeCell ref="B1683:F1683"/>
-    <mergeCell ref="B1684:F1684"/>
-    <mergeCell ref="B1685:F1685"/>
-    <mergeCell ref="B1686:F1686"/>
-    <mergeCell ref="B1675:F1675"/>
-    <mergeCell ref="B1676:F1676"/>
-    <mergeCell ref="B1677:F1677"/>
-    <mergeCell ref="B1678:F1678"/>
-    <mergeCell ref="B1679:F1679"/>
-    <mergeCell ref="B1680:F1680"/>
-    <mergeCell ref="B1669:F1669"/>
-    <mergeCell ref="B1670:F1670"/>
-    <mergeCell ref="B1671:F1671"/>
-    <mergeCell ref="B1672:F1672"/>
-    <mergeCell ref="B1673:F1673"/>
-    <mergeCell ref="B1674:F1674"/>
-    <mergeCell ref="B1699:F1699"/>
-    <mergeCell ref="B1700:F1700"/>
-    <mergeCell ref="B1701:F1701"/>
-    <mergeCell ref="B1702:F1702"/>
-    <mergeCell ref="B1703:F1703"/>
-    <mergeCell ref="B1704:F1704"/>
-    <mergeCell ref="B1693:F1693"/>
-    <mergeCell ref="B1694:F1694"/>
-    <mergeCell ref="B1695:F1695"/>
-    <mergeCell ref="B1696:F1696"/>
-    <mergeCell ref="B1697:F1697"/>
-    <mergeCell ref="B1698:F1698"/>
-    <mergeCell ref="B1687:F1687"/>
-    <mergeCell ref="B1688:F1688"/>
-    <mergeCell ref="B1689:F1689"/>
-    <mergeCell ref="B1690:F1690"/>
-    <mergeCell ref="B1691:F1691"/>
-    <mergeCell ref="B1692:F1692"/>
-    <mergeCell ref="B1717:F1717"/>
-    <mergeCell ref="B1718:F1718"/>
-    <mergeCell ref="B1719:F1719"/>
-    <mergeCell ref="B1720:F1720"/>
-    <mergeCell ref="B1721:F1721"/>
-    <mergeCell ref="B1722:F1722"/>
-    <mergeCell ref="B1711:F1711"/>
-    <mergeCell ref="B1712:F1712"/>
-    <mergeCell ref="B1713:F1713"/>
-    <mergeCell ref="B1714:F1714"/>
-    <mergeCell ref="B1715:F1715"/>
-    <mergeCell ref="B1716:F1716"/>
-    <mergeCell ref="B1705:F1705"/>
-    <mergeCell ref="B1706:F1706"/>
-    <mergeCell ref="B1707:F1707"/>
-    <mergeCell ref="B1708:F1708"/>
-    <mergeCell ref="B1709:F1709"/>
-    <mergeCell ref="B1710:F1710"/>
-    <mergeCell ref="B1735:F1735"/>
-    <mergeCell ref="B1736:F1736"/>
-    <mergeCell ref="B1737:F1737"/>
-    <mergeCell ref="B1738:F1738"/>
-    <mergeCell ref="B1739:F1739"/>
-    <mergeCell ref="B1740:F1740"/>
-    <mergeCell ref="B1729:F1729"/>
-    <mergeCell ref="B1730:F1730"/>
-    <mergeCell ref="B1731:F1731"/>
-    <mergeCell ref="B1732:F1732"/>
-    <mergeCell ref="B1733:F1733"/>
-    <mergeCell ref="B1734:F1734"/>
-    <mergeCell ref="B1723:F1723"/>
-    <mergeCell ref="B1724:F1724"/>
-    <mergeCell ref="B1725:F1725"/>
-    <mergeCell ref="B1726:F1726"/>
-    <mergeCell ref="B1727:F1727"/>
-    <mergeCell ref="B1728:F1728"/>
-    <mergeCell ref="B1753:F1753"/>
-    <mergeCell ref="B1754:F1754"/>
-    <mergeCell ref="B1755:F1755"/>
-    <mergeCell ref="B1756:F1756"/>
-    <mergeCell ref="B1757:F1757"/>
-    <mergeCell ref="B1758:F1758"/>
-    <mergeCell ref="B1747:F1747"/>
-    <mergeCell ref="B1748:F1748"/>
-    <mergeCell ref="B1749:F1749"/>
-    <mergeCell ref="B1750:F1750"/>
-    <mergeCell ref="B1751:F1751"/>
-    <mergeCell ref="B1752:F1752"/>
-    <mergeCell ref="B1741:F1741"/>
-    <mergeCell ref="B1742:F1742"/>
-    <mergeCell ref="B1743:F1743"/>
-    <mergeCell ref="B1744:F1744"/>
-    <mergeCell ref="B1745:F1745"/>
-    <mergeCell ref="B1746:F1746"/>
-    <mergeCell ref="B1771:F1771"/>
-    <mergeCell ref="B1772:F1772"/>
-    <mergeCell ref="B1773:F1773"/>
-    <mergeCell ref="B1774:F1774"/>
-    <mergeCell ref="B1775:F1775"/>
-    <mergeCell ref="B1776:F1776"/>
-    <mergeCell ref="B1765:F1765"/>
-    <mergeCell ref="B1766:F1766"/>
-    <mergeCell ref="B1767:F1767"/>
-    <mergeCell ref="B1768:F1768"/>
-    <mergeCell ref="B1769:F1769"/>
-    <mergeCell ref="B1770:F1770"/>
-    <mergeCell ref="B1759:F1759"/>
-    <mergeCell ref="B1760:F1760"/>
-    <mergeCell ref="B1761:F1761"/>
-    <mergeCell ref="B1762:F1762"/>
-    <mergeCell ref="B1763:F1763"/>
-    <mergeCell ref="B1764:F1764"/>
-    <mergeCell ref="B1789:F1789"/>
-    <mergeCell ref="B1790:F1790"/>
-    <mergeCell ref="B1791:F1791"/>
-    <mergeCell ref="B1792:F1792"/>
-    <mergeCell ref="B1793:F1793"/>
-    <mergeCell ref="B1794:F1794"/>
-    <mergeCell ref="B1783:F1783"/>
-    <mergeCell ref="B1784:F1784"/>
-    <mergeCell ref="B1785:F1785"/>
-    <mergeCell ref="B1786:F1786"/>
-    <mergeCell ref="B1787:F1787"/>
-    <mergeCell ref="B1788:F1788"/>
-    <mergeCell ref="B1777:F1777"/>
-    <mergeCell ref="B1778:F1778"/>
-    <mergeCell ref="B1779:F1779"/>
-    <mergeCell ref="B1780:F1780"/>
-    <mergeCell ref="B1781:F1781"/>
-    <mergeCell ref="B1782:F1782"/>
-    <mergeCell ref="B1807:F1807"/>
-    <mergeCell ref="B1808:F1808"/>
-    <mergeCell ref="B1809:F1809"/>
-    <mergeCell ref="B1810:F1810"/>
-    <mergeCell ref="B1811:F1811"/>
-    <mergeCell ref="B1812:F1812"/>
-    <mergeCell ref="B1801:F1801"/>
-    <mergeCell ref="B1802:F1802"/>
-    <mergeCell ref="B1803:F1803"/>
-    <mergeCell ref="B1804:F1804"/>
-    <mergeCell ref="B1805:F1805"/>
-    <mergeCell ref="B1806:F1806"/>
-    <mergeCell ref="B1795:F1795"/>
-    <mergeCell ref="B1796:F1796"/>
-    <mergeCell ref="B1797:F1797"/>
-    <mergeCell ref="B1798:F1798"/>
-    <mergeCell ref="B1799:F1799"/>
-    <mergeCell ref="B1800:F1800"/>
-    <mergeCell ref="B1825:F1825"/>
-    <mergeCell ref="B1826:F1826"/>
-    <mergeCell ref="B1827:F1827"/>
-    <mergeCell ref="B1828:F1828"/>
-    <mergeCell ref="B1829:F1829"/>
-    <mergeCell ref="B1830:F1830"/>
-    <mergeCell ref="B1819:F1819"/>
-    <mergeCell ref="B1820:F1820"/>
-    <mergeCell ref="B1821:F1821"/>
-    <mergeCell ref="B1822:F1822"/>
-    <mergeCell ref="B1823:F1823"/>
-    <mergeCell ref="B1824:F1824"/>
-    <mergeCell ref="B1813:F1813"/>
-    <mergeCell ref="B1814:F1814"/>
-    <mergeCell ref="B1815:F1815"/>
-    <mergeCell ref="B1816:F1816"/>
-    <mergeCell ref="B1817:F1817"/>
-    <mergeCell ref="B1818:F1818"/>
-    <mergeCell ref="B1843:F1843"/>
-    <mergeCell ref="B1844:F1844"/>
-    <mergeCell ref="B1845:F1845"/>
-    <mergeCell ref="B1846:F1846"/>
-    <mergeCell ref="B1847:F1847"/>
-    <mergeCell ref="B1848:F1848"/>
-    <mergeCell ref="B1837:F1837"/>
-    <mergeCell ref="B1838:F1838"/>
-    <mergeCell ref="B1839:F1839"/>
-    <mergeCell ref="B1840:F1840"/>
-    <mergeCell ref="B1841:F1841"/>
-    <mergeCell ref="B1842:F1842"/>
-    <mergeCell ref="B1831:F1831"/>
-    <mergeCell ref="B1832:F1832"/>
-    <mergeCell ref="B1833:F1833"/>
-    <mergeCell ref="B1834:F1834"/>
-    <mergeCell ref="B1835:F1835"/>
-    <mergeCell ref="B1836:F1836"/>
-    <mergeCell ref="B1861:F1861"/>
-    <mergeCell ref="B1862:F1862"/>
-    <mergeCell ref="B1863:F1863"/>
-    <mergeCell ref="B1864:F1864"/>
-    <mergeCell ref="B1865:F1865"/>
-    <mergeCell ref="B1866:F1866"/>
-    <mergeCell ref="B1855:F1855"/>
-    <mergeCell ref="B1856:F1856"/>
-    <mergeCell ref="B1857:F1857"/>
-    <mergeCell ref="B1858:F1858"/>
-    <mergeCell ref="B1859:F1859"/>
-    <mergeCell ref="B1860:F1860"/>
-    <mergeCell ref="B1849:F1849"/>
-    <mergeCell ref="B1850:F1850"/>
-    <mergeCell ref="B1851:F1851"/>
-    <mergeCell ref="B1852:F1852"/>
-    <mergeCell ref="B1853:F1853"/>
-    <mergeCell ref="B1854:F1854"/>
-    <mergeCell ref="B1879:F1879"/>
-    <mergeCell ref="B1880:F1880"/>
-    <mergeCell ref="B1881:F1881"/>
-    <mergeCell ref="B1882:F1882"/>
-    <mergeCell ref="B1883:F1883"/>
-    <mergeCell ref="B1884:F1884"/>
-    <mergeCell ref="B1873:F1873"/>
-    <mergeCell ref="B1874:F1874"/>
-    <mergeCell ref="B1875:F1875"/>
-    <mergeCell ref="B1876:F1876"/>
-    <mergeCell ref="B1877:F1877"/>
-    <mergeCell ref="B1878:F1878"/>
-    <mergeCell ref="B1867:F1867"/>
-    <mergeCell ref="B1868:F1868"/>
-    <mergeCell ref="B1869:F1869"/>
-    <mergeCell ref="B1870:F1870"/>
-    <mergeCell ref="B1871:F1871"/>
-    <mergeCell ref="B1872:F1872"/>
-    <mergeCell ref="B1897:F1897"/>
-    <mergeCell ref="B1898:F1898"/>
-    <mergeCell ref="B1899:F1899"/>
-    <mergeCell ref="B1900:F1900"/>
-    <mergeCell ref="B1901:F1901"/>
-    <mergeCell ref="B1902:F1902"/>
-    <mergeCell ref="B1891:F1891"/>
-    <mergeCell ref="B1892:F1892"/>
-    <mergeCell ref="B1893:F1893"/>
-    <mergeCell ref="B1894:F1894"/>
-    <mergeCell ref="B1895:F1895"/>
-    <mergeCell ref="B1896:F1896"/>
-    <mergeCell ref="B1885:F1885"/>
-    <mergeCell ref="B1886:F1886"/>
-    <mergeCell ref="B1887:F1887"/>
-    <mergeCell ref="B1888:F1888"/>
-    <mergeCell ref="B1889:F1889"/>
-    <mergeCell ref="B1890:F1890"/>
-    <mergeCell ref="B1915:F1915"/>
-    <mergeCell ref="B1916:F1916"/>
-    <mergeCell ref="B1917:F1917"/>
-    <mergeCell ref="B1918:F1918"/>
-    <mergeCell ref="B1919:F1919"/>
-    <mergeCell ref="B1920:F1920"/>
-    <mergeCell ref="B1909:F1909"/>
-    <mergeCell ref="B1910:F1910"/>
-    <mergeCell ref="B1911:F1911"/>
-    <mergeCell ref="B1912:F1912"/>
-    <mergeCell ref="B1913:F1913"/>
-    <mergeCell ref="B1914:F1914"/>
-    <mergeCell ref="B1903:F1903"/>
-    <mergeCell ref="B1904:F1904"/>
-    <mergeCell ref="B1905:F1905"/>
-    <mergeCell ref="B1906:F1906"/>
-    <mergeCell ref="B1907:F1907"/>
-    <mergeCell ref="B1908:F1908"/>
-    <mergeCell ref="B1933:F1933"/>
-    <mergeCell ref="B1934:F1934"/>
-    <mergeCell ref="B1935:F1935"/>
-    <mergeCell ref="B1936:F1936"/>
-    <mergeCell ref="B1937:F1937"/>
-    <mergeCell ref="B1938:F1938"/>
-    <mergeCell ref="B1927:F1927"/>
-    <mergeCell ref="B1928:F1928"/>
-    <mergeCell ref="B1929:F1929"/>
-    <mergeCell ref="B1930:F1930"/>
-    <mergeCell ref="B1931:F1931"/>
-    <mergeCell ref="B1932:F1932"/>
-    <mergeCell ref="B1921:F1921"/>
-    <mergeCell ref="B1922:F1922"/>
-    <mergeCell ref="B1923:F1923"/>
-    <mergeCell ref="B1924:F1924"/>
-    <mergeCell ref="B1925:F1925"/>
-    <mergeCell ref="B1926:F1926"/>
-    <mergeCell ref="B1951:F1951"/>
-    <mergeCell ref="B1952:F1952"/>
-    <mergeCell ref="B1953:F1953"/>
-    <mergeCell ref="B1954:F1954"/>
-    <mergeCell ref="B1955:F1955"/>
-    <mergeCell ref="B1956:F1956"/>
-    <mergeCell ref="B1945:F1945"/>
-    <mergeCell ref="B1946:F1946"/>
-    <mergeCell ref="B1947:F1947"/>
-    <mergeCell ref="B1948:F1948"/>
-    <mergeCell ref="B1949:F1949"/>
-    <mergeCell ref="B1950:F1950"/>
-    <mergeCell ref="B1939:F1939"/>
-    <mergeCell ref="B1940:F1940"/>
-    <mergeCell ref="B1941:F1941"/>
-    <mergeCell ref="B1942:F1942"/>
-    <mergeCell ref="B1943:F1943"/>
-    <mergeCell ref="B1944:F1944"/>
-    <mergeCell ref="B1969:F1969"/>
-    <mergeCell ref="B1970:F1970"/>
-    <mergeCell ref="B1971:F1971"/>
-    <mergeCell ref="B1972:F1972"/>
-    <mergeCell ref="B1973:F1973"/>
-    <mergeCell ref="B1974:F1974"/>
-    <mergeCell ref="B1963:F1963"/>
-    <mergeCell ref="B1964:F1964"/>
-    <mergeCell ref="B1965:F1965"/>
-    <mergeCell ref="B1966:F1966"/>
-    <mergeCell ref="B1967:F1967"/>
-    <mergeCell ref="B1968:F1968"/>
-    <mergeCell ref="B1957:F1957"/>
-    <mergeCell ref="B1958:F1958"/>
-    <mergeCell ref="B1959:F1959"/>
-    <mergeCell ref="B1960:F1960"/>
-    <mergeCell ref="B1961:F1961"/>
-    <mergeCell ref="B1962:F1962"/>
     <mergeCell ref="B1993:F1993"/>
     <mergeCell ref="B1994:F1994"/>
     <mergeCell ref="B1995:F1995"/>
@@ -16712,6 +14793,1980 @@
     <mergeCell ref="B1978:F1978"/>
     <mergeCell ref="B1979:F1979"/>
     <mergeCell ref="B1980:F1980"/>
+    <mergeCell ref="B1969:F1969"/>
+    <mergeCell ref="B1970:F1970"/>
+    <mergeCell ref="B1971:F1971"/>
+    <mergeCell ref="B1972:F1972"/>
+    <mergeCell ref="B1973:F1973"/>
+    <mergeCell ref="B1974:F1974"/>
+    <mergeCell ref="B1963:F1963"/>
+    <mergeCell ref="B1964:F1964"/>
+    <mergeCell ref="B1965:F1965"/>
+    <mergeCell ref="B1966:F1966"/>
+    <mergeCell ref="B1967:F1967"/>
+    <mergeCell ref="B1968:F1968"/>
+    <mergeCell ref="B1957:F1957"/>
+    <mergeCell ref="B1958:F1958"/>
+    <mergeCell ref="B1959:F1959"/>
+    <mergeCell ref="B1960:F1960"/>
+    <mergeCell ref="B1961:F1961"/>
+    <mergeCell ref="B1962:F1962"/>
+    <mergeCell ref="B1951:F1951"/>
+    <mergeCell ref="B1952:F1952"/>
+    <mergeCell ref="B1953:F1953"/>
+    <mergeCell ref="B1954:F1954"/>
+    <mergeCell ref="B1955:F1955"/>
+    <mergeCell ref="B1956:F1956"/>
+    <mergeCell ref="B1945:F1945"/>
+    <mergeCell ref="B1946:F1946"/>
+    <mergeCell ref="B1947:F1947"/>
+    <mergeCell ref="B1948:F1948"/>
+    <mergeCell ref="B1949:F1949"/>
+    <mergeCell ref="B1950:F1950"/>
+    <mergeCell ref="B1939:F1939"/>
+    <mergeCell ref="B1940:F1940"/>
+    <mergeCell ref="B1941:F1941"/>
+    <mergeCell ref="B1942:F1942"/>
+    <mergeCell ref="B1943:F1943"/>
+    <mergeCell ref="B1944:F1944"/>
+    <mergeCell ref="B1933:F1933"/>
+    <mergeCell ref="B1934:F1934"/>
+    <mergeCell ref="B1935:F1935"/>
+    <mergeCell ref="B1936:F1936"/>
+    <mergeCell ref="B1937:F1937"/>
+    <mergeCell ref="B1938:F1938"/>
+    <mergeCell ref="B1927:F1927"/>
+    <mergeCell ref="B1928:F1928"/>
+    <mergeCell ref="B1929:F1929"/>
+    <mergeCell ref="B1930:F1930"/>
+    <mergeCell ref="B1931:F1931"/>
+    <mergeCell ref="B1932:F1932"/>
+    <mergeCell ref="B1921:F1921"/>
+    <mergeCell ref="B1922:F1922"/>
+    <mergeCell ref="B1923:F1923"/>
+    <mergeCell ref="B1924:F1924"/>
+    <mergeCell ref="B1925:F1925"/>
+    <mergeCell ref="B1926:F1926"/>
+    <mergeCell ref="B1915:F1915"/>
+    <mergeCell ref="B1916:F1916"/>
+    <mergeCell ref="B1917:F1917"/>
+    <mergeCell ref="B1918:F1918"/>
+    <mergeCell ref="B1919:F1919"/>
+    <mergeCell ref="B1920:F1920"/>
+    <mergeCell ref="B1909:F1909"/>
+    <mergeCell ref="B1910:F1910"/>
+    <mergeCell ref="B1911:F1911"/>
+    <mergeCell ref="B1912:F1912"/>
+    <mergeCell ref="B1913:F1913"/>
+    <mergeCell ref="B1914:F1914"/>
+    <mergeCell ref="B1903:F1903"/>
+    <mergeCell ref="B1904:F1904"/>
+    <mergeCell ref="B1905:F1905"/>
+    <mergeCell ref="B1906:F1906"/>
+    <mergeCell ref="B1907:F1907"/>
+    <mergeCell ref="B1908:F1908"/>
+    <mergeCell ref="B1897:F1897"/>
+    <mergeCell ref="B1898:F1898"/>
+    <mergeCell ref="B1899:F1899"/>
+    <mergeCell ref="B1900:F1900"/>
+    <mergeCell ref="B1901:F1901"/>
+    <mergeCell ref="B1902:F1902"/>
+    <mergeCell ref="B1891:F1891"/>
+    <mergeCell ref="B1892:F1892"/>
+    <mergeCell ref="B1893:F1893"/>
+    <mergeCell ref="B1894:F1894"/>
+    <mergeCell ref="B1895:F1895"/>
+    <mergeCell ref="B1896:F1896"/>
+    <mergeCell ref="B1885:F1885"/>
+    <mergeCell ref="B1886:F1886"/>
+    <mergeCell ref="B1887:F1887"/>
+    <mergeCell ref="B1888:F1888"/>
+    <mergeCell ref="B1889:F1889"/>
+    <mergeCell ref="B1890:F1890"/>
+    <mergeCell ref="B1879:F1879"/>
+    <mergeCell ref="B1880:F1880"/>
+    <mergeCell ref="B1881:F1881"/>
+    <mergeCell ref="B1882:F1882"/>
+    <mergeCell ref="B1883:F1883"/>
+    <mergeCell ref="B1884:F1884"/>
+    <mergeCell ref="B1873:F1873"/>
+    <mergeCell ref="B1874:F1874"/>
+    <mergeCell ref="B1875:F1875"/>
+    <mergeCell ref="B1876:F1876"/>
+    <mergeCell ref="B1877:F1877"/>
+    <mergeCell ref="B1878:F1878"/>
+    <mergeCell ref="B1867:F1867"/>
+    <mergeCell ref="B1868:F1868"/>
+    <mergeCell ref="B1869:F1869"/>
+    <mergeCell ref="B1870:F1870"/>
+    <mergeCell ref="B1871:F1871"/>
+    <mergeCell ref="B1872:F1872"/>
+    <mergeCell ref="B1861:F1861"/>
+    <mergeCell ref="B1862:F1862"/>
+    <mergeCell ref="B1863:F1863"/>
+    <mergeCell ref="B1864:F1864"/>
+    <mergeCell ref="B1865:F1865"/>
+    <mergeCell ref="B1866:F1866"/>
+    <mergeCell ref="B1855:F1855"/>
+    <mergeCell ref="B1856:F1856"/>
+    <mergeCell ref="B1857:F1857"/>
+    <mergeCell ref="B1858:F1858"/>
+    <mergeCell ref="B1859:F1859"/>
+    <mergeCell ref="B1860:F1860"/>
+    <mergeCell ref="B1849:F1849"/>
+    <mergeCell ref="B1850:F1850"/>
+    <mergeCell ref="B1851:F1851"/>
+    <mergeCell ref="B1852:F1852"/>
+    <mergeCell ref="B1853:F1853"/>
+    <mergeCell ref="B1854:F1854"/>
+    <mergeCell ref="B1843:F1843"/>
+    <mergeCell ref="B1844:F1844"/>
+    <mergeCell ref="B1845:F1845"/>
+    <mergeCell ref="B1846:F1846"/>
+    <mergeCell ref="B1847:F1847"/>
+    <mergeCell ref="B1848:F1848"/>
+    <mergeCell ref="B1837:F1837"/>
+    <mergeCell ref="B1838:F1838"/>
+    <mergeCell ref="B1839:F1839"/>
+    <mergeCell ref="B1840:F1840"/>
+    <mergeCell ref="B1841:F1841"/>
+    <mergeCell ref="B1842:F1842"/>
+    <mergeCell ref="B1831:F1831"/>
+    <mergeCell ref="B1832:F1832"/>
+    <mergeCell ref="B1833:F1833"/>
+    <mergeCell ref="B1834:F1834"/>
+    <mergeCell ref="B1835:F1835"/>
+    <mergeCell ref="B1836:F1836"/>
+    <mergeCell ref="B1825:F1825"/>
+    <mergeCell ref="B1826:F1826"/>
+    <mergeCell ref="B1827:F1827"/>
+    <mergeCell ref="B1828:F1828"/>
+    <mergeCell ref="B1829:F1829"/>
+    <mergeCell ref="B1830:F1830"/>
+    <mergeCell ref="B1819:F1819"/>
+    <mergeCell ref="B1820:F1820"/>
+    <mergeCell ref="B1821:F1821"/>
+    <mergeCell ref="B1822:F1822"/>
+    <mergeCell ref="B1823:F1823"/>
+    <mergeCell ref="B1824:F1824"/>
+    <mergeCell ref="B1813:F1813"/>
+    <mergeCell ref="B1814:F1814"/>
+    <mergeCell ref="B1815:F1815"/>
+    <mergeCell ref="B1816:F1816"/>
+    <mergeCell ref="B1817:F1817"/>
+    <mergeCell ref="B1818:F1818"/>
+    <mergeCell ref="B1807:F1807"/>
+    <mergeCell ref="B1808:F1808"/>
+    <mergeCell ref="B1809:F1809"/>
+    <mergeCell ref="B1810:F1810"/>
+    <mergeCell ref="B1811:F1811"/>
+    <mergeCell ref="B1812:F1812"/>
+    <mergeCell ref="B1801:F1801"/>
+    <mergeCell ref="B1802:F1802"/>
+    <mergeCell ref="B1803:F1803"/>
+    <mergeCell ref="B1804:F1804"/>
+    <mergeCell ref="B1805:F1805"/>
+    <mergeCell ref="B1806:F1806"/>
+    <mergeCell ref="B1795:F1795"/>
+    <mergeCell ref="B1796:F1796"/>
+    <mergeCell ref="B1797:F1797"/>
+    <mergeCell ref="B1798:F1798"/>
+    <mergeCell ref="B1799:F1799"/>
+    <mergeCell ref="B1800:F1800"/>
+    <mergeCell ref="B1789:F1789"/>
+    <mergeCell ref="B1790:F1790"/>
+    <mergeCell ref="B1791:F1791"/>
+    <mergeCell ref="B1792:F1792"/>
+    <mergeCell ref="B1793:F1793"/>
+    <mergeCell ref="B1794:F1794"/>
+    <mergeCell ref="B1783:F1783"/>
+    <mergeCell ref="B1784:F1784"/>
+    <mergeCell ref="B1785:F1785"/>
+    <mergeCell ref="B1786:F1786"/>
+    <mergeCell ref="B1787:F1787"/>
+    <mergeCell ref="B1788:F1788"/>
+    <mergeCell ref="B1777:F1777"/>
+    <mergeCell ref="B1778:F1778"/>
+    <mergeCell ref="B1779:F1779"/>
+    <mergeCell ref="B1780:F1780"/>
+    <mergeCell ref="B1781:F1781"/>
+    <mergeCell ref="B1782:F1782"/>
+    <mergeCell ref="B1771:F1771"/>
+    <mergeCell ref="B1772:F1772"/>
+    <mergeCell ref="B1773:F1773"/>
+    <mergeCell ref="B1774:F1774"/>
+    <mergeCell ref="B1775:F1775"/>
+    <mergeCell ref="B1776:F1776"/>
+    <mergeCell ref="B1765:F1765"/>
+    <mergeCell ref="B1766:F1766"/>
+    <mergeCell ref="B1767:F1767"/>
+    <mergeCell ref="B1768:F1768"/>
+    <mergeCell ref="B1769:F1769"/>
+    <mergeCell ref="B1770:F1770"/>
+    <mergeCell ref="B1759:F1759"/>
+    <mergeCell ref="B1760:F1760"/>
+    <mergeCell ref="B1761:F1761"/>
+    <mergeCell ref="B1762:F1762"/>
+    <mergeCell ref="B1763:F1763"/>
+    <mergeCell ref="B1764:F1764"/>
+    <mergeCell ref="B1753:F1753"/>
+    <mergeCell ref="B1754:F1754"/>
+    <mergeCell ref="B1755:F1755"/>
+    <mergeCell ref="B1756:F1756"/>
+    <mergeCell ref="B1757:F1757"/>
+    <mergeCell ref="B1758:F1758"/>
+    <mergeCell ref="B1747:F1747"/>
+    <mergeCell ref="B1748:F1748"/>
+    <mergeCell ref="B1749:F1749"/>
+    <mergeCell ref="B1750:F1750"/>
+    <mergeCell ref="B1751:F1751"/>
+    <mergeCell ref="B1752:F1752"/>
+    <mergeCell ref="B1741:F1741"/>
+    <mergeCell ref="B1742:F1742"/>
+    <mergeCell ref="B1743:F1743"/>
+    <mergeCell ref="B1744:F1744"/>
+    <mergeCell ref="B1745:F1745"/>
+    <mergeCell ref="B1746:F1746"/>
+    <mergeCell ref="B1735:F1735"/>
+    <mergeCell ref="B1736:F1736"/>
+    <mergeCell ref="B1737:F1737"/>
+    <mergeCell ref="B1738:F1738"/>
+    <mergeCell ref="B1739:F1739"/>
+    <mergeCell ref="B1740:F1740"/>
+    <mergeCell ref="B1729:F1729"/>
+    <mergeCell ref="B1730:F1730"/>
+    <mergeCell ref="B1731:F1731"/>
+    <mergeCell ref="B1732:F1732"/>
+    <mergeCell ref="B1733:F1733"/>
+    <mergeCell ref="B1734:F1734"/>
+    <mergeCell ref="B1723:F1723"/>
+    <mergeCell ref="B1724:F1724"/>
+    <mergeCell ref="B1725:F1725"/>
+    <mergeCell ref="B1726:F1726"/>
+    <mergeCell ref="B1727:F1727"/>
+    <mergeCell ref="B1728:F1728"/>
+    <mergeCell ref="B1717:F1717"/>
+    <mergeCell ref="B1718:F1718"/>
+    <mergeCell ref="B1719:F1719"/>
+    <mergeCell ref="B1720:F1720"/>
+    <mergeCell ref="B1721:F1721"/>
+    <mergeCell ref="B1722:F1722"/>
+    <mergeCell ref="B1711:F1711"/>
+    <mergeCell ref="B1712:F1712"/>
+    <mergeCell ref="B1713:F1713"/>
+    <mergeCell ref="B1714:F1714"/>
+    <mergeCell ref="B1715:F1715"/>
+    <mergeCell ref="B1716:F1716"/>
+    <mergeCell ref="B1705:F1705"/>
+    <mergeCell ref="B1706:F1706"/>
+    <mergeCell ref="B1707:F1707"/>
+    <mergeCell ref="B1708:F1708"/>
+    <mergeCell ref="B1709:F1709"/>
+    <mergeCell ref="B1710:F1710"/>
+    <mergeCell ref="B1699:F1699"/>
+    <mergeCell ref="B1700:F1700"/>
+    <mergeCell ref="B1701:F1701"/>
+    <mergeCell ref="B1702:F1702"/>
+    <mergeCell ref="B1703:F1703"/>
+    <mergeCell ref="B1704:F1704"/>
+    <mergeCell ref="B1693:F1693"/>
+    <mergeCell ref="B1694:F1694"/>
+    <mergeCell ref="B1695:F1695"/>
+    <mergeCell ref="B1696:F1696"/>
+    <mergeCell ref="B1697:F1697"/>
+    <mergeCell ref="B1698:F1698"/>
+    <mergeCell ref="B1687:F1687"/>
+    <mergeCell ref="B1688:F1688"/>
+    <mergeCell ref="B1689:F1689"/>
+    <mergeCell ref="B1690:F1690"/>
+    <mergeCell ref="B1691:F1691"/>
+    <mergeCell ref="B1692:F1692"/>
+    <mergeCell ref="B1681:F1681"/>
+    <mergeCell ref="B1682:F1682"/>
+    <mergeCell ref="B1683:F1683"/>
+    <mergeCell ref="B1684:F1684"/>
+    <mergeCell ref="B1685:F1685"/>
+    <mergeCell ref="B1686:F1686"/>
+    <mergeCell ref="B1675:F1675"/>
+    <mergeCell ref="B1676:F1676"/>
+    <mergeCell ref="B1677:F1677"/>
+    <mergeCell ref="B1678:F1678"/>
+    <mergeCell ref="B1679:F1679"/>
+    <mergeCell ref="B1680:F1680"/>
+    <mergeCell ref="B1669:F1669"/>
+    <mergeCell ref="B1670:F1670"/>
+    <mergeCell ref="B1671:F1671"/>
+    <mergeCell ref="B1672:F1672"/>
+    <mergeCell ref="B1673:F1673"/>
+    <mergeCell ref="B1674:F1674"/>
+    <mergeCell ref="B1663:F1663"/>
+    <mergeCell ref="B1664:F1664"/>
+    <mergeCell ref="B1665:F1665"/>
+    <mergeCell ref="B1666:F1666"/>
+    <mergeCell ref="B1667:F1667"/>
+    <mergeCell ref="B1668:F1668"/>
+    <mergeCell ref="B1657:F1657"/>
+    <mergeCell ref="B1658:F1658"/>
+    <mergeCell ref="B1659:F1659"/>
+    <mergeCell ref="B1660:F1660"/>
+    <mergeCell ref="B1661:F1661"/>
+    <mergeCell ref="B1662:F1662"/>
+    <mergeCell ref="B1651:F1651"/>
+    <mergeCell ref="B1652:F1652"/>
+    <mergeCell ref="B1653:F1653"/>
+    <mergeCell ref="B1654:F1654"/>
+    <mergeCell ref="B1655:F1655"/>
+    <mergeCell ref="B1656:F1656"/>
+    <mergeCell ref="B1645:F1645"/>
+    <mergeCell ref="B1646:F1646"/>
+    <mergeCell ref="B1647:F1647"/>
+    <mergeCell ref="B1648:F1648"/>
+    <mergeCell ref="B1649:F1649"/>
+    <mergeCell ref="B1650:F1650"/>
+    <mergeCell ref="B1639:F1639"/>
+    <mergeCell ref="B1640:F1640"/>
+    <mergeCell ref="B1641:F1641"/>
+    <mergeCell ref="B1642:F1642"/>
+    <mergeCell ref="B1643:F1643"/>
+    <mergeCell ref="B1644:F1644"/>
+    <mergeCell ref="B1633:F1633"/>
+    <mergeCell ref="B1634:F1634"/>
+    <mergeCell ref="B1635:F1635"/>
+    <mergeCell ref="B1636:F1636"/>
+    <mergeCell ref="B1637:F1637"/>
+    <mergeCell ref="B1638:F1638"/>
+    <mergeCell ref="B1627:F1627"/>
+    <mergeCell ref="B1628:F1628"/>
+    <mergeCell ref="B1629:F1629"/>
+    <mergeCell ref="B1630:F1630"/>
+    <mergeCell ref="B1631:F1631"/>
+    <mergeCell ref="B1632:F1632"/>
+    <mergeCell ref="B1621:F1621"/>
+    <mergeCell ref="B1622:F1622"/>
+    <mergeCell ref="B1623:F1623"/>
+    <mergeCell ref="B1624:F1624"/>
+    <mergeCell ref="B1625:F1625"/>
+    <mergeCell ref="B1626:F1626"/>
+    <mergeCell ref="B1615:F1615"/>
+    <mergeCell ref="B1616:F1616"/>
+    <mergeCell ref="B1617:F1617"/>
+    <mergeCell ref="B1618:F1618"/>
+    <mergeCell ref="B1619:F1619"/>
+    <mergeCell ref="B1620:F1620"/>
+    <mergeCell ref="B1609:F1609"/>
+    <mergeCell ref="B1610:F1610"/>
+    <mergeCell ref="B1611:F1611"/>
+    <mergeCell ref="B1612:F1612"/>
+    <mergeCell ref="B1613:F1613"/>
+    <mergeCell ref="B1614:F1614"/>
+    <mergeCell ref="B1603:F1603"/>
+    <mergeCell ref="B1604:F1604"/>
+    <mergeCell ref="B1605:F1605"/>
+    <mergeCell ref="B1606:F1606"/>
+    <mergeCell ref="B1607:F1607"/>
+    <mergeCell ref="B1608:F1608"/>
+    <mergeCell ref="B1597:F1597"/>
+    <mergeCell ref="B1598:F1598"/>
+    <mergeCell ref="B1599:F1599"/>
+    <mergeCell ref="B1600:F1600"/>
+    <mergeCell ref="B1601:F1601"/>
+    <mergeCell ref="B1602:F1602"/>
+    <mergeCell ref="B1591:F1591"/>
+    <mergeCell ref="B1592:F1592"/>
+    <mergeCell ref="B1593:F1593"/>
+    <mergeCell ref="B1594:F1594"/>
+    <mergeCell ref="B1595:F1595"/>
+    <mergeCell ref="B1596:F1596"/>
+    <mergeCell ref="B1585:F1585"/>
+    <mergeCell ref="B1586:F1586"/>
+    <mergeCell ref="B1587:F1587"/>
+    <mergeCell ref="B1588:F1588"/>
+    <mergeCell ref="B1589:F1589"/>
+    <mergeCell ref="B1590:F1590"/>
+    <mergeCell ref="B1579:F1579"/>
+    <mergeCell ref="B1580:F1580"/>
+    <mergeCell ref="B1581:F1581"/>
+    <mergeCell ref="B1582:F1582"/>
+    <mergeCell ref="B1583:F1583"/>
+    <mergeCell ref="B1584:F1584"/>
+    <mergeCell ref="B1573:F1573"/>
+    <mergeCell ref="B1574:F1574"/>
+    <mergeCell ref="B1575:F1575"/>
+    <mergeCell ref="B1576:F1576"/>
+    <mergeCell ref="B1577:F1577"/>
+    <mergeCell ref="B1578:F1578"/>
+    <mergeCell ref="B1567:F1567"/>
+    <mergeCell ref="B1568:F1568"/>
+    <mergeCell ref="B1569:F1569"/>
+    <mergeCell ref="B1570:F1570"/>
+    <mergeCell ref="B1571:F1571"/>
+    <mergeCell ref="B1572:F1572"/>
+    <mergeCell ref="B1561:F1561"/>
+    <mergeCell ref="B1562:F1562"/>
+    <mergeCell ref="B1563:F1563"/>
+    <mergeCell ref="B1564:F1564"/>
+    <mergeCell ref="B1565:F1565"/>
+    <mergeCell ref="B1566:F1566"/>
+    <mergeCell ref="B1555:F1555"/>
+    <mergeCell ref="B1556:F1556"/>
+    <mergeCell ref="B1557:F1557"/>
+    <mergeCell ref="B1558:F1558"/>
+    <mergeCell ref="B1559:F1559"/>
+    <mergeCell ref="B1560:F1560"/>
+    <mergeCell ref="B1549:F1549"/>
+    <mergeCell ref="B1550:F1550"/>
+    <mergeCell ref="B1551:F1551"/>
+    <mergeCell ref="B1552:F1552"/>
+    <mergeCell ref="B1553:F1553"/>
+    <mergeCell ref="B1554:F1554"/>
+    <mergeCell ref="B1543:F1543"/>
+    <mergeCell ref="B1544:F1544"/>
+    <mergeCell ref="B1545:F1545"/>
+    <mergeCell ref="B1546:F1546"/>
+    <mergeCell ref="B1547:F1547"/>
+    <mergeCell ref="B1548:F1548"/>
+    <mergeCell ref="B1537:F1537"/>
+    <mergeCell ref="B1538:F1538"/>
+    <mergeCell ref="B1539:F1539"/>
+    <mergeCell ref="B1540:F1540"/>
+    <mergeCell ref="B1541:F1541"/>
+    <mergeCell ref="B1542:F1542"/>
+    <mergeCell ref="B1531:F1531"/>
+    <mergeCell ref="B1532:F1532"/>
+    <mergeCell ref="B1533:F1533"/>
+    <mergeCell ref="B1534:F1534"/>
+    <mergeCell ref="B1535:F1535"/>
+    <mergeCell ref="B1536:F1536"/>
+    <mergeCell ref="B1525:F1525"/>
+    <mergeCell ref="B1526:F1526"/>
+    <mergeCell ref="B1527:F1527"/>
+    <mergeCell ref="B1528:F1528"/>
+    <mergeCell ref="B1529:F1529"/>
+    <mergeCell ref="B1530:F1530"/>
+    <mergeCell ref="B1519:F1519"/>
+    <mergeCell ref="B1520:F1520"/>
+    <mergeCell ref="B1521:F1521"/>
+    <mergeCell ref="B1522:F1522"/>
+    <mergeCell ref="B1523:F1523"/>
+    <mergeCell ref="B1524:F1524"/>
+    <mergeCell ref="B1513:F1513"/>
+    <mergeCell ref="B1514:F1514"/>
+    <mergeCell ref="B1515:F1515"/>
+    <mergeCell ref="B1516:F1516"/>
+    <mergeCell ref="B1517:F1517"/>
+    <mergeCell ref="B1518:F1518"/>
+    <mergeCell ref="B1507:F1507"/>
+    <mergeCell ref="B1508:F1508"/>
+    <mergeCell ref="B1509:F1509"/>
+    <mergeCell ref="B1510:F1510"/>
+    <mergeCell ref="B1511:F1511"/>
+    <mergeCell ref="B1512:F1512"/>
+    <mergeCell ref="B1501:F1501"/>
+    <mergeCell ref="B1502:F1502"/>
+    <mergeCell ref="B1503:F1503"/>
+    <mergeCell ref="B1504:F1504"/>
+    <mergeCell ref="B1505:F1505"/>
+    <mergeCell ref="B1506:F1506"/>
+    <mergeCell ref="B1495:F1495"/>
+    <mergeCell ref="B1496:F1496"/>
+    <mergeCell ref="B1497:F1497"/>
+    <mergeCell ref="B1498:F1498"/>
+    <mergeCell ref="B1499:F1499"/>
+    <mergeCell ref="B1500:F1500"/>
+    <mergeCell ref="B1489:F1489"/>
+    <mergeCell ref="B1490:F1490"/>
+    <mergeCell ref="B1491:F1491"/>
+    <mergeCell ref="B1492:F1492"/>
+    <mergeCell ref="B1493:F1493"/>
+    <mergeCell ref="B1494:F1494"/>
+    <mergeCell ref="B1483:F1483"/>
+    <mergeCell ref="B1484:F1484"/>
+    <mergeCell ref="B1485:F1485"/>
+    <mergeCell ref="B1486:F1486"/>
+    <mergeCell ref="B1487:F1487"/>
+    <mergeCell ref="B1488:F1488"/>
+    <mergeCell ref="B1477:F1477"/>
+    <mergeCell ref="B1478:F1478"/>
+    <mergeCell ref="B1479:F1479"/>
+    <mergeCell ref="B1480:F1480"/>
+    <mergeCell ref="B1481:F1481"/>
+    <mergeCell ref="B1482:F1482"/>
+    <mergeCell ref="B1471:F1471"/>
+    <mergeCell ref="B1472:F1472"/>
+    <mergeCell ref="B1473:F1473"/>
+    <mergeCell ref="B1474:F1474"/>
+    <mergeCell ref="B1475:F1475"/>
+    <mergeCell ref="B1476:F1476"/>
+    <mergeCell ref="B1465:F1465"/>
+    <mergeCell ref="B1466:F1466"/>
+    <mergeCell ref="B1467:F1467"/>
+    <mergeCell ref="B1468:F1468"/>
+    <mergeCell ref="B1469:F1469"/>
+    <mergeCell ref="B1470:F1470"/>
+    <mergeCell ref="B1459:F1459"/>
+    <mergeCell ref="B1460:F1460"/>
+    <mergeCell ref="B1461:F1461"/>
+    <mergeCell ref="B1462:F1462"/>
+    <mergeCell ref="B1463:F1463"/>
+    <mergeCell ref="B1464:F1464"/>
+    <mergeCell ref="B1453:F1453"/>
+    <mergeCell ref="B1454:F1454"/>
+    <mergeCell ref="B1455:F1455"/>
+    <mergeCell ref="B1456:F1456"/>
+    <mergeCell ref="B1457:F1457"/>
+    <mergeCell ref="B1458:F1458"/>
+    <mergeCell ref="B1447:F1447"/>
+    <mergeCell ref="B1448:F1448"/>
+    <mergeCell ref="B1449:F1449"/>
+    <mergeCell ref="B1450:F1450"/>
+    <mergeCell ref="B1451:F1451"/>
+    <mergeCell ref="B1452:F1452"/>
+    <mergeCell ref="B1441:F1441"/>
+    <mergeCell ref="B1442:F1442"/>
+    <mergeCell ref="B1443:F1443"/>
+    <mergeCell ref="B1444:F1444"/>
+    <mergeCell ref="B1445:F1445"/>
+    <mergeCell ref="B1446:F1446"/>
+    <mergeCell ref="B1435:F1435"/>
+    <mergeCell ref="B1436:F1436"/>
+    <mergeCell ref="B1437:F1437"/>
+    <mergeCell ref="B1438:F1438"/>
+    <mergeCell ref="B1439:F1439"/>
+    <mergeCell ref="B1440:F1440"/>
+    <mergeCell ref="B1429:F1429"/>
+    <mergeCell ref="B1430:F1430"/>
+    <mergeCell ref="B1431:F1431"/>
+    <mergeCell ref="B1432:F1432"/>
+    <mergeCell ref="B1433:F1433"/>
+    <mergeCell ref="B1434:F1434"/>
+    <mergeCell ref="B1423:F1423"/>
+    <mergeCell ref="B1424:F1424"/>
+    <mergeCell ref="B1425:F1425"/>
+    <mergeCell ref="B1426:F1426"/>
+    <mergeCell ref="B1427:F1427"/>
+    <mergeCell ref="B1428:F1428"/>
+    <mergeCell ref="B1417:F1417"/>
+    <mergeCell ref="B1418:F1418"/>
+    <mergeCell ref="B1419:F1419"/>
+    <mergeCell ref="B1420:F1420"/>
+    <mergeCell ref="B1421:F1421"/>
+    <mergeCell ref="B1422:F1422"/>
+    <mergeCell ref="B1411:F1411"/>
+    <mergeCell ref="B1412:F1412"/>
+    <mergeCell ref="B1413:F1413"/>
+    <mergeCell ref="B1414:F1414"/>
+    <mergeCell ref="B1415:F1415"/>
+    <mergeCell ref="B1416:F1416"/>
+    <mergeCell ref="B1405:F1405"/>
+    <mergeCell ref="B1406:F1406"/>
+    <mergeCell ref="B1407:F1407"/>
+    <mergeCell ref="B1408:F1408"/>
+    <mergeCell ref="B1409:F1409"/>
+    <mergeCell ref="B1410:F1410"/>
+    <mergeCell ref="B1399:F1399"/>
+    <mergeCell ref="B1400:F1400"/>
+    <mergeCell ref="B1401:F1401"/>
+    <mergeCell ref="B1402:F1402"/>
+    <mergeCell ref="B1403:F1403"/>
+    <mergeCell ref="B1404:F1404"/>
+    <mergeCell ref="B1393:F1393"/>
+    <mergeCell ref="B1394:F1394"/>
+    <mergeCell ref="B1395:F1395"/>
+    <mergeCell ref="B1396:F1396"/>
+    <mergeCell ref="B1397:F1397"/>
+    <mergeCell ref="B1398:F1398"/>
+    <mergeCell ref="B1387:F1387"/>
+    <mergeCell ref="B1388:F1388"/>
+    <mergeCell ref="B1389:F1389"/>
+    <mergeCell ref="B1390:F1390"/>
+    <mergeCell ref="B1391:F1391"/>
+    <mergeCell ref="B1392:F1392"/>
+    <mergeCell ref="B1381:F1381"/>
+    <mergeCell ref="B1382:F1382"/>
+    <mergeCell ref="B1383:F1383"/>
+    <mergeCell ref="B1384:F1384"/>
+    <mergeCell ref="B1385:F1385"/>
+    <mergeCell ref="B1386:F1386"/>
+    <mergeCell ref="B1375:F1375"/>
+    <mergeCell ref="B1376:F1376"/>
+    <mergeCell ref="B1377:F1377"/>
+    <mergeCell ref="B1378:F1378"/>
+    <mergeCell ref="B1379:F1379"/>
+    <mergeCell ref="B1380:F1380"/>
+    <mergeCell ref="B1369:F1369"/>
+    <mergeCell ref="B1370:F1370"/>
+    <mergeCell ref="B1371:F1371"/>
+    <mergeCell ref="B1372:F1372"/>
+    <mergeCell ref="B1373:F1373"/>
+    <mergeCell ref="B1374:F1374"/>
+    <mergeCell ref="B1363:F1363"/>
+    <mergeCell ref="B1364:F1364"/>
+    <mergeCell ref="B1365:F1365"/>
+    <mergeCell ref="B1366:F1366"/>
+    <mergeCell ref="B1367:F1367"/>
+    <mergeCell ref="B1368:F1368"/>
+    <mergeCell ref="B1357:F1357"/>
+    <mergeCell ref="B1358:F1358"/>
+    <mergeCell ref="B1359:F1359"/>
+    <mergeCell ref="B1360:F1360"/>
+    <mergeCell ref="B1361:F1361"/>
+    <mergeCell ref="B1362:F1362"/>
+    <mergeCell ref="B1351:F1351"/>
+    <mergeCell ref="B1352:F1352"/>
+    <mergeCell ref="B1353:F1353"/>
+    <mergeCell ref="B1354:F1354"/>
+    <mergeCell ref="B1355:F1355"/>
+    <mergeCell ref="B1356:F1356"/>
+    <mergeCell ref="B1345:F1345"/>
+    <mergeCell ref="B1346:F1346"/>
+    <mergeCell ref="B1347:F1347"/>
+    <mergeCell ref="B1348:F1348"/>
+    <mergeCell ref="B1349:F1349"/>
+    <mergeCell ref="B1350:F1350"/>
+    <mergeCell ref="B1339:F1339"/>
+    <mergeCell ref="B1340:F1340"/>
+    <mergeCell ref="B1341:F1341"/>
+    <mergeCell ref="B1342:F1342"/>
+    <mergeCell ref="B1343:F1343"/>
+    <mergeCell ref="B1344:F1344"/>
+    <mergeCell ref="B1333:F1333"/>
+    <mergeCell ref="B1334:F1334"/>
+    <mergeCell ref="B1335:F1335"/>
+    <mergeCell ref="B1336:F1336"/>
+    <mergeCell ref="B1337:F1337"/>
+    <mergeCell ref="B1338:F1338"/>
+    <mergeCell ref="B1327:F1327"/>
+    <mergeCell ref="B1328:F1328"/>
+    <mergeCell ref="B1329:F1329"/>
+    <mergeCell ref="B1330:F1330"/>
+    <mergeCell ref="B1331:F1331"/>
+    <mergeCell ref="B1332:F1332"/>
+    <mergeCell ref="B1321:F1321"/>
+    <mergeCell ref="B1322:F1322"/>
+    <mergeCell ref="B1323:F1323"/>
+    <mergeCell ref="B1324:F1324"/>
+    <mergeCell ref="B1325:F1325"/>
+    <mergeCell ref="B1326:F1326"/>
+    <mergeCell ref="B1315:F1315"/>
+    <mergeCell ref="B1316:F1316"/>
+    <mergeCell ref="B1317:F1317"/>
+    <mergeCell ref="B1318:F1318"/>
+    <mergeCell ref="B1319:F1319"/>
+    <mergeCell ref="B1320:F1320"/>
+    <mergeCell ref="B1309:F1309"/>
+    <mergeCell ref="B1310:F1310"/>
+    <mergeCell ref="B1311:F1311"/>
+    <mergeCell ref="B1312:F1312"/>
+    <mergeCell ref="B1313:F1313"/>
+    <mergeCell ref="B1314:F1314"/>
+    <mergeCell ref="B1303:F1303"/>
+    <mergeCell ref="B1304:F1304"/>
+    <mergeCell ref="B1305:F1305"/>
+    <mergeCell ref="B1306:F1306"/>
+    <mergeCell ref="B1307:F1307"/>
+    <mergeCell ref="B1308:F1308"/>
+    <mergeCell ref="B1297:F1297"/>
+    <mergeCell ref="B1298:F1298"/>
+    <mergeCell ref="B1299:F1299"/>
+    <mergeCell ref="B1300:F1300"/>
+    <mergeCell ref="B1301:F1301"/>
+    <mergeCell ref="B1302:F1302"/>
+    <mergeCell ref="B1291:F1291"/>
+    <mergeCell ref="B1292:F1292"/>
+    <mergeCell ref="B1293:F1293"/>
+    <mergeCell ref="B1294:F1294"/>
+    <mergeCell ref="B1295:F1295"/>
+    <mergeCell ref="B1296:F1296"/>
+    <mergeCell ref="B1285:F1285"/>
+    <mergeCell ref="B1286:F1286"/>
+    <mergeCell ref="B1287:F1287"/>
+    <mergeCell ref="B1288:F1288"/>
+    <mergeCell ref="B1289:F1289"/>
+    <mergeCell ref="B1290:F1290"/>
+    <mergeCell ref="B1279:F1279"/>
+    <mergeCell ref="B1280:F1280"/>
+    <mergeCell ref="B1281:F1281"/>
+    <mergeCell ref="B1282:F1282"/>
+    <mergeCell ref="B1283:F1283"/>
+    <mergeCell ref="B1284:F1284"/>
+    <mergeCell ref="B1273:F1273"/>
+    <mergeCell ref="B1274:F1274"/>
+    <mergeCell ref="B1275:F1275"/>
+    <mergeCell ref="B1276:F1276"/>
+    <mergeCell ref="B1277:F1277"/>
+    <mergeCell ref="B1278:F1278"/>
+    <mergeCell ref="B1267:F1267"/>
+    <mergeCell ref="B1268:F1268"/>
+    <mergeCell ref="B1269:F1269"/>
+    <mergeCell ref="B1270:F1270"/>
+    <mergeCell ref="B1271:F1271"/>
+    <mergeCell ref="B1272:F1272"/>
+    <mergeCell ref="B1261:F1261"/>
+    <mergeCell ref="B1262:F1262"/>
+    <mergeCell ref="B1263:F1263"/>
+    <mergeCell ref="B1264:F1264"/>
+    <mergeCell ref="B1265:F1265"/>
+    <mergeCell ref="B1266:F1266"/>
+    <mergeCell ref="B1255:F1255"/>
+    <mergeCell ref="B1256:F1256"/>
+    <mergeCell ref="B1257:F1257"/>
+    <mergeCell ref="B1258:F1258"/>
+    <mergeCell ref="B1259:F1259"/>
+    <mergeCell ref="B1260:F1260"/>
+    <mergeCell ref="B1249:F1249"/>
+    <mergeCell ref="B1250:F1250"/>
+    <mergeCell ref="B1251:F1251"/>
+    <mergeCell ref="B1252:F1252"/>
+    <mergeCell ref="B1253:F1253"/>
+    <mergeCell ref="B1254:F1254"/>
+    <mergeCell ref="B1243:F1243"/>
+    <mergeCell ref="B1244:F1244"/>
+    <mergeCell ref="B1245:F1245"/>
+    <mergeCell ref="B1246:F1246"/>
+    <mergeCell ref="B1247:F1247"/>
+    <mergeCell ref="B1248:F1248"/>
+    <mergeCell ref="B1237:F1237"/>
+    <mergeCell ref="B1238:F1238"/>
+    <mergeCell ref="B1239:F1239"/>
+    <mergeCell ref="B1240:F1240"/>
+    <mergeCell ref="B1241:F1241"/>
+    <mergeCell ref="B1242:F1242"/>
+    <mergeCell ref="B1231:F1231"/>
+    <mergeCell ref="B1232:F1232"/>
+    <mergeCell ref="B1233:F1233"/>
+    <mergeCell ref="B1234:F1234"/>
+    <mergeCell ref="B1235:F1235"/>
+    <mergeCell ref="B1236:F1236"/>
+    <mergeCell ref="B1225:F1225"/>
+    <mergeCell ref="B1226:F1226"/>
+    <mergeCell ref="B1227:F1227"/>
+    <mergeCell ref="B1228:F1228"/>
+    <mergeCell ref="B1229:F1229"/>
+    <mergeCell ref="B1230:F1230"/>
+    <mergeCell ref="B1219:F1219"/>
+    <mergeCell ref="B1220:F1220"/>
+    <mergeCell ref="B1221:F1221"/>
+    <mergeCell ref="B1222:F1222"/>
+    <mergeCell ref="B1223:F1223"/>
+    <mergeCell ref="B1224:F1224"/>
+    <mergeCell ref="B1213:F1213"/>
+    <mergeCell ref="B1214:F1214"/>
+    <mergeCell ref="B1215:F1215"/>
+    <mergeCell ref="B1216:F1216"/>
+    <mergeCell ref="B1217:F1217"/>
+    <mergeCell ref="B1218:F1218"/>
+    <mergeCell ref="B1207:F1207"/>
+    <mergeCell ref="B1208:F1208"/>
+    <mergeCell ref="B1209:F1209"/>
+    <mergeCell ref="B1210:F1210"/>
+    <mergeCell ref="B1211:F1211"/>
+    <mergeCell ref="B1212:F1212"/>
+    <mergeCell ref="B1201:F1201"/>
+    <mergeCell ref="B1202:F1202"/>
+    <mergeCell ref="B1203:F1203"/>
+    <mergeCell ref="B1204:F1204"/>
+    <mergeCell ref="B1205:F1205"/>
+    <mergeCell ref="B1206:F1206"/>
+    <mergeCell ref="B1195:F1195"/>
+    <mergeCell ref="B1196:F1196"/>
+    <mergeCell ref="B1197:F1197"/>
+    <mergeCell ref="B1198:F1198"/>
+    <mergeCell ref="B1199:F1199"/>
+    <mergeCell ref="B1200:F1200"/>
+    <mergeCell ref="B1189:F1189"/>
+    <mergeCell ref="B1190:F1190"/>
+    <mergeCell ref="B1191:F1191"/>
+    <mergeCell ref="B1192:F1192"/>
+    <mergeCell ref="B1193:F1193"/>
+    <mergeCell ref="B1194:F1194"/>
+    <mergeCell ref="B1183:F1183"/>
+    <mergeCell ref="B1184:F1184"/>
+    <mergeCell ref="B1185:F1185"/>
+    <mergeCell ref="B1186:F1186"/>
+    <mergeCell ref="B1187:F1187"/>
+    <mergeCell ref="B1188:F1188"/>
+    <mergeCell ref="B1177:F1177"/>
+    <mergeCell ref="B1178:F1178"/>
+    <mergeCell ref="B1179:F1179"/>
+    <mergeCell ref="B1180:F1180"/>
+    <mergeCell ref="B1181:F1181"/>
+    <mergeCell ref="B1182:F1182"/>
+    <mergeCell ref="B1171:F1171"/>
+    <mergeCell ref="B1172:F1172"/>
+    <mergeCell ref="B1173:F1173"/>
+    <mergeCell ref="B1174:F1174"/>
+    <mergeCell ref="B1175:F1175"/>
+    <mergeCell ref="B1176:F1176"/>
+    <mergeCell ref="B1165:F1165"/>
+    <mergeCell ref="B1166:F1166"/>
+    <mergeCell ref="B1167:F1167"/>
+    <mergeCell ref="B1168:F1168"/>
+    <mergeCell ref="B1169:F1169"/>
+    <mergeCell ref="B1170:F1170"/>
+    <mergeCell ref="B1159:F1159"/>
+    <mergeCell ref="B1160:F1160"/>
+    <mergeCell ref="B1161:F1161"/>
+    <mergeCell ref="B1162:F1162"/>
+    <mergeCell ref="B1163:F1163"/>
+    <mergeCell ref="B1164:F1164"/>
+    <mergeCell ref="B1153:F1153"/>
+    <mergeCell ref="B1154:F1154"/>
+    <mergeCell ref="B1155:F1155"/>
+    <mergeCell ref="B1156:F1156"/>
+    <mergeCell ref="B1157:F1157"/>
+    <mergeCell ref="B1158:F1158"/>
+    <mergeCell ref="B1147:F1147"/>
+    <mergeCell ref="B1148:F1148"/>
+    <mergeCell ref="B1149:F1149"/>
+    <mergeCell ref="B1150:F1150"/>
+    <mergeCell ref="B1151:F1151"/>
+    <mergeCell ref="B1152:F1152"/>
+    <mergeCell ref="B1141:F1141"/>
+    <mergeCell ref="B1142:F1142"/>
+    <mergeCell ref="B1143:F1143"/>
+    <mergeCell ref="B1144:F1144"/>
+    <mergeCell ref="B1145:F1145"/>
+    <mergeCell ref="B1146:F1146"/>
+    <mergeCell ref="B1135:F1135"/>
+    <mergeCell ref="B1136:F1136"/>
+    <mergeCell ref="B1137:F1137"/>
+    <mergeCell ref="B1138:F1138"/>
+    <mergeCell ref="B1139:F1139"/>
+    <mergeCell ref="B1140:F1140"/>
+    <mergeCell ref="B1129:F1129"/>
+    <mergeCell ref="B1130:F1130"/>
+    <mergeCell ref="B1131:F1131"/>
+    <mergeCell ref="B1132:F1132"/>
+    <mergeCell ref="B1133:F1133"/>
+    <mergeCell ref="B1134:F1134"/>
+    <mergeCell ref="B1123:F1123"/>
+    <mergeCell ref="B1124:F1124"/>
+    <mergeCell ref="B1125:F1125"/>
+    <mergeCell ref="B1126:F1126"/>
+    <mergeCell ref="B1127:F1127"/>
+    <mergeCell ref="B1128:F1128"/>
+    <mergeCell ref="B1117:F1117"/>
+    <mergeCell ref="B1118:F1118"/>
+    <mergeCell ref="B1119:F1119"/>
+    <mergeCell ref="B1120:F1120"/>
+    <mergeCell ref="B1121:F1121"/>
+    <mergeCell ref="B1122:F1122"/>
+    <mergeCell ref="B1111:F1111"/>
+    <mergeCell ref="B1112:F1112"/>
+    <mergeCell ref="B1113:F1113"/>
+    <mergeCell ref="B1114:F1114"/>
+    <mergeCell ref="B1115:F1115"/>
+    <mergeCell ref="B1116:F1116"/>
+    <mergeCell ref="B1105:F1105"/>
+    <mergeCell ref="B1106:F1106"/>
+    <mergeCell ref="B1107:F1107"/>
+    <mergeCell ref="B1108:F1108"/>
+    <mergeCell ref="B1109:F1109"/>
+    <mergeCell ref="B1110:F1110"/>
+    <mergeCell ref="B1099:F1099"/>
+    <mergeCell ref="B1100:F1100"/>
+    <mergeCell ref="B1101:F1101"/>
+    <mergeCell ref="B1102:F1102"/>
+    <mergeCell ref="B1103:F1103"/>
+    <mergeCell ref="B1104:F1104"/>
+    <mergeCell ref="B1093:F1093"/>
+    <mergeCell ref="B1094:F1094"/>
+    <mergeCell ref="B1095:F1095"/>
+    <mergeCell ref="B1096:F1096"/>
+    <mergeCell ref="B1097:F1097"/>
+    <mergeCell ref="B1098:F1098"/>
+    <mergeCell ref="B1087:F1087"/>
+    <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1089:F1089"/>
+    <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1091:F1091"/>
+    <mergeCell ref="B1092:F1092"/>
+    <mergeCell ref="B1081:F1081"/>
+    <mergeCell ref="B1082:F1082"/>
+    <mergeCell ref="B1083:F1083"/>
+    <mergeCell ref="B1084:F1084"/>
+    <mergeCell ref="B1085:F1085"/>
+    <mergeCell ref="B1086:F1086"/>
+    <mergeCell ref="B1075:F1075"/>
+    <mergeCell ref="B1076:F1076"/>
+    <mergeCell ref="B1077:F1077"/>
+    <mergeCell ref="B1078:F1078"/>
+    <mergeCell ref="B1079:F1079"/>
+    <mergeCell ref="B1080:F1080"/>
+    <mergeCell ref="B1069:F1069"/>
+    <mergeCell ref="B1070:F1070"/>
+    <mergeCell ref="B1071:F1071"/>
+    <mergeCell ref="B1072:F1072"/>
+    <mergeCell ref="B1073:F1073"/>
+    <mergeCell ref="B1074:F1074"/>
+    <mergeCell ref="B1063:F1063"/>
+    <mergeCell ref="B1064:F1064"/>
+    <mergeCell ref="B1065:F1065"/>
+    <mergeCell ref="B1066:F1066"/>
+    <mergeCell ref="B1067:F1067"/>
+    <mergeCell ref="B1068:F1068"/>
+    <mergeCell ref="B1057:F1057"/>
+    <mergeCell ref="B1058:F1058"/>
+    <mergeCell ref="B1059:F1059"/>
+    <mergeCell ref="B1060:F1060"/>
+    <mergeCell ref="B1061:F1061"/>
+    <mergeCell ref="B1062:F1062"/>
+    <mergeCell ref="B1051:F1051"/>
+    <mergeCell ref="B1052:F1052"/>
+    <mergeCell ref="B1053:F1053"/>
+    <mergeCell ref="B1054:F1054"/>
+    <mergeCell ref="B1055:F1055"/>
+    <mergeCell ref="B1056:F1056"/>
+    <mergeCell ref="B1045:F1045"/>
+    <mergeCell ref="B1046:F1046"/>
+    <mergeCell ref="B1047:F1047"/>
+    <mergeCell ref="B1048:F1048"/>
+    <mergeCell ref="B1049:F1049"/>
+    <mergeCell ref="B1050:F1050"/>
+    <mergeCell ref="B1039:F1039"/>
+    <mergeCell ref="B1040:F1040"/>
+    <mergeCell ref="B1041:F1041"/>
+    <mergeCell ref="B1042:F1042"/>
+    <mergeCell ref="B1043:F1043"/>
+    <mergeCell ref="B1044:F1044"/>
+    <mergeCell ref="B1033:F1033"/>
+    <mergeCell ref="B1034:F1034"/>
+    <mergeCell ref="B1035:F1035"/>
+    <mergeCell ref="B1036:F1036"/>
+    <mergeCell ref="B1037:F1037"/>
+    <mergeCell ref="B1038:F1038"/>
+    <mergeCell ref="B1027:F1027"/>
+    <mergeCell ref="B1028:F1028"/>
+    <mergeCell ref="B1029:F1029"/>
+    <mergeCell ref="B1030:F1030"/>
+    <mergeCell ref="B1031:F1031"/>
+    <mergeCell ref="B1032:F1032"/>
+    <mergeCell ref="B1021:F1021"/>
+    <mergeCell ref="B1022:F1022"/>
+    <mergeCell ref="B1023:F1023"/>
+    <mergeCell ref="B1024:F1024"/>
+    <mergeCell ref="B1025:F1025"/>
+    <mergeCell ref="B1026:F1026"/>
+    <mergeCell ref="B1015:F1015"/>
+    <mergeCell ref="B1016:F1016"/>
+    <mergeCell ref="B1017:F1017"/>
+    <mergeCell ref="B1018:F1018"/>
+    <mergeCell ref="B1019:F1019"/>
+    <mergeCell ref="B1020:F1020"/>
+    <mergeCell ref="B1009:F1009"/>
+    <mergeCell ref="B1010:F1010"/>
+    <mergeCell ref="B1011:F1011"/>
+    <mergeCell ref="B1012:F1012"/>
+    <mergeCell ref="B1013:F1013"/>
+    <mergeCell ref="B1014:F1014"/>
+    <mergeCell ref="B1003:F1003"/>
+    <mergeCell ref="B1004:F1004"/>
+    <mergeCell ref="B1005:F1005"/>
+    <mergeCell ref="B1006:F1006"/>
+    <mergeCell ref="B1007:F1007"/>
+    <mergeCell ref="B1008:F1008"/>
+    <mergeCell ref="B997:F997"/>
+    <mergeCell ref="B998:F998"/>
+    <mergeCell ref="B999:F999"/>
+    <mergeCell ref="B1000:F1000"/>
+    <mergeCell ref="B1001:F1001"/>
+    <mergeCell ref="B1002:F1002"/>
+    <mergeCell ref="B991:F991"/>
+    <mergeCell ref="B992:F992"/>
+    <mergeCell ref="B993:F993"/>
+    <mergeCell ref="B994:F994"/>
+    <mergeCell ref="B995:F995"/>
+    <mergeCell ref="B996:F996"/>
+    <mergeCell ref="B985:F985"/>
+    <mergeCell ref="B986:F986"/>
+    <mergeCell ref="B987:F987"/>
+    <mergeCell ref="B988:F988"/>
+    <mergeCell ref="B989:F989"/>
+    <mergeCell ref="B990:F990"/>
+    <mergeCell ref="B979:F979"/>
+    <mergeCell ref="B980:F980"/>
+    <mergeCell ref="B981:F981"/>
+    <mergeCell ref="B982:F982"/>
+    <mergeCell ref="B983:F983"/>
+    <mergeCell ref="B984:F984"/>
+    <mergeCell ref="B973:F973"/>
+    <mergeCell ref="B974:F974"/>
+    <mergeCell ref="B975:F975"/>
+    <mergeCell ref="B976:F976"/>
+    <mergeCell ref="B977:F977"/>
+    <mergeCell ref="B978:F978"/>
+    <mergeCell ref="B967:F967"/>
+    <mergeCell ref="B968:F968"/>
+    <mergeCell ref="B969:F969"/>
+    <mergeCell ref="B970:F970"/>
+    <mergeCell ref="B971:F971"/>
+    <mergeCell ref="B972:F972"/>
+    <mergeCell ref="B961:F961"/>
+    <mergeCell ref="B962:F962"/>
+    <mergeCell ref="B963:F963"/>
+    <mergeCell ref="B964:F964"/>
+    <mergeCell ref="B965:F965"/>
+    <mergeCell ref="B966:F966"/>
+    <mergeCell ref="B955:F955"/>
+    <mergeCell ref="B956:F956"/>
+    <mergeCell ref="B957:F957"/>
+    <mergeCell ref="B958:F958"/>
+    <mergeCell ref="B959:F959"/>
+    <mergeCell ref="B960:F960"/>
+    <mergeCell ref="B949:F949"/>
+    <mergeCell ref="B950:F950"/>
+    <mergeCell ref="B951:F951"/>
+    <mergeCell ref="B952:F952"/>
+    <mergeCell ref="B953:F953"/>
+    <mergeCell ref="B954:F954"/>
+    <mergeCell ref="B943:F943"/>
+    <mergeCell ref="B944:F944"/>
+    <mergeCell ref="B945:F945"/>
+    <mergeCell ref="B946:F946"/>
+    <mergeCell ref="B947:F947"/>
+    <mergeCell ref="B948:F948"/>
+    <mergeCell ref="B937:F937"/>
+    <mergeCell ref="B938:F938"/>
+    <mergeCell ref="B939:F939"/>
+    <mergeCell ref="B940:F940"/>
+    <mergeCell ref="B941:F941"/>
+    <mergeCell ref="B942:F942"/>
+    <mergeCell ref="B931:F931"/>
+    <mergeCell ref="B932:F932"/>
+    <mergeCell ref="B933:F933"/>
+    <mergeCell ref="B934:F934"/>
+    <mergeCell ref="B935:F935"/>
+    <mergeCell ref="B936:F936"/>
+    <mergeCell ref="B925:F925"/>
+    <mergeCell ref="B926:F926"/>
+    <mergeCell ref="B927:F927"/>
+    <mergeCell ref="B928:F928"/>
+    <mergeCell ref="B929:F929"/>
+    <mergeCell ref="B930:F930"/>
+    <mergeCell ref="B919:F919"/>
+    <mergeCell ref="B920:F920"/>
+    <mergeCell ref="B921:F921"/>
+    <mergeCell ref="B922:F922"/>
+    <mergeCell ref="B923:F923"/>
+    <mergeCell ref="B924:F924"/>
+    <mergeCell ref="B913:F913"/>
+    <mergeCell ref="B914:F914"/>
+    <mergeCell ref="B915:F915"/>
+    <mergeCell ref="B916:F916"/>
+    <mergeCell ref="B917:F917"/>
+    <mergeCell ref="B918:F918"/>
+    <mergeCell ref="B907:F907"/>
+    <mergeCell ref="B908:F908"/>
+    <mergeCell ref="B909:F909"/>
+    <mergeCell ref="B910:F910"/>
+    <mergeCell ref="B911:F911"/>
+    <mergeCell ref="B912:F912"/>
+    <mergeCell ref="B901:F901"/>
+    <mergeCell ref="B902:F902"/>
+    <mergeCell ref="B903:F903"/>
+    <mergeCell ref="B904:F904"/>
+    <mergeCell ref="B905:F905"/>
+    <mergeCell ref="B906:F906"/>
+    <mergeCell ref="B895:F895"/>
+    <mergeCell ref="B896:F896"/>
+    <mergeCell ref="B897:F897"/>
+    <mergeCell ref="B898:F898"/>
+    <mergeCell ref="B899:F899"/>
+    <mergeCell ref="B900:F900"/>
+    <mergeCell ref="B889:F889"/>
+    <mergeCell ref="B890:F890"/>
+    <mergeCell ref="B891:F891"/>
+    <mergeCell ref="B892:F892"/>
+    <mergeCell ref="B893:F893"/>
+    <mergeCell ref="B894:F894"/>
+    <mergeCell ref="B883:F883"/>
+    <mergeCell ref="B884:F884"/>
+    <mergeCell ref="B885:F885"/>
+    <mergeCell ref="B886:F886"/>
+    <mergeCell ref="B887:F887"/>
+    <mergeCell ref="B888:F888"/>
+    <mergeCell ref="B877:F877"/>
+    <mergeCell ref="B878:F878"/>
+    <mergeCell ref="B879:F879"/>
+    <mergeCell ref="B880:F880"/>
+    <mergeCell ref="B881:F881"/>
+    <mergeCell ref="B882:F882"/>
+    <mergeCell ref="B871:F871"/>
+    <mergeCell ref="B872:F872"/>
+    <mergeCell ref="B873:F873"/>
+    <mergeCell ref="B874:F874"/>
+    <mergeCell ref="B875:F875"/>
+    <mergeCell ref="B876:F876"/>
+    <mergeCell ref="B865:F865"/>
+    <mergeCell ref="B866:F866"/>
+    <mergeCell ref="B867:F867"/>
+    <mergeCell ref="B868:F868"/>
+    <mergeCell ref="B869:F869"/>
+    <mergeCell ref="B870:F870"/>
+    <mergeCell ref="B859:F859"/>
+    <mergeCell ref="B860:F860"/>
+    <mergeCell ref="B861:F861"/>
+    <mergeCell ref="B862:F862"/>
+    <mergeCell ref="B863:F863"/>
+    <mergeCell ref="B864:F864"/>
+    <mergeCell ref="B853:F853"/>
+    <mergeCell ref="B854:F854"/>
+    <mergeCell ref="B855:F855"/>
+    <mergeCell ref="B856:F856"/>
+    <mergeCell ref="B857:F857"/>
+    <mergeCell ref="B858:F858"/>
+    <mergeCell ref="B847:F847"/>
+    <mergeCell ref="B848:F848"/>
+    <mergeCell ref="B849:F849"/>
+    <mergeCell ref="B850:F850"/>
+    <mergeCell ref="B851:F851"/>
+    <mergeCell ref="B852:F852"/>
+    <mergeCell ref="B841:F841"/>
+    <mergeCell ref="B842:F842"/>
+    <mergeCell ref="B843:F843"/>
+    <mergeCell ref="B844:F844"/>
+    <mergeCell ref="B845:F845"/>
+    <mergeCell ref="B846:F846"/>
+    <mergeCell ref="B835:F835"/>
+    <mergeCell ref="B836:F836"/>
+    <mergeCell ref="B837:F837"/>
+    <mergeCell ref="B838:F838"/>
+    <mergeCell ref="B839:F839"/>
+    <mergeCell ref="B840:F840"/>
+    <mergeCell ref="B829:F829"/>
+    <mergeCell ref="B830:F830"/>
+    <mergeCell ref="B831:F831"/>
+    <mergeCell ref="B832:F832"/>
+    <mergeCell ref="B833:F833"/>
+    <mergeCell ref="B834:F834"/>
+    <mergeCell ref="B823:F823"/>
+    <mergeCell ref="B824:F824"/>
+    <mergeCell ref="B825:F825"/>
+    <mergeCell ref="B826:F826"/>
+    <mergeCell ref="B827:F827"/>
+    <mergeCell ref="B828:F828"/>
+    <mergeCell ref="B817:F817"/>
+    <mergeCell ref="B818:F818"/>
+    <mergeCell ref="B819:F819"/>
+    <mergeCell ref="B820:F820"/>
+    <mergeCell ref="B821:F821"/>
+    <mergeCell ref="B822:F822"/>
+    <mergeCell ref="B811:F811"/>
+    <mergeCell ref="B812:F812"/>
+    <mergeCell ref="B813:F813"/>
+    <mergeCell ref="B814:F814"/>
+    <mergeCell ref="B815:F815"/>
+    <mergeCell ref="B816:F816"/>
+    <mergeCell ref="B805:F805"/>
+    <mergeCell ref="B806:F806"/>
+    <mergeCell ref="B807:F807"/>
+    <mergeCell ref="B808:F808"/>
+    <mergeCell ref="B809:F809"/>
+    <mergeCell ref="B810:F810"/>
+    <mergeCell ref="B799:F799"/>
+    <mergeCell ref="B800:F800"/>
+    <mergeCell ref="B801:F801"/>
+    <mergeCell ref="B802:F802"/>
+    <mergeCell ref="B803:F803"/>
+    <mergeCell ref="B804:F804"/>
+    <mergeCell ref="B793:F793"/>
+    <mergeCell ref="B794:F794"/>
+    <mergeCell ref="B795:F795"/>
+    <mergeCell ref="B796:F796"/>
+    <mergeCell ref="B797:F797"/>
+    <mergeCell ref="B798:F798"/>
+    <mergeCell ref="B787:F787"/>
+    <mergeCell ref="B788:F788"/>
+    <mergeCell ref="B789:F789"/>
+    <mergeCell ref="B790:F790"/>
+    <mergeCell ref="B791:F791"/>
+    <mergeCell ref="B792:F792"/>
+    <mergeCell ref="B781:F781"/>
+    <mergeCell ref="B782:F782"/>
+    <mergeCell ref="B783:F783"/>
+    <mergeCell ref="B784:F784"/>
+    <mergeCell ref="B785:F785"/>
+    <mergeCell ref="B786:F786"/>
+    <mergeCell ref="B775:F775"/>
+    <mergeCell ref="B776:F776"/>
+    <mergeCell ref="B777:F777"/>
+    <mergeCell ref="B778:F778"/>
+    <mergeCell ref="B779:F779"/>
+    <mergeCell ref="B780:F780"/>
+    <mergeCell ref="B769:F769"/>
+    <mergeCell ref="B770:F770"/>
+    <mergeCell ref="B771:F771"/>
+    <mergeCell ref="B772:F772"/>
+    <mergeCell ref="B773:F773"/>
+    <mergeCell ref="B774:F774"/>
+    <mergeCell ref="B763:F763"/>
+    <mergeCell ref="B764:F764"/>
+    <mergeCell ref="B765:F765"/>
+    <mergeCell ref="B766:F766"/>
+    <mergeCell ref="B767:F767"/>
+    <mergeCell ref="B768:F768"/>
+    <mergeCell ref="B757:F757"/>
+    <mergeCell ref="B758:F758"/>
+    <mergeCell ref="B759:F759"/>
+    <mergeCell ref="B760:F760"/>
+    <mergeCell ref="B761:F761"/>
+    <mergeCell ref="B762:F762"/>
+    <mergeCell ref="B751:F751"/>
+    <mergeCell ref="B752:F752"/>
+    <mergeCell ref="B753:F753"/>
+    <mergeCell ref="B754:F754"/>
+    <mergeCell ref="B755:F755"/>
+    <mergeCell ref="B756:F756"/>
+    <mergeCell ref="B745:F745"/>
+    <mergeCell ref="B746:F746"/>
+    <mergeCell ref="B747:F747"/>
+    <mergeCell ref="B748:F748"/>
+    <mergeCell ref="B749:F749"/>
+    <mergeCell ref="B750:F750"/>
+    <mergeCell ref="B739:F739"/>
+    <mergeCell ref="B740:F740"/>
+    <mergeCell ref="B741:F741"/>
+    <mergeCell ref="B742:F742"/>
+    <mergeCell ref="B743:F743"/>
+    <mergeCell ref="B744:F744"/>
+    <mergeCell ref="B733:F733"/>
+    <mergeCell ref="B734:F734"/>
+    <mergeCell ref="B735:F735"/>
+    <mergeCell ref="B736:F736"/>
+    <mergeCell ref="B737:F737"/>
+    <mergeCell ref="B738:F738"/>
+    <mergeCell ref="B727:F727"/>
+    <mergeCell ref="B728:F728"/>
+    <mergeCell ref="B729:F729"/>
+    <mergeCell ref="B730:F730"/>
+    <mergeCell ref="B731:F731"/>
+    <mergeCell ref="B732:F732"/>
+    <mergeCell ref="B721:F721"/>
+    <mergeCell ref="B722:F722"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="B724:F724"/>
+    <mergeCell ref="B725:F725"/>
+    <mergeCell ref="B726:F726"/>
+    <mergeCell ref="B715:F715"/>
+    <mergeCell ref="B716:F716"/>
+    <mergeCell ref="B717:F717"/>
+    <mergeCell ref="B718:F718"/>
+    <mergeCell ref="B719:F719"/>
+    <mergeCell ref="B720:F720"/>
+    <mergeCell ref="B709:F709"/>
+    <mergeCell ref="B710:F710"/>
+    <mergeCell ref="B711:F711"/>
+    <mergeCell ref="B712:F712"/>
+    <mergeCell ref="B713:F713"/>
+    <mergeCell ref="B714:F714"/>
+    <mergeCell ref="B703:F703"/>
+    <mergeCell ref="B704:F704"/>
+    <mergeCell ref="B705:F705"/>
+    <mergeCell ref="B706:F706"/>
+    <mergeCell ref="B707:F707"/>
+    <mergeCell ref="B708:F708"/>
+    <mergeCell ref="B697:F697"/>
+    <mergeCell ref="B698:F698"/>
+    <mergeCell ref="B699:F699"/>
+    <mergeCell ref="B700:F700"/>
+    <mergeCell ref="B701:F701"/>
+    <mergeCell ref="B702:F702"/>
+    <mergeCell ref="B691:F691"/>
+    <mergeCell ref="B692:F692"/>
+    <mergeCell ref="B693:F693"/>
+    <mergeCell ref="B694:F694"/>
+    <mergeCell ref="B695:F695"/>
+    <mergeCell ref="B696:F696"/>
+    <mergeCell ref="B685:F685"/>
+    <mergeCell ref="B686:F686"/>
+    <mergeCell ref="B687:F687"/>
+    <mergeCell ref="B688:F688"/>
+    <mergeCell ref="B689:F689"/>
+    <mergeCell ref="B690:F690"/>
+    <mergeCell ref="B679:F679"/>
+    <mergeCell ref="B680:F680"/>
+    <mergeCell ref="B681:F681"/>
+    <mergeCell ref="B682:F682"/>
+    <mergeCell ref="B683:F683"/>
+    <mergeCell ref="B684:F684"/>
+    <mergeCell ref="B673:F673"/>
+    <mergeCell ref="B674:F674"/>
+    <mergeCell ref="B675:F675"/>
+    <mergeCell ref="B676:F676"/>
+    <mergeCell ref="B677:F677"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="B667:F667"/>
+    <mergeCell ref="B668:F668"/>
+    <mergeCell ref="B669:F669"/>
+    <mergeCell ref="B670:F670"/>
+    <mergeCell ref="B671:F671"/>
+    <mergeCell ref="B672:F672"/>
+    <mergeCell ref="B661:F661"/>
+    <mergeCell ref="B662:F662"/>
+    <mergeCell ref="B663:F663"/>
+    <mergeCell ref="B664:F664"/>
+    <mergeCell ref="B665:F665"/>
+    <mergeCell ref="B666:F666"/>
+    <mergeCell ref="B655:F655"/>
+    <mergeCell ref="B656:F656"/>
+    <mergeCell ref="B657:F657"/>
+    <mergeCell ref="B658:F658"/>
+    <mergeCell ref="B659:F659"/>
+    <mergeCell ref="B660:F660"/>
+    <mergeCell ref="B649:F649"/>
+    <mergeCell ref="B650:F650"/>
+    <mergeCell ref="B651:F651"/>
+    <mergeCell ref="B652:F652"/>
+    <mergeCell ref="B653:F653"/>
+    <mergeCell ref="B654:F654"/>
+    <mergeCell ref="B643:F643"/>
+    <mergeCell ref="B644:F644"/>
+    <mergeCell ref="B645:F645"/>
+    <mergeCell ref="B646:F646"/>
+    <mergeCell ref="B647:F647"/>
+    <mergeCell ref="B648:F648"/>
+    <mergeCell ref="B637:F637"/>
+    <mergeCell ref="B638:F638"/>
+    <mergeCell ref="B639:F639"/>
+    <mergeCell ref="B640:F640"/>
+    <mergeCell ref="B641:F641"/>
+    <mergeCell ref="B642:F642"/>
+    <mergeCell ref="B631:F631"/>
+    <mergeCell ref="B632:F632"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="B634:F634"/>
+    <mergeCell ref="B635:F635"/>
+    <mergeCell ref="B636:F636"/>
+    <mergeCell ref="B625:F625"/>
+    <mergeCell ref="B626:F626"/>
+    <mergeCell ref="B627:F627"/>
+    <mergeCell ref="B628:F628"/>
+    <mergeCell ref="B629:F629"/>
+    <mergeCell ref="B630:F630"/>
+    <mergeCell ref="B619:F619"/>
+    <mergeCell ref="B620:F620"/>
+    <mergeCell ref="B621:F621"/>
+    <mergeCell ref="B622:F622"/>
+    <mergeCell ref="B623:F623"/>
+    <mergeCell ref="B624:F624"/>
+    <mergeCell ref="B613:F613"/>
+    <mergeCell ref="B614:F614"/>
+    <mergeCell ref="B615:F615"/>
+    <mergeCell ref="B616:F616"/>
+    <mergeCell ref="B617:F617"/>
+    <mergeCell ref="B618:F618"/>
+    <mergeCell ref="B607:F607"/>
+    <mergeCell ref="B608:F608"/>
+    <mergeCell ref="B609:F609"/>
+    <mergeCell ref="B610:F610"/>
+    <mergeCell ref="B611:F611"/>
+    <mergeCell ref="B612:F612"/>
+    <mergeCell ref="B601:F601"/>
+    <mergeCell ref="B602:F602"/>
+    <mergeCell ref="B603:F603"/>
+    <mergeCell ref="B604:F604"/>
+    <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B606:F606"/>
+    <mergeCell ref="B595:F595"/>
+    <mergeCell ref="B596:F596"/>
+    <mergeCell ref="B597:F597"/>
+    <mergeCell ref="B598:F598"/>
+    <mergeCell ref="B599:F599"/>
+    <mergeCell ref="B600:F600"/>
+    <mergeCell ref="B589:F589"/>
+    <mergeCell ref="B590:F590"/>
+    <mergeCell ref="B591:F591"/>
+    <mergeCell ref="B592:F592"/>
+    <mergeCell ref="B593:F593"/>
+    <mergeCell ref="B594:F594"/>
+    <mergeCell ref="B583:F583"/>
+    <mergeCell ref="B584:F584"/>
+    <mergeCell ref="B585:F585"/>
+    <mergeCell ref="B586:F586"/>
+    <mergeCell ref="B587:F587"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="B577:F577"/>
+    <mergeCell ref="B578:F578"/>
+    <mergeCell ref="B579:F579"/>
+    <mergeCell ref="B580:F580"/>
+    <mergeCell ref="B581:F581"/>
+    <mergeCell ref="B582:F582"/>
+    <mergeCell ref="B571:F571"/>
+    <mergeCell ref="B572:F572"/>
+    <mergeCell ref="B573:F573"/>
+    <mergeCell ref="B574:F574"/>
+    <mergeCell ref="B575:F575"/>
+    <mergeCell ref="B576:F576"/>
+    <mergeCell ref="B565:F565"/>
+    <mergeCell ref="B566:F566"/>
+    <mergeCell ref="B567:F567"/>
+    <mergeCell ref="B568:F568"/>
+    <mergeCell ref="B569:F569"/>
+    <mergeCell ref="B570:F570"/>
+    <mergeCell ref="B559:F559"/>
+    <mergeCell ref="B560:F560"/>
+    <mergeCell ref="B561:F561"/>
+    <mergeCell ref="B562:F562"/>
+    <mergeCell ref="B563:F563"/>
+    <mergeCell ref="B564:F564"/>
+    <mergeCell ref="B553:F553"/>
+    <mergeCell ref="B554:F554"/>
+    <mergeCell ref="B555:F555"/>
+    <mergeCell ref="B556:F556"/>
+    <mergeCell ref="B557:F557"/>
+    <mergeCell ref="B558:F558"/>
+    <mergeCell ref="B547:F547"/>
+    <mergeCell ref="B548:F548"/>
+    <mergeCell ref="B549:F549"/>
+    <mergeCell ref="B550:F550"/>
+    <mergeCell ref="B551:F551"/>
+    <mergeCell ref="B552:F552"/>
+    <mergeCell ref="B541:F541"/>
+    <mergeCell ref="B542:F542"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="B544:F544"/>
+    <mergeCell ref="B545:F545"/>
+    <mergeCell ref="B546:F546"/>
+    <mergeCell ref="B535:F535"/>
+    <mergeCell ref="B536:F536"/>
+    <mergeCell ref="B537:F537"/>
+    <mergeCell ref="B538:F538"/>
+    <mergeCell ref="B539:F539"/>
+    <mergeCell ref="B540:F540"/>
+    <mergeCell ref="B529:F529"/>
+    <mergeCell ref="B530:F530"/>
+    <mergeCell ref="B531:F531"/>
+    <mergeCell ref="B532:F532"/>
+    <mergeCell ref="B533:F533"/>
+    <mergeCell ref="B534:F534"/>
+    <mergeCell ref="B523:F523"/>
+    <mergeCell ref="B524:F524"/>
+    <mergeCell ref="B525:F525"/>
+    <mergeCell ref="B526:F526"/>
+    <mergeCell ref="B527:F527"/>
+    <mergeCell ref="B528:F528"/>
+    <mergeCell ref="B517:F517"/>
+    <mergeCell ref="B518:F518"/>
+    <mergeCell ref="B519:F519"/>
+    <mergeCell ref="B520:F520"/>
+    <mergeCell ref="B521:F521"/>
+    <mergeCell ref="B522:F522"/>
+    <mergeCell ref="B511:F511"/>
+    <mergeCell ref="B512:F512"/>
+    <mergeCell ref="B513:F513"/>
+    <mergeCell ref="B514:F514"/>
+    <mergeCell ref="B515:F515"/>
+    <mergeCell ref="B516:F516"/>
+    <mergeCell ref="B505:F505"/>
+    <mergeCell ref="B506:F506"/>
+    <mergeCell ref="B507:F507"/>
+    <mergeCell ref="B508:F508"/>
+    <mergeCell ref="B509:F509"/>
+    <mergeCell ref="B510:F510"/>
+    <mergeCell ref="B499:F499"/>
+    <mergeCell ref="B500:F500"/>
+    <mergeCell ref="B501:F501"/>
+    <mergeCell ref="B502:F502"/>
+    <mergeCell ref="B503:F503"/>
+    <mergeCell ref="B504:F504"/>
+    <mergeCell ref="B493:F493"/>
+    <mergeCell ref="B494:F494"/>
+    <mergeCell ref="B495:F495"/>
+    <mergeCell ref="B496:F496"/>
+    <mergeCell ref="B497:F497"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="B487:F487"/>
+    <mergeCell ref="B488:F488"/>
+    <mergeCell ref="B489:F489"/>
+    <mergeCell ref="B490:F490"/>
+    <mergeCell ref="B491:F491"/>
+    <mergeCell ref="B492:F492"/>
+    <mergeCell ref="B481:F481"/>
+    <mergeCell ref="B482:F482"/>
+    <mergeCell ref="B483:F483"/>
+    <mergeCell ref="B484:F484"/>
+    <mergeCell ref="B485:F485"/>
+    <mergeCell ref="B486:F486"/>
+    <mergeCell ref="B475:F475"/>
+    <mergeCell ref="B476:F476"/>
+    <mergeCell ref="B477:F477"/>
+    <mergeCell ref="B478:F478"/>
+    <mergeCell ref="B479:F479"/>
+    <mergeCell ref="B480:F480"/>
+    <mergeCell ref="B469:F469"/>
+    <mergeCell ref="B470:F470"/>
+    <mergeCell ref="B471:F471"/>
+    <mergeCell ref="B472:F472"/>
+    <mergeCell ref="B473:F473"/>
+    <mergeCell ref="B474:F474"/>
+    <mergeCell ref="B463:F463"/>
+    <mergeCell ref="B464:F464"/>
+    <mergeCell ref="B465:F465"/>
+    <mergeCell ref="B466:F466"/>
+    <mergeCell ref="B467:F467"/>
+    <mergeCell ref="B468:F468"/>
+    <mergeCell ref="B457:F457"/>
+    <mergeCell ref="B458:F458"/>
+    <mergeCell ref="B459:F459"/>
+    <mergeCell ref="B460:F460"/>
+    <mergeCell ref="B461:F461"/>
+    <mergeCell ref="B462:F462"/>
+    <mergeCell ref="B451:F451"/>
+    <mergeCell ref="B452:F452"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="B454:F454"/>
+    <mergeCell ref="B455:F455"/>
+    <mergeCell ref="B456:F456"/>
+    <mergeCell ref="B445:F445"/>
+    <mergeCell ref="B446:F446"/>
+    <mergeCell ref="B447:F447"/>
+    <mergeCell ref="B448:F448"/>
+    <mergeCell ref="B449:F449"/>
+    <mergeCell ref="B450:F450"/>
+    <mergeCell ref="B439:F439"/>
+    <mergeCell ref="B440:F440"/>
+    <mergeCell ref="B441:F441"/>
+    <mergeCell ref="B442:F442"/>
+    <mergeCell ref="B443:F443"/>
+    <mergeCell ref="B444:F444"/>
+    <mergeCell ref="B433:F433"/>
+    <mergeCell ref="B434:F434"/>
+    <mergeCell ref="B435:F435"/>
+    <mergeCell ref="B436:F436"/>
+    <mergeCell ref="B437:F437"/>
+    <mergeCell ref="B438:F438"/>
+    <mergeCell ref="B427:F427"/>
+    <mergeCell ref="B428:F428"/>
+    <mergeCell ref="B429:F429"/>
+    <mergeCell ref="B430:F430"/>
+    <mergeCell ref="B431:F431"/>
+    <mergeCell ref="B432:F432"/>
+    <mergeCell ref="B421:F421"/>
+    <mergeCell ref="B422:F422"/>
+    <mergeCell ref="B423:F423"/>
+    <mergeCell ref="B424:F424"/>
+    <mergeCell ref="B425:F425"/>
+    <mergeCell ref="B426:F426"/>
+    <mergeCell ref="B415:F415"/>
+    <mergeCell ref="B416:F416"/>
+    <mergeCell ref="B417:F417"/>
+    <mergeCell ref="B418:F418"/>
+    <mergeCell ref="B419:F419"/>
+    <mergeCell ref="B420:F420"/>
+    <mergeCell ref="B409:F409"/>
+    <mergeCell ref="B410:F410"/>
+    <mergeCell ref="B411:F411"/>
+    <mergeCell ref="B412:F412"/>
+    <mergeCell ref="B413:F413"/>
+    <mergeCell ref="B414:F414"/>
+    <mergeCell ref="B403:F403"/>
+    <mergeCell ref="B404:F404"/>
+    <mergeCell ref="B405:F405"/>
+    <mergeCell ref="B406:F406"/>
+    <mergeCell ref="B407:F407"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="B397:F397"/>
+    <mergeCell ref="B398:F398"/>
+    <mergeCell ref="B399:F399"/>
+    <mergeCell ref="B400:F400"/>
+    <mergeCell ref="B401:F401"/>
+    <mergeCell ref="B402:F402"/>
+    <mergeCell ref="B391:F391"/>
+    <mergeCell ref="B392:F392"/>
+    <mergeCell ref="B393:F393"/>
+    <mergeCell ref="B394:F394"/>
+    <mergeCell ref="B395:F395"/>
+    <mergeCell ref="B396:F396"/>
+    <mergeCell ref="B385:F385"/>
+    <mergeCell ref="B386:F386"/>
+    <mergeCell ref="B387:F387"/>
+    <mergeCell ref="B388:F388"/>
+    <mergeCell ref="B389:F389"/>
+    <mergeCell ref="B390:F390"/>
+    <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B381:F381"/>
+    <mergeCell ref="B382:F382"/>
+    <mergeCell ref="B383:F383"/>
+    <mergeCell ref="B384:F384"/>
+    <mergeCell ref="B373:F373"/>
+    <mergeCell ref="B374:F374"/>
+    <mergeCell ref="B375:F375"/>
+    <mergeCell ref="B376:F376"/>
+    <mergeCell ref="B377:F377"/>
+    <mergeCell ref="B378:F378"/>
+    <mergeCell ref="B367:F367"/>
+    <mergeCell ref="B368:F368"/>
+    <mergeCell ref="B369:F369"/>
+    <mergeCell ref="B370:F370"/>
+    <mergeCell ref="B371:F371"/>
+    <mergeCell ref="B372:F372"/>
+    <mergeCell ref="B361:F361"/>
+    <mergeCell ref="B362:F362"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="B364:F364"/>
+    <mergeCell ref="B365:F365"/>
+    <mergeCell ref="B366:F366"/>
+    <mergeCell ref="B355:F355"/>
+    <mergeCell ref="B356:F356"/>
+    <mergeCell ref="B357:F357"/>
+    <mergeCell ref="B358:F358"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="B360:F360"/>
+    <mergeCell ref="B349:F349"/>
+    <mergeCell ref="B350:F350"/>
+    <mergeCell ref="B351:F351"/>
+    <mergeCell ref="B352:F352"/>
+    <mergeCell ref="B353:F353"/>
+    <mergeCell ref="B354:F354"/>
+    <mergeCell ref="B343:F343"/>
+    <mergeCell ref="B344:F344"/>
+    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B346:F346"/>
+    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="B348:F348"/>
+    <mergeCell ref="B337:F337"/>
+    <mergeCell ref="B338:F338"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="B340:F340"/>
+    <mergeCell ref="B341:F341"/>
+    <mergeCell ref="B342:F342"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B335:F335"/>
+    <mergeCell ref="B336:F336"/>
+    <mergeCell ref="B325:F325"/>
+    <mergeCell ref="B326:F326"/>
+    <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B328:F328"/>
+    <mergeCell ref="B329:F329"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B320:F320"/>
+    <mergeCell ref="B321:F321"/>
+    <mergeCell ref="B322:F322"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B324:F324"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B315:F315"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B317:F317"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B311:F311"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B306:F306"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B291:F291"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="B282:F282"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="B274:F274"/>
+    <mergeCell ref="B275:F275"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="B247:F247"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B250:F250"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B246:F246"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B236:F236"/>
+    <mergeCell ref="B237:F237"/>
+    <mergeCell ref="B238:F238"/>
+    <mergeCell ref="B239:F239"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B230:F230"/>
+    <mergeCell ref="B231:F231"/>
+    <mergeCell ref="B232:F232"/>
+    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B234:F234"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="B224:F224"/>
+    <mergeCell ref="B225:F225"/>
+    <mergeCell ref="B226:F226"/>
+    <mergeCell ref="B227:F227"/>
+    <mergeCell ref="B228:F228"/>
+    <mergeCell ref="B217:F217"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="B220:F220"/>
+    <mergeCell ref="B221:F221"/>
+    <mergeCell ref="B222:F222"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B214:F214"/>
+    <mergeCell ref="B215:F215"/>
+    <mergeCell ref="B216:F216"/>
+    <mergeCell ref="B205:F205"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B209:F209"/>
+    <mergeCell ref="B210:F210"/>
+    <mergeCell ref="B199:F199"/>
+    <mergeCell ref="B200:F200"/>
+    <mergeCell ref="B201:F201"/>
+    <mergeCell ref="B202:F202"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B204:F204"/>
+    <mergeCell ref="B193:F193"/>
+    <mergeCell ref="B194:F194"/>
+    <mergeCell ref="B195:F195"/>
+    <mergeCell ref="B196:F196"/>
+    <mergeCell ref="B197:F197"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B187:F187"/>
+    <mergeCell ref="B188:F188"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B190:F190"/>
+    <mergeCell ref="B191:F191"/>
+    <mergeCell ref="B192:F192"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B175:F175"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B178:F178"/>
+    <mergeCell ref="B179:F179"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B170:F170"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B173:F173"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B168:F168"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="B152:F152"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B127:F127"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B121:F121"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B109:F109"/>
+    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B105:F105"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B108:F108"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added work log data
</commit_message>
<xml_diff>
--- a/Documents/WorkLogs/JoshuaFord_workLog.xlsx
+++ b/Documents/WorkLogs/JoshuaFord_workLog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -81,6 +81,54 @@
   </si>
   <si>
     <t>finish question list, choose a method to use</t>
+  </si>
+  <si>
+    <t>worked on more questions for the customer, made a compelling argument for a desktop app, and worked will UMLs</t>
+  </si>
+  <si>
+    <t>Got questions ready for client (review), developed the prototype ideas farther.</t>
+  </si>
+  <si>
+    <t>Reviewed client questions, made several flowcharts to better understand the design solution, and worked on a good name for the product.</t>
+  </si>
+  <si>
+    <t>reviewed client answers to given questions, thought up some future question based on last client meeting, reviewed desktop proposal.</t>
+  </si>
+  <si>
+    <t>See meeting minutes</t>
+  </si>
+  <si>
+    <t>read over spec doc</t>
+  </si>
+  <si>
+    <t>see client meeting minutes</t>
+  </si>
+  <si>
+    <t>Discussed programming language best for this problem, and worked on more client questions.</t>
+  </si>
+  <si>
+    <t>more work on the Spec Doc. Yay</t>
+  </si>
+  <si>
+    <t>Discussed FileIO and began planning on how to implenemt it.</t>
+  </si>
+  <si>
+    <t>Spoke with dr. Roden about the spec Doc. Back to the drawing board</t>
+  </si>
+  <si>
+    <t>see teacher meeting minutes</t>
+  </si>
+  <si>
+    <t>Looked over My FileIn class, got feedback did some adjusting.</t>
+  </si>
+  <si>
+    <t>see meeting minutes</t>
+  </si>
+  <si>
+    <t>worked on a good design for compression. Feel like I'm hitting a brick wall.</t>
+  </si>
+  <si>
+    <t>worked on final touches to LIFES system.</t>
   </si>
 </sst>
 </file>
@@ -648,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -718,7 +766,7 @@
       </c>
       <c r="I4" s="11">
         <f>SUM(G4:G2000)</f>
-        <v>39.25</v>
+        <v>109.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
@@ -932,321 +980,577 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
+      <c r="A19" s="9">
+        <v>42040</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
+      <c r="G19" s="6">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="12"/>
+      <c r="A20" s="9">
+        <v>42045</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
+      <c r="G20" s="6">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
+      <c r="A21" s="9">
+        <v>42047</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
+      <c r="G21" s="6">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
+      <c r="A22" s="9">
+        <v>42048</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
+      <c r="G22" s="6">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
+      <c r="A23" s="9">
+        <v>42058</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
+      <c r="G23" s="6">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="12"/>
+      <c r="A24" s="9">
+        <v>42058</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
+      <c r="G24" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
+      <c r="A25" s="9">
+        <v>42059</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
+      <c r="G25" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="12"/>
+      <c r="A26" s="9">
+        <v>42059</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
+      <c r="G26" s="6">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="12"/>
+      <c r="A27" s="9">
+        <v>42062</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
+      <c r="G27" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="12"/>
+      <c r="A28" s="9">
+        <v>42066</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
+      <c r="G28" s="6">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="12"/>
+      <c r="A29" s="9">
+        <v>42073</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
+      <c r="G29" s="6">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="12"/>
+      <c r="A30" s="9">
+        <v>42076</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
+      <c r="G30" s="6">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="12"/>
+      <c r="A31" s="9">
+        <v>42076</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
+      <c r="G31" s="6">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="12"/>
+      <c r="A32" s="9">
+        <v>42079</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="12"/>
+      <c r="G32" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="9">
+        <v>42082</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="12"/>
+      <c r="G33" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="9">
+        <v>42082</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" s="12"/>
+      <c r="G34" s="6">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="9">
+        <v>42093</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" s="12"/>
+      <c r="G35" s="6">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="9">
+        <v>42094</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="12"/>
+      <c r="G36" s="6">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="9">
+        <v>42096</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="12"/>
+      <c r="G37" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="9">
+        <v>42096</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="12"/>
+      <c r="G38" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="9">
+        <v>42101</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="12"/>
+      <c r="G39" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="9">
+        <v>42103</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="12"/>
+      <c r="G40" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="9">
+        <v>42108</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="12"/>
+      <c r="G41" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="9">
+        <v>42110</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="12"/>
+      <c r="G42" s="6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="9">
+        <v>42110</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="12"/>
+      <c r="G43" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="9">
+        <v>42114</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="12"/>
+      <c r="G44" s="6">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="9">
+        <v>42117</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" s="12"/>
+      <c r="G45" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="9">
+        <v>42123</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="12"/>
+      <c r="G46" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="9">
+        <v>42124</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="12"/>
+      <c r="G47" s="6">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="9">
+        <v>42125</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B49" s="12"/>
+      <c r="G48" s="6">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="9">
+        <v>42128</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B50" s="12"/>
+      <c r="G49" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="9">
+        <v>42129</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G50" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
       <c r="D64" s="12"/>
@@ -14772,6 +15076,1980 @@
     </row>
   </sheetData>
   <mergeCells count="1995">
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B115:F115"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B109:F109"/>
+    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B105:F105"/>
+    <mergeCell ref="B106:F106"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B108:F108"/>
+    <mergeCell ref="B133:F133"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B135:F135"/>
+    <mergeCell ref="B136:F136"/>
+    <mergeCell ref="B137:F137"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B127:F127"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="B132:F132"/>
+    <mergeCell ref="B121:F121"/>
+    <mergeCell ref="B122:F122"/>
+    <mergeCell ref="B123:F123"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B151:F151"/>
+    <mergeCell ref="B152:F152"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B154:F154"/>
+    <mergeCell ref="B155:F155"/>
+    <mergeCell ref="B156:F156"/>
+    <mergeCell ref="B145:F145"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B147:F147"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B139:F139"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B144:F144"/>
+    <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B170:F170"/>
+    <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B173:F173"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B163:F163"/>
+    <mergeCell ref="B164:F164"/>
+    <mergeCell ref="B165:F165"/>
+    <mergeCell ref="B166:F166"/>
+    <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B168:F168"/>
+    <mergeCell ref="B157:F157"/>
+    <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B159:F159"/>
+    <mergeCell ref="B160:F160"/>
+    <mergeCell ref="B161:F161"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B187:F187"/>
+    <mergeCell ref="B188:F188"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B190:F190"/>
+    <mergeCell ref="B191:F191"/>
+    <mergeCell ref="B192:F192"/>
+    <mergeCell ref="B181:F181"/>
+    <mergeCell ref="B182:F182"/>
+    <mergeCell ref="B183:F183"/>
+    <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B175:F175"/>
+    <mergeCell ref="B176:F176"/>
+    <mergeCell ref="B177:F177"/>
+    <mergeCell ref="B178:F178"/>
+    <mergeCell ref="B179:F179"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B205:F205"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B209:F209"/>
+    <mergeCell ref="B210:F210"/>
+    <mergeCell ref="B199:F199"/>
+    <mergeCell ref="B200:F200"/>
+    <mergeCell ref="B201:F201"/>
+    <mergeCell ref="B202:F202"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B204:F204"/>
+    <mergeCell ref="B193:F193"/>
+    <mergeCell ref="B194:F194"/>
+    <mergeCell ref="B195:F195"/>
+    <mergeCell ref="B196:F196"/>
+    <mergeCell ref="B197:F197"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="B224:F224"/>
+    <mergeCell ref="B225:F225"/>
+    <mergeCell ref="B226:F226"/>
+    <mergeCell ref="B227:F227"/>
+    <mergeCell ref="B228:F228"/>
+    <mergeCell ref="B217:F217"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="B220:F220"/>
+    <mergeCell ref="B221:F221"/>
+    <mergeCell ref="B222:F222"/>
+    <mergeCell ref="B211:F211"/>
+    <mergeCell ref="B212:F212"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B214:F214"/>
+    <mergeCell ref="B215:F215"/>
+    <mergeCell ref="B216:F216"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B242:F242"/>
+    <mergeCell ref="B243:F243"/>
+    <mergeCell ref="B244:F244"/>
+    <mergeCell ref="B245:F245"/>
+    <mergeCell ref="B246:F246"/>
+    <mergeCell ref="B235:F235"/>
+    <mergeCell ref="B236:F236"/>
+    <mergeCell ref="B237:F237"/>
+    <mergeCell ref="B238:F238"/>
+    <mergeCell ref="B239:F239"/>
+    <mergeCell ref="B240:F240"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B230:F230"/>
+    <mergeCell ref="B231:F231"/>
+    <mergeCell ref="B232:F232"/>
+    <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B234:F234"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
+    <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B264:F264"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="B247:F247"/>
+    <mergeCell ref="B248:F248"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B250:F250"/>
+    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="B282:F282"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="B274:F274"/>
+    <mergeCell ref="B275:F275"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B291:F291"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B315:F315"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B317:F317"/>
+    <mergeCell ref="B318:F318"/>
+    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B311:F311"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B306:F306"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B335:F335"/>
+    <mergeCell ref="B336:F336"/>
+    <mergeCell ref="B325:F325"/>
+    <mergeCell ref="B326:F326"/>
+    <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B328:F328"/>
+    <mergeCell ref="B329:F329"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B320:F320"/>
+    <mergeCell ref="B321:F321"/>
+    <mergeCell ref="B322:F322"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B324:F324"/>
+    <mergeCell ref="B349:F349"/>
+    <mergeCell ref="B350:F350"/>
+    <mergeCell ref="B351:F351"/>
+    <mergeCell ref="B352:F352"/>
+    <mergeCell ref="B353:F353"/>
+    <mergeCell ref="B354:F354"/>
+    <mergeCell ref="B343:F343"/>
+    <mergeCell ref="B344:F344"/>
+    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B346:F346"/>
+    <mergeCell ref="B347:F347"/>
+    <mergeCell ref="B348:F348"/>
+    <mergeCell ref="B337:F337"/>
+    <mergeCell ref="B338:F338"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="B340:F340"/>
+    <mergeCell ref="B341:F341"/>
+    <mergeCell ref="B342:F342"/>
+    <mergeCell ref="B367:F367"/>
+    <mergeCell ref="B368:F368"/>
+    <mergeCell ref="B369:F369"/>
+    <mergeCell ref="B370:F370"/>
+    <mergeCell ref="B371:F371"/>
+    <mergeCell ref="B372:F372"/>
+    <mergeCell ref="B361:F361"/>
+    <mergeCell ref="B362:F362"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="B364:F364"/>
+    <mergeCell ref="B365:F365"/>
+    <mergeCell ref="B366:F366"/>
+    <mergeCell ref="B355:F355"/>
+    <mergeCell ref="B356:F356"/>
+    <mergeCell ref="B357:F357"/>
+    <mergeCell ref="B358:F358"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="B360:F360"/>
+    <mergeCell ref="B385:F385"/>
+    <mergeCell ref="B386:F386"/>
+    <mergeCell ref="B387:F387"/>
+    <mergeCell ref="B388:F388"/>
+    <mergeCell ref="B389:F389"/>
+    <mergeCell ref="B390:F390"/>
+    <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B381:F381"/>
+    <mergeCell ref="B382:F382"/>
+    <mergeCell ref="B383:F383"/>
+    <mergeCell ref="B384:F384"/>
+    <mergeCell ref="B373:F373"/>
+    <mergeCell ref="B374:F374"/>
+    <mergeCell ref="B375:F375"/>
+    <mergeCell ref="B376:F376"/>
+    <mergeCell ref="B377:F377"/>
+    <mergeCell ref="B378:F378"/>
+    <mergeCell ref="B403:F403"/>
+    <mergeCell ref="B404:F404"/>
+    <mergeCell ref="B405:F405"/>
+    <mergeCell ref="B406:F406"/>
+    <mergeCell ref="B407:F407"/>
+    <mergeCell ref="B408:F408"/>
+    <mergeCell ref="B397:F397"/>
+    <mergeCell ref="B398:F398"/>
+    <mergeCell ref="B399:F399"/>
+    <mergeCell ref="B400:F400"/>
+    <mergeCell ref="B401:F401"/>
+    <mergeCell ref="B402:F402"/>
+    <mergeCell ref="B391:F391"/>
+    <mergeCell ref="B392:F392"/>
+    <mergeCell ref="B393:F393"/>
+    <mergeCell ref="B394:F394"/>
+    <mergeCell ref="B395:F395"/>
+    <mergeCell ref="B396:F396"/>
+    <mergeCell ref="B421:F421"/>
+    <mergeCell ref="B422:F422"/>
+    <mergeCell ref="B423:F423"/>
+    <mergeCell ref="B424:F424"/>
+    <mergeCell ref="B425:F425"/>
+    <mergeCell ref="B426:F426"/>
+    <mergeCell ref="B415:F415"/>
+    <mergeCell ref="B416:F416"/>
+    <mergeCell ref="B417:F417"/>
+    <mergeCell ref="B418:F418"/>
+    <mergeCell ref="B419:F419"/>
+    <mergeCell ref="B420:F420"/>
+    <mergeCell ref="B409:F409"/>
+    <mergeCell ref="B410:F410"/>
+    <mergeCell ref="B411:F411"/>
+    <mergeCell ref="B412:F412"/>
+    <mergeCell ref="B413:F413"/>
+    <mergeCell ref="B414:F414"/>
+    <mergeCell ref="B439:F439"/>
+    <mergeCell ref="B440:F440"/>
+    <mergeCell ref="B441:F441"/>
+    <mergeCell ref="B442:F442"/>
+    <mergeCell ref="B443:F443"/>
+    <mergeCell ref="B444:F444"/>
+    <mergeCell ref="B433:F433"/>
+    <mergeCell ref="B434:F434"/>
+    <mergeCell ref="B435:F435"/>
+    <mergeCell ref="B436:F436"/>
+    <mergeCell ref="B437:F437"/>
+    <mergeCell ref="B438:F438"/>
+    <mergeCell ref="B427:F427"/>
+    <mergeCell ref="B428:F428"/>
+    <mergeCell ref="B429:F429"/>
+    <mergeCell ref="B430:F430"/>
+    <mergeCell ref="B431:F431"/>
+    <mergeCell ref="B432:F432"/>
+    <mergeCell ref="B457:F457"/>
+    <mergeCell ref="B458:F458"/>
+    <mergeCell ref="B459:F459"/>
+    <mergeCell ref="B460:F460"/>
+    <mergeCell ref="B461:F461"/>
+    <mergeCell ref="B462:F462"/>
+    <mergeCell ref="B451:F451"/>
+    <mergeCell ref="B452:F452"/>
+    <mergeCell ref="B453:F453"/>
+    <mergeCell ref="B454:F454"/>
+    <mergeCell ref="B455:F455"/>
+    <mergeCell ref="B456:F456"/>
+    <mergeCell ref="B445:F445"/>
+    <mergeCell ref="B446:F446"/>
+    <mergeCell ref="B447:F447"/>
+    <mergeCell ref="B448:F448"/>
+    <mergeCell ref="B449:F449"/>
+    <mergeCell ref="B450:F450"/>
+    <mergeCell ref="B475:F475"/>
+    <mergeCell ref="B476:F476"/>
+    <mergeCell ref="B477:F477"/>
+    <mergeCell ref="B478:F478"/>
+    <mergeCell ref="B479:F479"/>
+    <mergeCell ref="B480:F480"/>
+    <mergeCell ref="B469:F469"/>
+    <mergeCell ref="B470:F470"/>
+    <mergeCell ref="B471:F471"/>
+    <mergeCell ref="B472:F472"/>
+    <mergeCell ref="B473:F473"/>
+    <mergeCell ref="B474:F474"/>
+    <mergeCell ref="B463:F463"/>
+    <mergeCell ref="B464:F464"/>
+    <mergeCell ref="B465:F465"/>
+    <mergeCell ref="B466:F466"/>
+    <mergeCell ref="B467:F467"/>
+    <mergeCell ref="B468:F468"/>
+    <mergeCell ref="B493:F493"/>
+    <mergeCell ref="B494:F494"/>
+    <mergeCell ref="B495:F495"/>
+    <mergeCell ref="B496:F496"/>
+    <mergeCell ref="B497:F497"/>
+    <mergeCell ref="B498:F498"/>
+    <mergeCell ref="B487:F487"/>
+    <mergeCell ref="B488:F488"/>
+    <mergeCell ref="B489:F489"/>
+    <mergeCell ref="B490:F490"/>
+    <mergeCell ref="B491:F491"/>
+    <mergeCell ref="B492:F492"/>
+    <mergeCell ref="B481:F481"/>
+    <mergeCell ref="B482:F482"/>
+    <mergeCell ref="B483:F483"/>
+    <mergeCell ref="B484:F484"/>
+    <mergeCell ref="B485:F485"/>
+    <mergeCell ref="B486:F486"/>
+    <mergeCell ref="B511:F511"/>
+    <mergeCell ref="B512:F512"/>
+    <mergeCell ref="B513:F513"/>
+    <mergeCell ref="B514:F514"/>
+    <mergeCell ref="B515:F515"/>
+    <mergeCell ref="B516:F516"/>
+    <mergeCell ref="B505:F505"/>
+    <mergeCell ref="B506:F506"/>
+    <mergeCell ref="B507:F507"/>
+    <mergeCell ref="B508:F508"/>
+    <mergeCell ref="B509:F509"/>
+    <mergeCell ref="B510:F510"/>
+    <mergeCell ref="B499:F499"/>
+    <mergeCell ref="B500:F500"/>
+    <mergeCell ref="B501:F501"/>
+    <mergeCell ref="B502:F502"/>
+    <mergeCell ref="B503:F503"/>
+    <mergeCell ref="B504:F504"/>
+    <mergeCell ref="B529:F529"/>
+    <mergeCell ref="B530:F530"/>
+    <mergeCell ref="B531:F531"/>
+    <mergeCell ref="B532:F532"/>
+    <mergeCell ref="B533:F533"/>
+    <mergeCell ref="B534:F534"/>
+    <mergeCell ref="B523:F523"/>
+    <mergeCell ref="B524:F524"/>
+    <mergeCell ref="B525:F525"/>
+    <mergeCell ref="B526:F526"/>
+    <mergeCell ref="B527:F527"/>
+    <mergeCell ref="B528:F528"/>
+    <mergeCell ref="B517:F517"/>
+    <mergeCell ref="B518:F518"/>
+    <mergeCell ref="B519:F519"/>
+    <mergeCell ref="B520:F520"/>
+    <mergeCell ref="B521:F521"/>
+    <mergeCell ref="B522:F522"/>
+    <mergeCell ref="B547:F547"/>
+    <mergeCell ref="B548:F548"/>
+    <mergeCell ref="B549:F549"/>
+    <mergeCell ref="B550:F550"/>
+    <mergeCell ref="B551:F551"/>
+    <mergeCell ref="B552:F552"/>
+    <mergeCell ref="B541:F541"/>
+    <mergeCell ref="B542:F542"/>
+    <mergeCell ref="B543:F543"/>
+    <mergeCell ref="B544:F544"/>
+    <mergeCell ref="B545:F545"/>
+    <mergeCell ref="B546:F546"/>
+    <mergeCell ref="B535:F535"/>
+    <mergeCell ref="B536:F536"/>
+    <mergeCell ref="B537:F537"/>
+    <mergeCell ref="B538:F538"/>
+    <mergeCell ref="B539:F539"/>
+    <mergeCell ref="B540:F540"/>
+    <mergeCell ref="B565:F565"/>
+    <mergeCell ref="B566:F566"/>
+    <mergeCell ref="B567:F567"/>
+    <mergeCell ref="B568:F568"/>
+    <mergeCell ref="B569:F569"/>
+    <mergeCell ref="B570:F570"/>
+    <mergeCell ref="B559:F559"/>
+    <mergeCell ref="B560:F560"/>
+    <mergeCell ref="B561:F561"/>
+    <mergeCell ref="B562:F562"/>
+    <mergeCell ref="B563:F563"/>
+    <mergeCell ref="B564:F564"/>
+    <mergeCell ref="B553:F553"/>
+    <mergeCell ref="B554:F554"/>
+    <mergeCell ref="B555:F555"/>
+    <mergeCell ref="B556:F556"/>
+    <mergeCell ref="B557:F557"/>
+    <mergeCell ref="B558:F558"/>
+    <mergeCell ref="B583:F583"/>
+    <mergeCell ref="B584:F584"/>
+    <mergeCell ref="B585:F585"/>
+    <mergeCell ref="B586:F586"/>
+    <mergeCell ref="B587:F587"/>
+    <mergeCell ref="B588:F588"/>
+    <mergeCell ref="B577:F577"/>
+    <mergeCell ref="B578:F578"/>
+    <mergeCell ref="B579:F579"/>
+    <mergeCell ref="B580:F580"/>
+    <mergeCell ref="B581:F581"/>
+    <mergeCell ref="B582:F582"/>
+    <mergeCell ref="B571:F571"/>
+    <mergeCell ref="B572:F572"/>
+    <mergeCell ref="B573:F573"/>
+    <mergeCell ref="B574:F574"/>
+    <mergeCell ref="B575:F575"/>
+    <mergeCell ref="B576:F576"/>
+    <mergeCell ref="B601:F601"/>
+    <mergeCell ref="B602:F602"/>
+    <mergeCell ref="B603:F603"/>
+    <mergeCell ref="B604:F604"/>
+    <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B606:F606"/>
+    <mergeCell ref="B595:F595"/>
+    <mergeCell ref="B596:F596"/>
+    <mergeCell ref="B597:F597"/>
+    <mergeCell ref="B598:F598"/>
+    <mergeCell ref="B599:F599"/>
+    <mergeCell ref="B600:F600"/>
+    <mergeCell ref="B589:F589"/>
+    <mergeCell ref="B590:F590"/>
+    <mergeCell ref="B591:F591"/>
+    <mergeCell ref="B592:F592"/>
+    <mergeCell ref="B593:F593"/>
+    <mergeCell ref="B594:F594"/>
+    <mergeCell ref="B619:F619"/>
+    <mergeCell ref="B620:F620"/>
+    <mergeCell ref="B621:F621"/>
+    <mergeCell ref="B622:F622"/>
+    <mergeCell ref="B623:F623"/>
+    <mergeCell ref="B624:F624"/>
+    <mergeCell ref="B613:F613"/>
+    <mergeCell ref="B614:F614"/>
+    <mergeCell ref="B615:F615"/>
+    <mergeCell ref="B616:F616"/>
+    <mergeCell ref="B617:F617"/>
+    <mergeCell ref="B618:F618"/>
+    <mergeCell ref="B607:F607"/>
+    <mergeCell ref="B608:F608"/>
+    <mergeCell ref="B609:F609"/>
+    <mergeCell ref="B610:F610"/>
+    <mergeCell ref="B611:F611"/>
+    <mergeCell ref="B612:F612"/>
+    <mergeCell ref="B637:F637"/>
+    <mergeCell ref="B638:F638"/>
+    <mergeCell ref="B639:F639"/>
+    <mergeCell ref="B640:F640"/>
+    <mergeCell ref="B641:F641"/>
+    <mergeCell ref="B642:F642"/>
+    <mergeCell ref="B631:F631"/>
+    <mergeCell ref="B632:F632"/>
+    <mergeCell ref="B633:F633"/>
+    <mergeCell ref="B634:F634"/>
+    <mergeCell ref="B635:F635"/>
+    <mergeCell ref="B636:F636"/>
+    <mergeCell ref="B625:F625"/>
+    <mergeCell ref="B626:F626"/>
+    <mergeCell ref="B627:F627"/>
+    <mergeCell ref="B628:F628"/>
+    <mergeCell ref="B629:F629"/>
+    <mergeCell ref="B630:F630"/>
+    <mergeCell ref="B655:F655"/>
+    <mergeCell ref="B656:F656"/>
+    <mergeCell ref="B657:F657"/>
+    <mergeCell ref="B658:F658"/>
+    <mergeCell ref="B659:F659"/>
+    <mergeCell ref="B660:F660"/>
+    <mergeCell ref="B649:F649"/>
+    <mergeCell ref="B650:F650"/>
+    <mergeCell ref="B651:F651"/>
+    <mergeCell ref="B652:F652"/>
+    <mergeCell ref="B653:F653"/>
+    <mergeCell ref="B654:F654"/>
+    <mergeCell ref="B643:F643"/>
+    <mergeCell ref="B644:F644"/>
+    <mergeCell ref="B645:F645"/>
+    <mergeCell ref="B646:F646"/>
+    <mergeCell ref="B647:F647"/>
+    <mergeCell ref="B648:F648"/>
+    <mergeCell ref="B673:F673"/>
+    <mergeCell ref="B674:F674"/>
+    <mergeCell ref="B675:F675"/>
+    <mergeCell ref="B676:F676"/>
+    <mergeCell ref="B677:F677"/>
+    <mergeCell ref="B678:F678"/>
+    <mergeCell ref="B667:F667"/>
+    <mergeCell ref="B668:F668"/>
+    <mergeCell ref="B669:F669"/>
+    <mergeCell ref="B670:F670"/>
+    <mergeCell ref="B671:F671"/>
+    <mergeCell ref="B672:F672"/>
+    <mergeCell ref="B661:F661"/>
+    <mergeCell ref="B662:F662"/>
+    <mergeCell ref="B663:F663"/>
+    <mergeCell ref="B664:F664"/>
+    <mergeCell ref="B665:F665"/>
+    <mergeCell ref="B666:F666"/>
+    <mergeCell ref="B691:F691"/>
+    <mergeCell ref="B692:F692"/>
+    <mergeCell ref="B693:F693"/>
+    <mergeCell ref="B694:F694"/>
+    <mergeCell ref="B695:F695"/>
+    <mergeCell ref="B696:F696"/>
+    <mergeCell ref="B685:F685"/>
+    <mergeCell ref="B686:F686"/>
+    <mergeCell ref="B687:F687"/>
+    <mergeCell ref="B688:F688"/>
+    <mergeCell ref="B689:F689"/>
+    <mergeCell ref="B690:F690"/>
+    <mergeCell ref="B679:F679"/>
+    <mergeCell ref="B680:F680"/>
+    <mergeCell ref="B681:F681"/>
+    <mergeCell ref="B682:F682"/>
+    <mergeCell ref="B683:F683"/>
+    <mergeCell ref="B684:F684"/>
+    <mergeCell ref="B709:F709"/>
+    <mergeCell ref="B710:F710"/>
+    <mergeCell ref="B711:F711"/>
+    <mergeCell ref="B712:F712"/>
+    <mergeCell ref="B713:F713"/>
+    <mergeCell ref="B714:F714"/>
+    <mergeCell ref="B703:F703"/>
+    <mergeCell ref="B704:F704"/>
+    <mergeCell ref="B705:F705"/>
+    <mergeCell ref="B706:F706"/>
+    <mergeCell ref="B707:F707"/>
+    <mergeCell ref="B708:F708"/>
+    <mergeCell ref="B697:F697"/>
+    <mergeCell ref="B698:F698"/>
+    <mergeCell ref="B699:F699"/>
+    <mergeCell ref="B700:F700"/>
+    <mergeCell ref="B701:F701"/>
+    <mergeCell ref="B702:F702"/>
+    <mergeCell ref="B727:F727"/>
+    <mergeCell ref="B728:F728"/>
+    <mergeCell ref="B729:F729"/>
+    <mergeCell ref="B730:F730"/>
+    <mergeCell ref="B731:F731"/>
+    <mergeCell ref="B732:F732"/>
+    <mergeCell ref="B721:F721"/>
+    <mergeCell ref="B722:F722"/>
+    <mergeCell ref="B723:F723"/>
+    <mergeCell ref="B724:F724"/>
+    <mergeCell ref="B725:F725"/>
+    <mergeCell ref="B726:F726"/>
+    <mergeCell ref="B715:F715"/>
+    <mergeCell ref="B716:F716"/>
+    <mergeCell ref="B717:F717"/>
+    <mergeCell ref="B718:F718"/>
+    <mergeCell ref="B719:F719"/>
+    <mergeCell ref="B720:F720"/>
+    <mergeCell ref="B745:F745"/>
+    <mergeCell ref="B746:F746"/>
+    <mergeCell ref="B747:F747"/>
+    <mergeCell ref="B748:F748"/>
+    <mergeCell ref="B749:F749"/>
+    <mergeCell ref="B750:F750"/>
+    <mergeCell ref="B739:F739"/>
+    <mergeCell ref="B740:F740"/>
+    <mergeCell ref="B741:F741"/>
+    <mergeCell ref="B742:F742"/>
+    <mergeCell ref="B743:F743"/>
+    <mergeCell ref="B744:F744"/>
+    <mergeCell ref="B733:F733"/>
+    <mergeCell ref="B734:F734"/>
+    <mergeCell ref="B735:F735"/>
+    <mergeCell ref="B736:F736"/>
+    <mergeCell ref="B737:F737"/>
+    <mergeCell ref="B738:F738"/>
+    <mergeCell ref="B763:F763"/>
+    <mergeCell ref="B764:F764"/>
+    <mergeCell ref="B765:F765"/>
+    <mergeCell ref="B766:F766"/>
+    <mergeCell ref="B767:F767"/>
+    <mergeCell ref="B768:F768"/>
+    <mergeCell ref="B757:F757"/>
+    <mergeCell ref="B758:F758"/>
+    <mergeCell ref="B759:F759"/>
+    <mergeCell ref="B760:F760"/>
+    <mergeCell ref="B761:F761"/>
+    <mergeCell ref="B762:F762"/>
+    <mergeCell ref="B751:F751"/>
+    <mergeCell ref="B752:F752"/>
+    <mergeCell ref="B753:F753"/>
+    <mergeCell ref="B754:F754"/>
+    <mergeCell ref="B755:F755"/>
+    <mergeCell ref="B756:F756"/>
+    <mergeCell ref="B781:F781"/>
+    <mergeCell ref="B782:F782"/>
+    <mergeCell ref="B783:F783"/>
+    <mergeCell ref="B784:F784"/>
+    <mergeCell ref="B785:F785"/>
+    <mergeCell ref="B786:F786"/>
+    <mergeCell ref="B775:F775"/>
+    <mergeCell ref="B776:F776"/>
+    <mergeCell ref="B777:F777"/>
+    <mergeCell ref="B778:F778"/>
+    <mergeCell ref="B779:F779"/>
+    <mergeCell ref="B780:F780"/>
+    <mergeCell ref="B769:F769"/>
+    <mergeCell ref="B770:F770"/>
+    <mergeCell ref="B771:F771"/>
+    <mergeCell ref="B772:F772"/>
+    <mergeCell ref="B773:F773"/>
+    <mergeCell ref="B774:F774"/>
+    <mergeCell ref="B799:F799"/>
+    <mergeCell ref="B800:F800"/>
+    <mergeCell ref="B801:F801"/>
+    <mergeCell ref="B802:F802"/>
+    <mergeCell ref="B803:F803"/>
+    <mergeCell ref="B804:F804"/>
+    <mergeCell ref="B793:F793"/>
+    <mergeCell ref="B794:F794"/>
+    <mergeCell ref="B795:F795"/>
+    <mergeCell ref="B796:F796"/>
+    <mergeCell ref="B797:F797"/>
+    <mergeCell ref="B798:F798"/>
+    <mergeCell ref="B787:F787"/>
+    <mergeCell ref="B788:F788"/>
+    <mergeCell ref="B789:F789"/>
+    <mergeCell ref="B790:F790"/>
+    <mergeCell ref="B791:F791"/>
+    <mergeCell ref="B792:F792"/>
+    <mergeCell ref="B817:F817"/>
+    <mergeCell ref="B818:F818"/>
+    <mergeCell ref="B819:F819"/>
+    <mergeCell ref="B820:F820"/>
+    <mergeCell ref="B821:F821"/>
+    <mergeCell ref="B822:F822"/>
+    <mergeCell ref="B811:F811"/>
+    <mergeCell ref="B812:F812"/>
+    <mergeCell ref="B813:F813"/>
+    <mergeCell ref="B814:F814"/>
+    <mergeCell ref="B815:F815"/>
+    <mergeCell ref="B816:F816"/>
+    <mergeCell ref="B805:F805"/>
+    <mergeCell ref="B806:F806"/>
+    <mergeCell ref="B807:F807"/>
+    <mergeCell ref="B808:F808"/>
+    <mergeCell ref="B809:F809"/>
+    <mergeCell ref="B810:F810"/>
+    <mergeCell ref="B835:F835"/>
+    <mergeCell ref="B836:F836"/>
+    <mergeCell ref="B837:F837"/>
+    <mergeCell ref="B838:F838"/>
+    <mergeCell ref="B839:F839"/>
+    <mergeCell ref="B840:F840"/>
+    <mergeCell ref="B829:F829"/>
+    <mergeCell ref="B830:F830"/>
+    <mergeCell ref="B831:F831"/>
+    <mergeCell ref="B832:F832"/>
+    <mergeCell ref="B833:F833"/>
+    <mergeCell ref="B834:F834"/>
+    <mergeCell ref="B823:F823"/>
+    <mergeCell ref="B824:F824"/>
+    <mergeCell ref="B825:F825"/>
+    <mergeCell ref="B826:F826"/>
+    <mergeCell ref="B827:F827"/>
+    <mergeCell ref="B828:F828"/>
+    <mergeCell ref="B853:F853"/>
+    <mergeCell ref="B854:F854"/>
+    <mergeCell ref="B855:F855"/>
+    <mergeCell ref="B856:F856"/>
+    <mergeCell ref="B857:F857"/>
+    <mergeCell ref="B858:F858"/>
+    <mergeCell ref="B847:F847"/>
+    <mergeCell ref="B848:F848"/>
+    <mergeCell ref="B849:F849"/>
+    <mergeCell ref="B850:F850"/>
+    <mergeCell ref="B851:F851"/>
+    <mergeCell ref="B852:F852"/>
+    <mergeCell ref="B841:F841"/>
+    <mergeCell ref="B842:F842"/>
+    <mergeCell ref="B843:F843"/>
+    <mergeCell ref="B844:F844"/>
+    <mergeCell ref="B845:F845"/>
+    <mergeCell ref="B846:F846"/>
+    <mergeCell ref="B871:F871"/>
+    <mergeCell ref="B872:F872"/>
+    <mergeCell ref="B873:F873"/>
+    <mergeCell ref="B874:F874"/>
+    <mergeCell ref="B875:F875"/>
+    <mergeCell ref="B876:F876"/>
+    <mergeCell ref="B865:F865"/>
+    <mergeCell ref="B866:F866"/>
+    <mergeCell ref="B867:F867"/>
+    <mergeCell ref="B868:F868"/>
+    <mergeCell ref="B869:F869"/>
+    <mergeCell ref="B870:F870"/>
+    <mergeCell ref="B859:F859"/>
+    <mergeCell ref="B860:F860"/>
+    <mergeCell ref="B861:F861"/>
+    <mergeCell ref="B862:F862"/>
+    <mergeCell ref="B863:F863"/>
+    <mergeCell ref="B864:F864"/>
+    <mergeCell ref="B889:F889"/>
+    <mergeCell ref="B890:F890"/>
+    <mergeCell ref="B891:F891"/>
+    <mergeCell ref="B892:F892"/>
+    <mergeCell ref="B893:F893"/>
+    <mergeCell ref="B894:F894"/>
+    <mergeCell ref="B883:F883"/>
+    <mergeCell ref="B884:F884"/>
+    <mergeCell ref="B885:F885"/>
+    <mergeCell ref="B886:F886"/>
+    <mergeCell ref="B887:F887"/>
+    <mergeCell ref="B888:F888"/>
+    <mergeCell ref="B877:F877"/>
+    <mergeCell ref="B878:F878"/>
+    <mergeCell ref="B879:F879"/>
+    <mergeCell ref="B880:F880"/>
+    <mergeCell ref="B881:F881"/>
+    <mergeCell ref="B882:F882"/>
+    <mergeCell ref="B907:F907"/>
+    <mergeCell ref="B908:F908"/>
+    <mergeCell ref="B909:F909"/>
+    <mergeCell ref="B910:F910"/>
+    <mergeCell ref="B911:F911"/>
+    <mergeCell ref="B912:F912"/>
+    <mergeCell ref="B901:F901"/>
+    <mergeCell ref="B902:F902"/>
+    <mergeCell ref="B903:F903"/>
+    <mergeCell ref="B904:F904"/>
+    <mergeCell ref="B905:F905"/>
+    <mergeCell ref="B906:F906"/>
+    <mergeCell ref="B895:F895"/>
+    <mergeCell ref="B896:F896"/>
+    <mergeCell ref="B897:F897"/>
+    <mergeCell ref="B898:F898"/>
+    <mergeCell ref="B899:F899"/>
+    <mergeCell ref="B900:F900"/>
+    <mergeCell ref="B925:F925"/>
+    <mergeCell ref="B926:F926"/>
+    <mergeCell ref="B927:F927"/>
+    <mergeCell ref="B928:F928"/>
+    <mergeCell ref="B929:F929"/>
+    <mergeCell ref="B930:F930"/>
+    <mergeCell ref="B919:F919"/>
+    <mergeCell ref="B920:F920"/>
+    <mergeCell ref="B921:F921"/>
+    <mergeCell ref="B922:F922"/>
+    <mergeCell ref="B923:F923"/>
+    <mergeCell ref="B924:F924"/>
+    <mergeCell ref="B913:F913"/>
+    <mergeCell ref="B914:F914"/>
+    <mergeCell ref="B915:F915"/>
+    <mergeCell ref="B916:F916"/>
+    <mergeCell ref="B917:F917"/>
+    <mergeCell ref="B918:F918"/>
+    <mergeCell ref="B943:F943"/>
+    <mergeCell ref="B944:F944"/>
+    <mergeCell ref="B945:F945"/>
+    <mergeCell ref="B946:F946"/>
+    <mergeCell ref="B947:F947"/>
+    <mergeCell ref="B948:F948"/>
+    <mergeCell ref="B937:F937"/>
+    <mergeCell ref="B938:F938"/>
+    <mergeCell ref="B939:F939"/>
+    <mergeCell ref="B940:F940"/>
+    <mergeCell ref="B941:F941"/>
+    <mergeCell ref="B942:F942"/>
+    <mergeCell ref="B931:F931"/>
+    <mergeCell ref="B932:F932"/>
+    <mergeCell ref="B933:F933"/>
+    <mergeCell ref="B934:F934"/>
+    <mergeCell ref="B935:F935"/>
+    <mergeCell ref="B936:F936"/>
+    <mergeCell ref="B961:F961"/>
+    <mergeCell ref="B962:F962"/>
+    <mergeCell ref="B963:F963"/>
+    <mergeCell ref="B964:F964"/>
+    <mergeCell ref="B965:F965"/>
+    <mergeCell ref="B966:F966"/>
+    <mergeCell ref="B955:F955"/>
+    <mergeCell ref="B956:F956"/>
+    <mergeCell ref="B957:F957"/>
+    <mergeCell ref="B958:F958"/>
+    <mergeCell ref="B959:F959"/>
+    <mergeCell ref="B960:F960"/>
+    <mergeCell ref="B949:F949"/>
+    <mergeCell ref="B950:F950"/>
+    <mergeCell ref="B951:F951"/>
+    <mergeCell ref="B952:F952"/>
+    <mergeCell ref="B953:F953"/>
+    <mergeCell ref="B954:F954"/>
+    <mergeCell ref="B979:F979"/>
+    <mergeCell ref="B980:F980"/>
+    <mergeCell ref="B981:F981"/>
+    <mergeCell ref="B982:F982"/>
+    <mergeCell ref="B983:F983"/>
+    <mergeCell ref="B984:F984"/>
+    <mergeCell ref="B973:F973"/>
+    <mergeCell ref="B974:F974"/>
+    <mergeCell ref="B975:F975"/>
+    <mergeCell ref="B976:F976"/>
+    <mergeCell ref="B977:F977"/>
+    <mergeCell ref="B978:F978"/>
+    <mergeCell ref="B967:F967"/>
+    <mergeCell ref="B968:F968"/>
+    <mergeCell ref="B969:F969"/>
+    <mergeCell ref="B970:F970"/>
+    <mergeCell ref="B971:F971"/>
+    <mergeCell ref="B972:F972"/>
+    <mergeCell ref="B997:F997"/>
+    <mergeCell ref="B998:F998"/>
+    <mergeCell ref="B999:F999"/>
+    <mergeCell ref="B1000:F1000"/>
+    <mergeCell ref="B1001:F1001"/>
+    <mergeCell ref="B1002:F1002"/>
+    <mergeCell ref="B991:F991"/>
+    <mergeCell ref="B992:F992"/>
+    <mergeCell ref="B993:F993"/>
+    <mergeCell ref="B994:F994"/>
+    <mergeCell ref="B995:F995"/>
+    <mergeCell ref="B996:F996"/>
+    <mergeCell ref="B985:F985"/>
+    <mergeCell ref="B986:F986"/>
+    <mergeCell ref="B987:F987"/>
+    <mergeCell ref="B988:F988"/>
+    <mergeCell ref="B989:F989"/>
+    <mergeCell ref="B990:F990"/>
+    <mergeCell ref="B1015:F1015"/>
+    <mergeCell ref="B1016:F1016"/>
+    <mergeCell ref="B1017:F1017"/>
+    <mergeCell ref="B1018:F1018"/>
+    <mergeCell ref="B1019:F1019"/>
+    <mergeCell ref="B1020:F1020"/>
+    <mergeCell ref="B1009:F1009"/>
+    <mergeCell ref="B1010:F1010"/>
+    <mergeCell ref="B1011:F1011"/>
+    <mergeCell ref="B1012:F1012"/>
+    <mergeCell ref="B1013:F1013"/>
+    <mergeCell ref="B1014:F1014"/>
+    <mergeCell ref="B1003:F1003"/>
+    <mergeCell ref="B1004:F1004"/>
+    <mergeCell ref="B1005:F1005"/>
+    <mergeCell ref="B1006:F1006"/>
+    <mergeCell ref="B1007:F1007"/>
+    <mergeCell ref="B1008:F1008"/>
+    <mergeCell ref="B1033:F1033"/>
+    <mergeCell ref="B1034:F1034"/>
+    <mergeCell ref="B1035:F1035"/>
+    <mergeCell ref="B1036:F1036"/>
+    <mergeCell ref="B1037:F1037"/>
+    <mergeCell ref="B1038:F1038"/>
+    <mergeCell ref="B1027:F1027"/>
+    <mergeCell ref="B1028:F1028"/>
+    <mergeCell ref="B1029:F1029"/>
+    <mergeCell ref="B1030:F1030"/>
+    <mergeCell ref="B1031:F1031"/>
+    <mergeCell ref="B1032:F1032"/>
+    <mergeCell ref="B1021:F1021"/>
+    <mergeCell ref="B1022:F1022"/>
+    <mergeCell ref="B1023:F1023"/>
+    <mergeCell ref="B1024:F1024"/>
+    <mergeCell ref="B1025:F1025"/>
+    <mergeCell ref="B1026:F1026"/>
+    <mergeCell ref="B1051:F1051"/>
+    <mergeCell ref="B1052:F1052"/>
+    <mergeCell ref="B1053:F1053"/>
+    <mergeCell ref="B1054:F1054"/>
+    <mergeCell ref="B1055:F1055"/>
+    <mergeCell ref="B1056:F1056"/>
+    <mergeCell ref="B1045:F1045"/>
+    <mergeCell ref="B1046:F1046"/>
+    <mergeCell ref="B1047:F1047"/>
+    <mergeCell ref="B1048:F1048"/>
+    <mergeCell ref="B1049:F1049"/>
+    <mergeCell ref="B1050:F1050"/>
+    <mergeCell ref="B1039:F1039"/>
+    <mergeCell ref="B1040:F1040"/>
+    <mergeCell ref="B1041:F1041"/>
+    <mergeCell ref="B1042:F1042"/>
+    <mergeCell ref="B1043:F1043"/>
+    <mergeCell ref="B1044:F1044"/>
+    <mergeCell ref="B1069:F1069"/>
+    <mergeCell ref="B1070:F1070"/>
+    <mergeCell ref="B1071:F1071"/>
+    <mergeCell ref="B1072:F1072"/>
+    <mergeCell ref="B1073:F1073"/>
+    <mergeCell ref="B1074:F1074"/>
+    <mergeCell ref="B1063:F1063"/>
+    <mergeCell ref="B1064:F1064"/>
+    <mergeCell ref="B1065:F1065"/>
+    <mergeCell ref="B1066:F1066"/>
+    <mergeCell ref="B1067:F1067"/>
+    <mergeCell ref="B1068:F1068"/>
+    <mergeCell ref="B1057:F1057"/>
+    <mergeCell ref="B1058:F1058"/>
+    <mergeCell ref="B1059:F1059"/>
+    <mergeCell ref="B1060:F1060"/>
+    <mergeCell ref="B1061:F1061"/>
+    <mergeCell ref="B1062:F1062"/>
+    <mergeCell ref="B1087:F1087"/>
+    <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1089:F1089"/>
+    <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1091:F1091"/>
+    <mergeCell ref="B1092:F1092"/>
+    <mergeCell ref="B1081:F1081"/>
+    <mergeCell ref="B1082:F1082"/>
+    <mergeCell ref="B1083:F1083"/>
+    <mergeCell ref="B1084:F1084"/>
+    <mergeCell ref="B1085:F1085"/>
+    <mergeCell ref="B1086:F1086"/>
+    <mergeCell ref="B1075:F1075"/>
+    <mergeCell ref="B1076:F1076"/>
+    <mergeCell ref="B1077:F1077"/>
+    <mergeCell ref="B1078:F1078"/>
+    <mergeCell ref="B1079:F1079"/>
+    <mergeCell ref="B1080:F1080"/>
+    <mergeCell ref="B1105:F1105"/>
+    <mergeCell ref="B1106:F1106"/>
+    <mergeCell ref="B1107:F1107"/>
+    <mergeCell ref="B1108:F1108"/>
+    <mergeCell ref="B1109:F1109"/>
+    <mergeCell ref="B1110:F1110"/>
+    <mergeCell ref="B1099:F1099"/>
+    <mergeCell ref="B1100:F1100"/>
+    <mergeCell ref="B1101:F1101"/>
+    <mergeCell ref="B1102:F1102"/>
+    <mergeCell ref="B1103:F1103"/>
+    <mergeCell ref="B1104:F1104"/>
+    <mergeCell ref="B1093:F1093"/>
+    <mergeCell ref="B1094:F1094"/>
+    <mergeCell ref="B1095:F1095"/>
+    <mergeCell ref="B1096:F1096"/>
+    <mergeCell ref="B1097:F1097"/>
+    <mergeCell ref="B1098:F1098"/>
+    <mergeCell ref="B1123:F1123"/>
+    <mergeCell ref="B1124:F1124"/>
+    <mergeCell ref="B1125:F1125"/>
+    <mergeCell ref="B1126:F1126"/>
+    <mergeCell ref="B1127:F1127"/>
+    <mergeCell ref="B1128:F1128"/>
+    <mergeCell ref="B1117:F1117"/>
+    <mergeCell ref="B1118:F1118"/>
+    <mergeCell ref="B1119:F1119"/>
+    <mergeCell ref="B1120:F1120"/>
+    <mergeCell ref="B1121:F1121"/>
+    <mergeCell ref="B1122:F1122"/>
+    <mergeCell ref="B1111:F1111"/>
+    <mergeCell ref="B1112:F1112"/>
+    <mergeCell ref="B1113:F1113"/>
+    <mergeCell ref="B1114:F1114"/>
+    <mergeCell ref="B1115:F1115"/>
+    <mergeCell ref="B1116:F1116"/>
+    <mergeCell ref="B1141:F1141"/>
+    <mergeCell ref="B1142:F1142"/>
+    <mergeCell ref="B1143:F1143"/>
+    <mergeCell ref="B1144:F1144"/>
+    <mergeCell ref="B1145:F1145"/>
+    <mergeCell ref="B1146:F1146"/>
+    <mergeCell ref="B1135:F1135"/>
+    <mergeCell ref="B1136:F1136"/>
+    <mergeCell ref="B1137:F1137"/>
+    <mergeCell ref="B1138:F1138"/>
+    <mergeCell ref="B1139:F1139"/>
+    <mergeCell ref="B1140:F1140"/>
+    <mergeCell ref="B1129:F1129"/>
+    <mergeCell ref="B1130:F1130"/>
+    <mergeCell ref="B1131:F1131"/>
+    <mergeCell ref="B1132:F1132"/>
+    <mergeCell ref="B1133:F1133"/>
+    <mergeCell ref="B1134:F1134"/>
+    <mergeCell ref="B1159:F1159"/>
+    <mergeCell ref="B1160:F1160"/>
+    <mergeCell ref="B1161:F1161"/>
+    <mergeCell ref="B1162:F1162"/>
+    <mergeCell ref="B1163:F1163"/>
+    <mergeCell ref="B1164:F1164"/>
+    <mergeCell ref="B1153:F1153"/>
+    <mergeCell ref="B1154:F1154"/>
+    <mergeCell ref="B1155:F1155"/>
+    <mergeCell ref="B1156:F1156"/>
+    <mergeCell ref="B1157:F1157"/>
+    <mergeCell ref="B1158:F1158"/>
+    <mergeCell ref="B1147:F1147"/>
+    <mergeCell ref="B1148:F1148"/>
+    <mergeCell ref="B1149:F1149"/>
+    <mergeCell ref="B1150:F1150"/>
+    <mergeCell ref="B1151:F1151"/>
+    <mergeCell ref="B1152:F1152"/>
+    <mergeCell ref="B1177:F1177"/>
+    <mergeCell ref="B1178:F1178"/>
+    <mergeCell ref="B1179:F1179"/>
+    <mergeCell ref="B1180:F1180"/>
+    <mergeCell ref="B1181:F1181"/>
+    <mergeCell ref="B1182:F1182"/>
+    <mergeCell ref="B1171:F1171"/>
+    <mergeCell ref="B1172:F1172"/>
+    <mergeCell ref="B1173:F1173"/>
+    <mergeCell ref="B1174:F1174"/>
+    <mergeCell ref="B1175:F1175"/>
+    <mergeCell ref="B1176:F1176"/>
+    <mergeCell ref="B1165:F1165"/>
+    <mergeCell ref="B1166:F1166"/>
+    <mergeCell ref="B1167:F1167"/>
+    <mergeCell ref="B1168:F1168"/>
+    <mergeCell ref="B1169:F1169"/>
+    <mergeCell ref="B1170:F1170"/>
+    <mergeCell ref="B1195:F1195"/>
+    <mergeCell ref="B1196:F1196"/>
+    <mergeCell ref="B1197:F1197"/>
+    <mergeCell ref="B1198:F1198"/>
+    <mergeCell ref="B1199:F1199"/>
+    <mergeCell ref="B1200:F1200"/>
+    <mergeCell ref="B1189:F1189"/>
+    <mergeCell ref="B1190:F1190"/>
+    <mergeCell ref="B1191:F1191"/>
+    <mergeCell ref="B1192:F1192"/>
+    <mergeCell ref="B1193:F1193"/>
+    <mergeCell ref="B1194:F1194"/>
+    <mergeCell ref="B1183:F1183"/>
+    <mergeCell ref="B1184:F1184"/>
+    <mergeCell ref="B1185:F1185"/>
+    <mergeCell ref="B1186:F1186"/>
+    <mergeCell ref="B1187:F1187"/>
+    <mergeCell ref="B1188:F1188"/>
+    <mergeCell ref="B1213:F1213"/>
+    <mergeCell ref="B1214:F1214"/>
+    <mergeCell ref="B1215:F1215"/>
+    <mergeCell ref="B1216:F1216"/>
+    <mergeCell ref="B1217:F1217"/>
+    <mergeCell ref="B1218:F1218"/>
+    <mergeCell ref="B1207:F1207"/>
+    <mergeCell ref="B1208:F1208"/>
+    <mergeCell ref="B1209:F1209"/>
+    <mergeCell ref="B1210:F1210"/>
+    <mergeCell ref="B1211:F1211"/>
+    <mergeCell ref="B1212:F1212"/>
+    <mergeCell ref="B1201:F1201"/>
+    <mergeCell ref="B1202:F1202"/>
+    <mergeCell ref="B1203:F1203"/>
+    <mergeCell ref="B1204:F1204"/>
+    <mergeCell ref="B1205:F1205"/>
+    <mergeCell ref="B1206:F1206"/>
+    <mergeCell ref="B1231:F1231"/>
+    <mergeCell ref="B1232:F1232"/>
+    <mergeCell ref="B1233:F1233"/>
+    <mergeCell ref="B1234:F1234"/>
+    <mergeCell ref="B1235:F1235"/>
+    <mergeCell ref="B1236:F1236"/>
+    <mergeCell ref="B1225:F1225"/>
+    <mergeCell ref="B1226:F1226"/>
+    <mergeCell ref="B1227:F1227"/>
+    <mergeCell ref="B1228:F1228"/>
+    <mergeCell ref="B1229:F1229"/>
+    <mergeCell ref="B1230:F1230"/>
+    <mergeCell ref="B1219:F1219"/>
+    <mergeCell ref="B1220:F1220"/>
+    <mergeCell ref="B1221:F1221"/>
+    <mergeCell ref="B1222:F1222"/>
+    <mergeCell ref="B1223:F1223"/>
+    <mergeCell ref="B1224:F1224"/>
+    <mergeCell ref="B1249:F1249"/>
+    <mergeCell ref="B1250:F1250"/>
+    <mergeCell ref="B1251:F1251"/>
+    <mergeCell ref="B1252:F1252"/>
+    <mergeCell ref="B1253:F1253"/>
+    <mergeCell ref="B1254:F1254"/>
+    <mergeCell ref="B1243:F1243"/>
+    <mergeCell ref="B1244:F1244"/>
+    <mergeCell ref="B1245:F1245"/>
+    <mergeCell ref="B1246:F1246"/>
+    <mergeCell ref="B1247:F1247"/>
+    <mergeCell ref="B1248:F1248"/>
+    <mergeCell ref="B1237:F1237"/>
+    <mergeCell ref="B1238:F1238"/>
+    <mergeCell ref="B1239:F1239"/>
+    <mergeCell ref="B1240:F1240"/>
+    <mergeCell ref="B1241:F1241"/>
+    <mergeCell ref="B1242:F1242"/>
+    <mergeCell ref="B1267:F1267"/>
+    <mergeCell ref="B1268:F1268"/>
+    <mergeCell ref="B1269:F1269"/>
+    <mergeCell ref="B1270:F1270"/>
+    <mergeCell ref="B1271:F1271"/>
+    <mergeCell ref="B1272:F1272"/>
+    <mergeCell ref="B1261:F1261"/>
+    <mergeCell ref="B1262:F1262"/>
+    <mergeCell ref="B1263:F1263"/>
+    <mergeCell ref="B1264:F1264"/>
+    <mergeCell ref="B1265:F1265"/>
+    <mergeCell ref="B1266:F1266"/>
+    <mergeCell ref="B1255:F1255"/>
+    <mergeCell ref="B1256:F1256"/>
+    <mergeCell ref="B1257:F1257"/>
+    <mergeCell ref="B1258:F1258"/>
+    <mergeCell ref="B1259:F1259"/>
+    <mergeCell ref="B1260:F1260"/>
+    <mergeCell ref="B1285:F1285"/>
+    <mergeCell ref="B1286:F1286"/>
+    <mergeCell ref="B1287:F1287"/>
+    <mergeCell ref="B1288:F1288"/>
+    <mergeCell ref="B1289:F1289"/>
+    <mergeCell ref="B1290:F1290"/>
+    <mergeCell ref="B1279:F1279"/>
+    <mergeCell ref="B1280:F1280"/>
+    <mergeCell ref="B1281:F1281"/>
+    <mergeCell ref="B1282:F1282"/>
+    <mergeCell ref="B1283:F1283"/>
+    <mergeCell ref="B1284:F1284"/>
+    <mergeCell ref="B1273:F1273"/>
+    <mergeCell ref="B1274:F1274"/>
+    <mergeCell ref="B1275:F1275"/>
+    <mergeCell ref="B1276:F1276"/>
+    <mergeCell ref="B1277:F1277"/>
+    <mergeCell ref="B1278:F1278"/>
+    <mergeCell ref="B1303:F1303"/>
+    <mergeCell ref="B1304:F1304"/>
+    <mergeCell ref="B1305:F1305"/>
+    <mergeCell ref="B1306:F1306"/>
+    <mergeCell ref="B1307:F1307"/>
+    <mergeCell ref="B1308:F1308"/>
+    <mergeCell ref="B1297:F1297"/>
+    <mergeCell ref="B1298:F1298"/>
+    <mergeCell ref="B1299:F1299"/>
+    <mergeCell ref="B1300:F1300"/>
+    <mergeCell ref="B1301:F1301"/>
+    <mergeCell ref="B1302:F1302"/>
+    <mergeCell ref="B1291:F1291"/>
+    <mergeCell ref="B1292:F1292"/>
+    <mergeCell ref="B1293:F1293"/>
+    <mergeCell ref="B1294:F1294"/>
+    <mergeCell ref="B1295:F1295"/>
+    <mergeCell ref="B1296:F1296"/>
+    <mergeCell ref="B1321:F1321"/>
+    <mergeCell ref="B1322:F1322"/>
+    <mergeCell ref="B1323:F1323"/>
+    <mergeCell ref="B1324:F1324"/>
+    <mergeCell ref="B1325:F1325"/>
+    <mergeCell ref="B1326:F1326"/>
+    <mergeCell ref="B1315:F1315"/>
+    <mergeCell ref="B1316:F1316"/>
+    <mergeCell ref="B1317:F1317"/>
+    <mergeCell ref="B1318:F1318"/>
+    <mergeCell ref="B1319:F1319"/>
+    <mergeCell ref="B1320:F1320"/>
+    <mergeCell ref="B1309:F1309"/>
+    <mergeCell ref="B1310:F1310"/>
+    <mergeCell ref="B1311:F1311"/>
+    <mergeCell ref="B1312:F1312"/>
+    <mergeCell ref="B1313:F1313"/>
+    <mergeCell ref="B1314:F1314"/>
+    <mergeCell ref="B1339:F1339"/>
+    <mergeCell ref="B1340:F1340"/>
+    <mergeCell ref="B1341:F1341"/>
+    <mergeCell ref="B1342:F1342"/>
+    <mergeCell ref="B1343:F1343"/>
+    <mergeCell ref="B1344:F1344"/>
+    <mergeCell ref="B1333:F1333"/>
+    <mergeCell ref="B1334:F1334"/>
+    <mergeCell ref="B1335:F1335"/>
+    <mergeCell ref="B1336:F1336"/>
+    <mergeCell ref="B1337:F1337"/>
+    <mergeCell ref="B1338:F1338"/>
+    <mergeCell ref="B1327:F1327"/>
+    <mergeCell ref="B1328:F1328"/>
+    <mergeCell ref="B1329:F1329"/>
+    <mergeCell ref="B1330:F1330"/>
+    <mergeCell ref="B1331:F1331"/>
+    <mergeCell ref="B1332:F1332"/>
+    <mergeCell ref="B1357:F1357"/>
+    <mergeCell ref="B1358:F1358"/>
+    <mergeCell ref="B1359:F1359"/>
+    <mergeCell ref="B1360:F1360"/>
+    <mergeCell ref="B1361:F1361"/>
+    <mergeCell ref="B1362:F1362"/>
+    <mergeCell ref="B1351:F1351"/>
+    <mergeCell ref="B1352:F1352"/>
+    <mergeCell ref="B1353:F1353"/>
+    <mergeCell ref="B1354:F1354"/>
+    <mergeCell ref="B1355:F1355"/>
+    <mergeCell ref="B1356:F1356"/>
+    <mergeCell ref="B1345:F1345"/>
+    <mergeCell ref="B1346:F1346"/>
+    <mergeCell ref="B1347:F1347"/>
+    <mergeCell ref="B1348:F1348"/>
+    <mergeCell ref="B1349:F1349"/>
+    <mergeCell ref="B1350:F1350"/>
+    <mergeCell ref="B1375:F1375"/>
+    <mergeCell ref="B1376:F1376"/>
+    <mergeCell ref="B1377:F1377"/>
+    <mergeCell ref="B1378:F1378"/>
+    <mergeCell ref="B1379:F1379"/>
+    <mergeCell ref="B1380:F1380"/>
+    <mergeCell ref="B1369:F1369"/>
+    <mergeCell ref="B1370:F1370"/>
+    <mergeCell ref="B1371:F1371"/>
+    <mergeCell ref="B1372:F1372"/>
+    <mergeCell ref="B1373:F1373"/>
+    <mergeCell ref="B1374:F1374"/>
+    <mergeCell ref="B1363:F1363"/>
+    <mergeCell ref="B1364:F1364"/>
+    <mergeCell ref="B1365:F1365"/>
+    <mergeCell ref="B1366:F1366"/>
+    <mergeCell ref="B1367:F1367"/>
+    <mergeCell ref="B1368:F1368"/>
+    <mergeCell ref="B1393:F1393"/>
+    <mergeCell ref="B1394:F1394"/>
+    <mergeCell ref="B1395:F1395"/>
+    <mergeCell ref="B1396:F1396"/>
+    <mergeCell ref="B1397:F1397"/>
+    <mergeCell ref="B1398:F1398"/>
+    <mergeCell ref="B1387:F1387"/>
+    <mergeCell ref="B1388:F1388"/>
+    <mergeCell ref="B1389:F1389"/>
+    <mergeCell ref="B1390:F1390"/>
+    <mergeCell ref="B1391:F1391"/>
+    <mergeCell ref="B1392:F1392"/>
+    <mergeCell ref="B1381:F1381"/>
+    <mergeCell ref="B1382:F1382"/>
+    <mergeCell ref="B1383:F1383"/>
+    <mergeCell ref="B1384:F1384"/>
+    <mergeCell ref="B1385:F1385"/>
+    <mergeCell ref="B1386:F1386"/>
+    <mergeCell ref="B1411:F1411"/>
+    <mergeCell ref="B1412:F1412"/>
+    <mergeCell ref="B1413:F1413"/>
+    <mergeCell ref="B1414:F1414"/>
+    <mergeCell ref="B1415:F1415"/>
+    <mergeCell ref="B1416:F1416"/>
+    <mergeCell ref="B1405:F1405"/>
+    <mergeCell ref="B1406:F1406"/>
+    <mergeCell ref="B1407:F1407"/>
+    <mergeCell ref="B1408:F1408"/>
+    <mergeCell ref="B1409:F1409"/>
+    <mergeCell ref="B1410:F1410"/>
+    <mergeCell ref="B1399:F1399"/>
+    <mergeCell ref="B1400:F1400"/>
+    <mergeCell ref="B1401:F1401"/>
+    <mergeCell ref="B1402:F1402"/>
+    <mergeCell ref="B1403:F1403"/>
+    <mergeCell ref="B1404:F1404"/>
+    <mergeCell ref="B1429:F1429"/>
+    <mergeCell ref="B1430:F1430"/>
+    <mergeCell ref="B1431:F1431"/>
+    <mergeCell ref="B1432:F1432"/>
+    <mergeCell ref="B1433:F1433"/>
+    <mergeCell ref="B1434:F1434"/>
+    <mergeCell ref="B1423:F1423"/>
+    <mergeCell ref="B1424:F1424"/>
+    <mergeCell ref="B1425:F1425"/>
+    <mergeCell ref="B1426:F1426"/>
+    <mergeCell ref="B1427:F1427"/>
+    <mergeCell ref="B1428:F1428"/>
+    <mergeCell ref="B1417:F1417"/>
+    <mergeCell ref="B1418:F1418"/>
+    <mergeCell ref="B1419:F1419"/>
+    <mergeCell ref="B1420:F1420"/>
+    <mergeCell ref="B1421:F1421"/>
+    <mergeCell ref="B1422:F1422"/>
+    <mergeCell ref="B1447:F1447"/>
+    <mergeCell ref="B1448:F1448"/>
+    <mergeCell ref="B1449:F1449"/>
+    <mergeCell ref="B1450:F1450"/>
+    <mergeCell ref="B1451:F1451"/>
+    <mergeCell ref="B1452:F1452"/>
+    <mergeCell ref="B1441:F1441"/>
+    <mergeCell ref="B1442:F1442"/>
+    <mergeCell ref="B1443:F1443"/>
+    <mergeCell ref="B1444:F1444"/>
+    <mergeCell ref="B1445:F1445"/>
+    <mergeCell ref="B1446:F1446"/>
+    <mergeCell ref="B1435:F1435"/>
+    <mergeCell ref="B1436:F1436"/>
+    <mergeCell ref="B1437:F1437"/>
+    <mergeCell ref="B1438:F1438"/>
+    <mergeCell ref="B1439:F1439"/>
+    <mergeCell ref="B1440:F1440"/>
+    <mergeCell ref="B1465:F1465"/>
+    <mergeCell ref="B1466:F1466"/>
+    <mergeCell ref="B1467:F1467"/>
+    <mergeCell ref="B1468:F1468"/>
+    <mergeCell ref="B1469:F1469"/>
+    <mergeCell ref="B1470:F1470"/>
+    <mergeCell ref="B1459:F1459"/>
+    <mergeCell ref="B1460:F1460"/>
+    <mergeCell ref="B1461:F1461"/>
+    <mergeCell ref="B1462:F1462"/>
+    <mergeCell ref="B1463:F1463"/>
+    <mergeCell ref="B1464:F1464"/>
+    <mergeCell ref="B1453:F1453"/>
+    <mergeCell ref="B1454:F1454"/>
+    <mergeCell ref="B1455:F1455"/>
+    <mergeCell ref="B1456:F1456"/>
+    <mergeCell ref="B1457:F1457"/>
+    <mergeCell ref="B1458:F1458"/>
+    <mergeCell ref="B1483:F1483"/>
+    <mergeCell ref="B1484:F1484"/>
+    <mergeCell ref="B1485:F1485"/>
+    <mergeCell ref="B1486:F1486"/>
+    <mergeCell ref="B1487:F1487"/>
+    <mergeCell ref="B1488:F1488"/>
+    <mergeCell ref="B1477:F1477"/>
+    <mergeCell ref="B1478:F1478"/>
+    <mergeCell ref="B1479:F1479"/>
+    <mergeCell ref="B1480:F1480"/>
+    <mergeCell ref="B1481:F1481"/>
+    <mergeCell ref="B1482:F1482"/>
+    <mergeCell ref="B1471:F1471"/>
+    <mergeCell ref="B1472:F1472"/>
+    <mergeCell ref="B1473:F1473"/>
+    <mergeCell ref="B1474:F1474"/>
+    <mergeCell ref="B1475:F1475"/>
+    <mergeCell ref="B1476:F1476"/>
+    <mergeCell ref="B1501:F1501"/>
+    <mergeCell ref="B1502:F1502"/>
+    <mergeCell ref="B1503:F1503"/>
+    <mergeCell ref="B1504:F1504"/>
+    <mergeCell ref="B1505:F1505"/>
+    <mergeCell ref="B1506:F1506"/>
+    <mergeCell ref="B1495:F1495"/>
+    <mergeCell ref="B1496:F1496"/>
+    <mergeCell ref="B1497:F1497"/>
+    <mergeCell ref="B1498:F1498"/>
+    <mergeCell ref="B1499:F1499"/>
+    <mergeCell ref="B1500:F1500"/>
+    <mergeCell ref="B1489:F1489"/>
+    <mergeCell ref="B1490:F1490"/>
+    <mergeCell ref="B1491:F1491"/>
+    <mergeCell ref="B1492:F1492"/>
+    <mergeCell ref="B1493:F1493"/>
+    <mergeCell ref="B1494:F1494"/>
+    <mergeCell ref="B1519:F1519"/>
+    <mergeCell ref="B1520:F1520"/>
+    <mergeCell ref="B1521:F1521"/>
+    <mergeCell ref="B1522:F1522"/>
+    <mergeCell ref="B1523:F1523"/>
+    <mergeCell ref="B1524:F1524"/>
+    <mergeCell ref="B1513:F1513"/>
+    <mergeCell ref="B1514:F1514"/>
+    <mergeCell ref="B1515:F1515"/>
+    <mergeCell ref="B1516:F1516"/>
+    <mergeCell ref="B1517:F1517"/>
+    <mergeCell ref="B1518:F1518"/>
+    <mergeCell ref="B1507:F1507"/>
+    <mergeCell ref="B1508:F1508"/>
+    <mergeCell ref="B1509:F1509"/>
+    <mergeCell ref="B1510:F1510"/>
+    <mergeCell ref="B1511:F1511"/>
+    <mergeCell ref="B1512:F1512"/>
+    <mergeCell ref="B1537:F1537"/>
+    <mergeCell ref="B1538:F1538"/>
+    <mergeCell ref="B1539:F1539"/>
+    <mergeCell ref="B1540:F1540"/>
+    <mergeCell ref="B1541:F1541"/>
+    <mergeCell ref="B1542:F1542"/>
+    <mergeCell ref="B1531:F1531"/>
+    <mergeCell ref="B1532:F1532"/>
+    <mergeCell ref="B1533:F1533"/>
+    <mergeCell ref="B1534:F1534"/>
+    <mergeCell ref="B1535:F1535"/>
+    <mergeCell ref="B1536:F1536"/>
+    <mergeCell ref="B1525:F1525"/>
+    <mergeCell ref="B1526:F1526"/>
+    <mergeCell ref="B1527:F1527"/>
+    <mergeCell ref="B1528:F1528"/>
+    <mergeCell ref="B1529:F1529"/>
+    <mergeCell ref="B1530:F1530"/>
+    <mergeCell ref="B1555:F1555"/>
+    <mergeCell ref="B1556:F1556"/>
+    <mergeCell ref="B1557:F1557"/>
+    <mergeCell ref="B1558:F1558"/>
+    <mergeCell ref="B1559:F1559"/>
+    <mergeCell ref="B1560:F1560"/>
+    <mergeCell ref="B1549:F1549"/>
+    <mergeCell ref="B1550:F1550"/>
+    <mergeCell ref="B1551:F1551"/>
+    <mergeCell ref="B1552:F1552"/>
+    <mergeCell ref="B1553:F1553"/>
+    <mergeCell ref="B1554:F1554"/>
+    <mergeCell ref="B1543:F1543"/>
+    <mergeCell ref="B1544:F1544"/>
+    <mergeCell ref="B1545:F1545"/>
+    <mergeCell ref="B1546:F1546"/>
+    <mergeCell ref="B1547:F1547"/>
+    <mergeCell ref="B1548:F1548"/>
+    <mergeCell ref="B1573:F1573"/>
+    <mergeCell ref="B1574:F1574"/>
+    <mergeCell ref="B1575:F1575"/>
+    <mergeCell ref="B1576:F1576"/>
+    <mergeCell ref="B1577:F1577"/>
+    <mergeCell ref="B1578:F1578"/>
+    <mergeCell ref="B1567:F1567"/>
+    <mergeCell ref="B1568:F1568"/>
+    <mergeCell ref="B1569:F1569"/>
+    <mergeCell ref="B1570:F1570"/>
+    <mergeCell ref="B1571:F1571"/>
+    <mergeCell ref="B1572:F1572"/>
+    <mergeCell ref="B1561:F1561"/>
+    <mergeCell ref="B1562:F1562"/>
+    <mergeCell ref="B1563:F1563"/>
+    <mergeCell ref="B1564:F1564"/>
+    <mergeCell ref="B1565:F1565"/>
+    <mergeCell ref="B1566:F1566"/>
+    <mergeCell ref="B1591:F1591"/>
+    <mergeCell ref="B1592:F1592"/>
+    <mergeCell ref="B1593:F1593"/>
+    <mergeCell ref="B1594:F1594"/>
+    <mergeCell ref="B1595:F1595"/>
+    <mergeCell ref="B1596:F1596"/>
+    <mergeCell ref="B1585:F1585"/>
+    <mergeCell ref="B1586:F1586"/>
+    <mergeCell ref="B1587:F1587"/>
+    <mergeCell ref="B1588:F1588"/>
+    <mergeCell ref="B1589:F1589"/>
+    <mergeCell ref="B1590:F1590"/>
+    <mergeCell ref="B1579:F1579"/>
+    <mergeCell ref="B1580:F1580"/>
+    <mergeCell ref="B1581:F1581"/>
+    <mergeCell ref="B1582:F1582"/>
+    <mergeCell ref="B1583:F1583"/>
+    <mergeCell ref="B1584:F1584"/>
+    <mergeCell ref="B1609:F1609"/>
+    <mergeCell ref="B1610:F1610"/>
+    <mergeCell ref="B1611:F1611"/>
+    <mergeCell ref="B1612:F1612"/>
+    <mergeCell ref="B1613:F1613"/>
+    <mergeCell ref="B1614:F1614"/>
+    <mergeCell ref="B1603:F1603"/>
+    <mergeCell ref="B1604:F1604"/>
+    <mergeCell ref="B1605:F1605"/>
+    <mergeCell ref="B1606:F1606"/>
+    <mergeCell ref="B1607:F1607"/>
+    <mergeCell ref="B1608:F1608"/>
+    <mergeCell ref="B1597:F1597"/>
+    <mergeCell ref="B1598:F1598"/>
+    <mergeCell ref="B1599:F1599"/>
+    <mergeCell ref="B1600:F1600"/>
+    <mergeCell ref="B1601:F1601"/>
+    <mergeCell ref="B1602:F1602"/>
+    <mergeCell ref="B1627:F1627"/>
+    <mergeCell ref="B1628:F1628"/>
+    <mergeCell ref="B1629:F1629"/>
+    <mergeCell ref="B1630:F1630"/>
+    <mergeCell ref="B1631:F1631"/>
+    <mergeCell ref="B1632:F1632"/>
+    <mergeCell ref="B1621:F1621"/>
+    <mergeCell ref="B1622:F1622"/>
+    <mergeCell ref="B1623:F1623"/>
+    <mergeCell ref="B1624:F1624"/>
+    <mergeCell ref="B1625:F1625"/>
+    <mergeCell ref="B1626:F1626"/>
+    <mergeCell ref="B1615:F1615"/>
+    <mergeCell ref="B1616:F1616"/>
+    <mergeCell ref="B1617:F1617"/>
+    <mergeCell ref="B1618:F1618"/>
+    <mergeCell ref="B1619:F1619"/>
+    <mergeCell ref="B1620:F1620"/>
+    <mergeCell ref="B1645:F1645"/>
+    <mergeCell ref="B1646:F1646"/>
+    <mergeCell ref="B1647:F1647"/>
+    <mergeCell ref="B1648:F1648"/>
+    <mergeCell ref="B1649:F1649"/>
+    <mergeCell ref="B1650:F1650"/>
+    <mergeCell ref="B1639:F1639"/>
+    <mergeCell ref="B1640:F1640"/>
+    <mergeCell ref="B1641:F1641"/>
+    <mergeCell ref="B1642:F1642"/>
+    <mergeCell ref="B1643:F1643"/>
+    <mergeCell ref="B1644:F1644"/>
+    <mergeCell ref="B1633:F1633"/>
+    <mergeCell ref="B1634:F1634"/>
+    <mergeCell ref="B1635:F1635"/>
+    <mergeCell ref="B1636:F1636"/>
+    <mergeCell ref="B1637:F1637"/>
+    <mergeCell ref="B1638:F1638"/>
+    <mergeCell ref="B1663:F1663"/>
+    <mergeCell ref="B1664:F1664"/>
+    <mergeCell ref="B1665:F1665"/>
+    <mergeCell ref="B1666:F1666"/>
+    <mergeCell ref="B1667:F1667"/>
+    <mergeCell ref="B1668:F1668"/>
+    <mergeCell ref="B1657:F1657"/>
+    <mergeCell ref="B1658:F1658"/>
+    <mergeCell ref="B1659:F1659"/>
+    <mergeCell ref="B1660:F1660"/>
+    <mergeCell ref="B1661:F1661"/>
+    <mergeCell ref="B1662:F1662"/>
+    <mergeCell ref="B1651:F1651"/>
+    <mergeCell ref="B1652:F1652"/>
+    <mergeCell ref="B1653:F1653"/>
+    <mergeCell ref="B1654:F1654"/>
+    <mergeCell ref="B1655:F1655"/>
+    <mergeCell ref="B1656:F1656"/>
+    <mergeCell ref="B1681:F1681"/>
+    <mergeCell ref="B1682:F1682"/>
+    <mergeCell ref="B1683:F1683"/>
+    <mergeCell ref="B1684:F1684"/>
+    <mergeCell ref="B1685:F1685"/>
+    <mergeCell ref="B1686:F1686"/>
+    <mergeCell ref="B1675:F1675"/>
+    <mergeCell ref="B1676:F1676"/>
+    <mergeCell ref="B1677:F1677"/>
+    <mergeCell ref="B1678:F1678"/>
+    <mergeCell ref="B1679:F1679"/>
+    <mergeCell ref="B1680:F1680"/>
+    <mergeCell ref="B1669:F1669"/>
+    <mergeCell ref="B1670:F1670"/>
+    <mergeCell ref="B1671:F1671"/>
+    <mergeCell ref="B1672:F1672"/>
+    <mergeCell ref="B1673:F1673"/>
+    <mergeCell ref="B1674:F1674"/>
+    <mergeCell ref="B1699:F1699"/>
+    <mergeCell ref="B1700:F1700"/>
+    <mergeCell ref="B1701:F1701"/>
+    <mergeCell ref="B1702:F1702"/>
+    <mergeCell ref="B1703:F1703"/>
+    <mergeCell ref="B1704:F1704"/>
+    <mergeCell ref="B1693:F1693"/>
+    <mergeCell ref="B1694:F1694"/>
+    <mergeCell ref="B1695:F1695"/>
+    <mergeCell ref="B1696:F1696"/>
+    <mergeCell ref="B1697:F1697"/>
+    <mergeCell ref="B1698:F1698"/>
+    <mergeCell ref="B1687:F1687"/>
+    <mergeCell ref="B1688:F1688"/>
+    <mergeCell ref="B1689:F1689"/>
+    <mergeCell ref="B1690:F1690"/>
+    <mergeCell ref="B1691:F1691"/>
+    <mergeCell ref="B1692:F1692"/>
+    <mergeCell ref="B1717:F1717"/>
+    <mergeCell ref="B1718:F1718"/>
+    <mergeCell ref="B1719:F1719"/>
+    <mergeCell ref="B1720:F1720"/>
+    <mergeCell ref="B1721:F1721"/>
+    <mergeCell ref="B1722:F1722"/>
+    <mergeCell ref="B1711:F1711"/>
+    <mergeCell ref="B1712:F1712"/>
+    <mergeCell ref="B1713:F1713"/>
+    <mergeCell ref="B1714:F1714"/>
+    <mergeCell ref="B1715:F1715"/>
+    <mergeCell ref="B1716:F1716"/>
+    <mergeCell ref="B1705:F1705"/>
+    <mergeCell ref="B1706:F1706"/>
+    <mergeCell ref="B1707:F1707"/>
+    <mergeCell ref="B1708:F1708"/>
+    <mergeCell ref="B1709:F1709"/>
+    <mergeCell ref="B1710:F1710"/>
+    <mergeCell ref="B1735:F1735"/>
+    <mergeCell ref="B1736:F1736"/>
+    <mergeCell ref="B1737:F1737"/>
+    <mergeCell ref="B1738:F1738"/>
+    <mergeCell ref="B1739:F1739"/>
+    <mergeCell ref="B1740:F1740"/>
+    <mergeCell ref="B1729:F1729"/>
+    <mergeCell ref="B1730:F1730"/>
+    <mergeCell ref="B1731:F1731"/>
+    <mergeCell ref="B1732:F1732"/>
+    <mergeCell ref="B1733:F1733"/>
+    <mergeCell ref="B1734:F1734"/>
+    <mergeCell ref="B1723:F1723"/>
+    <mergeCell ref="B1724:F1724"/>
+    <mergeCell ref="B1725:F1725"/>
+    <mergeCell ref="B1726:F1726"/>
+    <mergeCell ref="B1727:F1727"/>
+    <mergeCell ref="B1728:F1728"/>
+    <mergeCell ref="B1753:F1753"/>
+    <mergeCell ref="B1754:F1754"/>
+    <mergeCell ref="B1755:F1755"/>
+    <mergeCell ref="B1756:F1756"/>
+    <mergeCell ref="B1757:F1757"/>
+    <mergeCell ref="B1758:F1758"/>
+    <mergeCell ref="B1747:F1747"/>
+    <mergeCell ref="B1748:F1748"/>
+    <mergeCell ref="B1749:F1749"/>
+    <mergeCell ref="B1750:F1750"/>
+    <mergeCell ref="B1751:F1751"/>
+    <mergeCell ref="B1752:F1752"/>
+    <mergeCell ref="B1741:F1741"/>
+    <mergeCell ref="B1742:F1742"/>
+    <mergeCell ref="B1743:F1743"/>
+    <mergeCell ref="B1744:F1744"/>
+    <mergeCell ref="B1745:F1745"/>
+    <mergeCell ref="B1746:F1746"/>
+    <mergeCell ref="B1771:F1771"/>
+    <mergeCell ref="B1772:F1772"/>
+    <mergeCell ref="B1773:F1773"/>
+    <mergeCell ref="B1774:F1774"/>
+    <mergeCell ref="B1775:F1775"/>
+    <mergeCell ref="B1776:F1776"/>
+    <mergeCell ref="B1765:F1765"/>
+    <mergeCell ref="B1766:F1766"/>
+    <mergeCell ref="B1767:F1767"/>
+    <mergeCell ref="B1768:F1768"/>
+    <mergeCell ref="B1769:F1769"/>
+    <mergeCell ref="B1770:F1770"/>
+    <mergeCell ref="B1759:F1759"/>
+    <mergeCell ref="B1760:F1760"/>
+    <mergeCell ref="B1761:F1761"/>
+    <mergeCell ref="B1762:F1762"/>
+    <mergeCell ref="B1763:F1763"/>
+    <mergeCell ref="B1764:F1764"/>
+    <mergeCell ref="B1789:F1789"/>
+    <mergeCell ref="B1790:F1790"/>
+    <mergeCell ref="B1791:F1791"/>
+    <mergeCell ref="B1792:F1792"/>
+    <mergeCell ref="B1793:F1793"/>
+    <mergeCell ref="B1794:F1794"/>
+    <mergeCell ref="B1783:F1783"/>
+    <mergeCell ref="B1784:F1784"/>
+    <mergeCell ref="B1785:F1785"/>
+    <mergeCell ref="B1786:F1786"/>
+    <mergeCell ref="B1787:F1787"/>
+    <mergeCell ref="B1788:F1788"/>
+    <mergeCell ref="B1777:F1777"/>
+    <mergeCell ref="B1778:F1778"/>
+    <mergeCell ref="B1779:F1779"/>
+    <mergeCell ref="B1780:F1780"/>
+    <mergeCell ref="B1781:F1781"/>
+    <mergeCell ref="B1782:F1782"/>
+    <mergeCell ref="B1807:F1807"/>
+    <mergeCell ref="B1808:F1808"/>
+    <mergeCell ref="B1809:F1809"/>
+    <mergeCell ref="B1810:F1810"/>
+    <mergeCell ref="B1811:F1811"/>
+    <mergeCell ref="B1812:F1812"/>
+    <mergeCell ref="B1801:F1801"/>
+    <mergeCell ref="B1802:F1802"/>
+    <mergeCell ref="B1803:F1803"/>
+    <mergeCell ref="B1804:F1804"/>
+    <mergeCell ref="B1805:F1805"/>
+    <mergeCell ref="B1806:F1806"/>
+    <mergeCell ref="B1795:F1795"/>
+    <mergeCell ref="B1796:F1796"/>
+    <mergeCell ref="B1797:F1797"/>
+    <mergeCell ref="B1798:F1798"/>
+    <mergeCell ref="B1799:F1799"/>
+    <mergeCell ref="B1800:F1800"/>
+    <mergeCell ref="B1825:F1825"/>
+    <mergeCell ref="B1826:F1826"/>
+    <mergeCell ref="B1827:F1827"/>
+    <mergeCell ref="B1828:F1828"/>
+    <mergeCell ref="B1829:F1829"/>
+    <mergeCell ref="B1830:F1830"/>
+    <mergeCell ref="B1819:F1819"/>
+    <mergeCell ref="B1820:F1820"/>
+    <mergeCell ref="B1821:F1821"/>
+    <mergeCell ref="B1822:F1822"/>
+    <mergeCell ref="B1823:F1823"/>
+    <mergeCell ref="B1824:F1824"/>
+    <mergeCell ref="B1813:F1813"/>
+    <mergeCell ref="B1814:F1814"/>
+    <mergeCell ref="B1815:F1815"/>
+    <mergeCell ref="B1816:F1816"/>
+    <mergeCell ref="B1817:F1817"/>
+    <mergeCell ref="B1818:F1818"/>
+    <mergeCell ref="B1843:F1843"/>
+    <mergeCell ref="B1844:F1844"/>
+    <mergeCell ref="B1845:F1845"/>
+    <mergeCell ref="B1846:F1846"/>
+    <mergeCell ref="B1847:F1847"/>
+    <mergeCell ref="B1848:F1848"/>
+    <mergeCell ref="B1837:F1837"/>
+    <mergeCell ref="B1838:F1838"/>
+    <mergeCell ref="B1839:F1839"/>
+    <mergeCell ref="B1840:F1840"/>
+    <mergeCell ref="B1841:F1841"/>
+    <mergeCell ref="B1842:F1842"/>
+    <mergeCell ref="B1831:F1831"/>
+    <mergeCell ref="B1832:F1832"/>
+    <mergeCell ref="B1833:F1833"/>
+    <mergeCell ref="B1834:F1834"/>
+    <mergeCell ref="B1835:F1835"/>
+    <mergeCell ref="B1836:F1836"/>
+    <mergeCell ref="B1861:F1861"/>
+    <mergeCell ref="B1862:F1862"/>
+    <mergeCell ref="B1863:F1863"/>
+    <mergeCell ref="B1864:F1864"/>
+    <mergeCell ref="B1865:F1865"/>
+    <mergeCell ref="B1866:F1866"/>
+    <mergeCell ref="B1855:F1855"/>
+    <mergeCell ref="B1856:F1856"/>
+    <mergeCell ref="B1857:F1857"/>
+    <mergeCell ref="B1858:F1858"/>
+    <mergeCell ref="B1859:F1859"/>
+    <mergeCell ref="B1860:F1860"/>
+    <mergeCell ref="B1849:F1849"/>
+    <mergeCell ref="B1850:F1850"/>
+    <mergeCell ref="B1851:F1851"/>
+    <mergeCell ref="B1852:F1852"/>
+    <mergeCell ref="B1853:F1853"/>
+    <mergeCell ref="B1854:F1854"/>
+    <mergeCell ref="B1879:F1879"/>
+    <mergeCell ref="B1880:F1880"/>
+    <mergeCell ref="B1881:F1881"/>
+    <mergeCell ref="B1882:F1882"/>
+    <mergeCell ref="B1883:F1883"/>
+    <mergeCell ref="B1884:F1884"/>
+    <mergeCell ref="B1873:F1873"/>
+    <mergeCell ref="B1874:F1874"/>
+    <mergeCell ref="B1875:F1875"/>
+    <mergeCell ref="B1876:F1876"/>
+    <mergeCell ref="B1877:F1877"/>
+    <mergeCell ref="B1878:F1878"/>
+    <mergeCell ref="B1867:F1867"/>
+    <mergeCell ref="B1868:F1868"/>
+    <mergeCell ref="B1869:F1869"/>
+    <mergeCell ref="B1870:F1870"/>
+    <mergeCell ref="B1871:F1871"/>
+    <mergeCell ref="B1872:F1872"/>
+    <mergeCell ref="B1897:F1897"/>
+    <mergeCell ref="B1898:F1898"/>
+    <mergeCell ref="B1899:F1899"/>
+    <mergeCell ref="B1900:F1900"/>
+    <mergeCell ref="B1901:F1901"/>
+    <mergeCell ref="B1902:F1902"/>
+    <mergeCell ref="B1891:F1891"/>
+    <mergeCell ref="B1892:F1892"/>
+    <mergeCell ref="B1893:F1893"/>
+    <mergeCell ref="B1894:F1894"/>
+    <mergeCell ref="B1895:F1895"/>
+    <mergeCell ref="B1896:F1896"/>
+    <mergeCell ref="B1885:F1885"/>
+    <mergeCell ref="B1886:F1886"/>
+    <mergeCell ref="B1887:F1887"/>
+    <mergeCell ref="B1888:F1888"/>
+    <mergeCell ref="B1889:F1889"/>
+    <mergeCell ref="B1890:F1890"/>
+    <mergeCell ref="B1915:F1915"/>
+    <mergeCell ref="B1916:F1916"/>
+    <mergeCell ref="B1917:F1917"/>
+    <mergeCell ref="B1918:F1918"/>
+    <mergeCell ref="B1919:F1919"/>
+    <mergeCell ref="B1920:F1920"/>
+    <mergeCell ref="B1909:F1909"/>
+    <mergeCell ref="B1910:F1910"/>
+    <mergeCell ref="B1911:F1911"/>
+    <mergeCell ref="B1912:F1912"/>
+    <mergeCell ref="B1913:F1913"/>
+    <mergeCell ref="B1914:F1914"/>
+    <mergeCell ref="B1903:F1903"/>
+    <mergeCell ref="B1904:F1904"/>
+    <mergeCell ref="B1905:F1905"/>
+    <mergeCell ref="B1906:F1906"/>
+    <mergeCell ref="B1907:F1907"/>
+    <mergeCell ref="B1908:F1908"/>
+    <mergeCell ref="B1933:F1933"/>
+    <mergeCell ref="B1934:F1934"/>
+    <mergeCell ref="B1935:F1935"/>
+    <mergeCell ref="B1936:F1936"/>
+    <mergeCell ref="B1937:F1937"/>
+    <mergeCell ref="B1938:F1938"/>
+    <mergeCell ref="B1927:F1927"/>
+    <mergeCell ref="B1928:F1928"/>
+    <mergeCell ref="B1929:F1929"/>
+    <mergeCell ref="B1930:F1930"/>
+    <mergeCell ref="B1931:F1931"/>
+    <mergeCell ref="B1932:F1932"/>
+    <mergeCell ref="B1921:F1921"/>
+    <mergeCell ref="B1922:F1922"/>
+    <mergeCell ref="B1923:F1923"/>
+    <mergeCell ref="B1924:F1924"/>
+    <mergeCell ref="B1925:F1925"/>
+    <mergeCell ref="B1926:F1926"/>
+    <mergeCell ref="B1951:F1951"/>
+    <mergeCell ref="B1952:F1952"/>
+    <mergeCell ref="B1953:F1953"/>
+    <mergeCell ref="B1954:F1954"/>
+    <mergeCell ref="B1955:F1955"/>
+    <mergeCell ref="B1956:F1956"/>
+    <mergeCell ref="B1945:F1945"/>
+    <mergeCell ref="B1946:F1946"/>
+    <mergeCell ref="B1947:F1947"/>
+    <mergeCell ref="B1948:F1948"/>
+    <mergeCell ref="B1949:F1949"/>
+    <mergeCell ref="B1950:F1950"/>
+    <mergeCell ref="B1939:F1939"/>
+    <mergeCell ref="B1940:F1940"/>
+    <mergeCell ref="B1941:F1941"/>
+    <mergeCell ref="B1942:F1942"/>
+    <mergeCell ref="B1943:F1943"/>
+    <mergeCell ref="B1944:F1944"/>
+    <mergeCell ref="B1969:F1969"/>
+    <mergeCell ref="B1970:F1970"/>
+    <mergeCell ref="B1971:F1971"/>
+    <mergeCell ref="B1972:F1972"/>
+    <mergeCell ref="B1973:F1973"/>
+    <mergeCell ref="B1974:F1974"/>
+    <mergeCell ref="B1963:F1963"/>
+    <mergeCell ref="B1964:F1964"/>
+    <mergeCell ref="B1965:F1965"/>
+    <mergeCell ref="B1966:F1966"/>
+    <mergeCell ref="B1967:F1967"/>
+    <mergeCell ref="B1968:F1968"/>
+    <mergeCell ref="B1957:F1957"/>
+    <mergeCell ref="B1958:F1958"/>
+    <mergeCell ref="B1959:F1959"/>
+    <mergeCell ref="B1960:F1960"/>
+    <mergeCell ref="B1961:F1961"/>
+    <mergeCell ref="B1962:F1962"/>
     <mergeCell ref="B1993:F1993"/>
     <mergeCell ref="B1994:F1994"/>
     <mergeCell ref="B1995:F1995"/>
@@ -14793,1980 +17071,6 @@
     <mergeCell ref="B1978:F1978"/>
     <mergeCell ref="B1979:F1979"/>
     <mergeCell ref="B1980:F1980"/>
-    <mergeCell ref="B1969:F1969"/>
-    <mergeCell ref="B1970:F1970"/>
-    <mergeCell ref="B1971:F1971"/>
-    <mergeCell ref="B1972:F1972"/>
-    <mergeCell ref="B1973:F1973"/>
-    <mergeCell ref="B1974:F1974"/>
-    <mergeCell ref="B1963:F1963"/>
-    <mergeCell ref="B1964:F1964"/>
-    <mergeCell ref="B1965:F1965"/>
-    <mergeCell ref="B1966:F1966"/>
-    <mergeCell ref="B1967:F1967"/>
-    <mergeCell ref="B1968:F1968"/>
-    <mergeCell ref="B1957:F1957"/>
-    <mergeCell ref="B1958:F1958"/>
-    <mergeCell ref="B1959:F1959"/>
-    <mergeCell ref="B1960:F1960"/>
-    <mergeCell ref="B1961:F1961"/>
-    <mergeCell ref="B1962:F1962"/>
-    <mergeCell ref="B1951:F1951"/>
-    <mergeCell ref="B1952:F1952"/>
-    <mergeCell ref="B1953:F1953"/>
-    <mergeCell ref="B1954:F1954"/>
-    <mergeCell ref="B1955:F1955"/>
-    <mergeCell ref="B1956:F1956"/>
-    <mergeCell ref="B1945:F1945"/>
-    <mergeCell ref="B1946:F1946"/>
-    <mergeCell ref="B1947:F1947"/>
-    <mergeCell ref="B1948:F1948"/>
-    <mergeCell ref="B1949:F1949"/>
-    <mergeCell ref="B1950:F1950"/>
-    <mergeCell ref="B1939:F1939"/>
-    <mergeCell ref="B1940:F1940"/>
-    <mergeCell ref="B1941:F1941"/>
-    <mergeCell ref="B1942:F1942"/>
-    <mergeCell ref="B1943:F1943"/>
-    <mergeCell ref="B1944:F1944"/>
-    <mergeCell ref="B1933:F1933"/>
-    <mergeCell ref="B1934:F1934"/>
-    <mergeCell ref="B1935:F1935"/>
-    <mergeCell ref="B1936:F1936"/>
-    <mergeCell ref="B1937:F1937"/>
-    <mergeCell ref="B1938:F1938"/>
-    <mergeCell ref="B1927:F1927"/>
-    <mergeCell ref="B1928:F1928"/>
-    <mergeCell ref="B1929:F1929"/>
-    <mergeCell ref="B1930:F1930"/>
-    <mergeCell ref="B1931:F1931"/>
-    <mergeCell ref="B1932:F1932"/>
-    <mergeCell ref="B1921:F1921"/>
-    <mergeCell ref="B1922:F1922"/>
-    <mergeCell ref="B1923:F1923"/>
-    <mergeCell ref="B1924:F1924"/>
-    <mergeCell ref="B1925:F1925"/>
-    <mergeCell ref="B1926:F1926"/>
-    <mergeCell ref="B1915:F1915"/>
-    <mergeCell ref="B1916:F1916"/>
-    <mergeCell ref="B1917:F1917"/>
-    <mergeCell ref="B1918:F1918"/>
-    <mergeCell ref="B1919:F1919"/>
-    <mergeCell ref="B1920:F1920"/>
-    <mergeCell ref="B1909:F1909"/>
-    <mergeCell ref="B1910:F1910"/>
-    <mergeCell ref="B1911:F1911"/>
-    <mergeCell ref="B1912:F1912"/>
-    <mergeCell ref="B1913:F1913"/>
-    <mergeCell ref="B1914:F1914"/>
-    <mergeCell ref="B1903:F1903"/>
-    <mergeCell ref="B1904:F1904"/>
-    <mergeCell ref="B1905:F1905"/>
-    <mergeCell ref="B1906:F1906"/>
-    <mergeCell ref="B1907:F1907"/>
-    <mergeCell ref="B1908:F1908"/>
-    <mergeCell ref="B1897:F1897"/>
-    <mergeCell ref="B1898:F1898"/>
-    <mergeCell ref="B1899:F1899"/>
-    <mergeCell ref="B1900:F1900"/>
-    <mergeCell ref="B1901:F1901"/>
-    <mergeCell ref="B1902:F1902"/>
-    <mergeCell ref="B1891:F1891"/>
-    <mergeCell ref="B1892:F1892"/>
-    <mergeCell ref="B1893:F1893"/>
-    <mergeCell ref="B1894:F1894"/>
-    <mergeCell ref="B1895:F1895"/>
-    <mergeCell ref="B1896:F1896"/>
-    <mergeCell ref="B1885:F1885"/>
-    <mergeCell ref="B1886:F1886"/>
-    <mergeCell ref="B1887:F1887"/>
-    <mergeCell ref="B1888:F1888"/>
-    <mergeCell ref="B1889:F1889"/>
-    <mergeCell ref="B1890:F1890"/>
-    <mergeCell ref="B1879:F1879"/>
-    <mergeCell ref="B1880:F1880"/>
-    <mergeCell ref="B1881:F1881"/>
-    <mergeCell ref="B1882:F1882"/>
-    <mergeCell ref="B1883:F1883"/>
-    <mergeCell ref="B1884:F1884"/>
-    <mergeCell ref="B1873:F1873"/>
-    <mergeCell ref="B1874:F1874"/>
-    <mergeCell ref="B1875:F1875"/>
-    <mergeCell ref="B1876:F1876"/>
-    <mergeCell ref="B1877:F1877"/>
-    <mergeCell ref="B1878:F1878"/>
-    <mergeCell ref="B1867:F1867"/>
-    <mergeCell ref="B1868:F1868"/>
-    <mergeCell ref="B1869:F1869"/>
-    <mergeCell ref="B1870:F1870"/>
-    <mergeCell ref="B1871:F1871"/>
-    <mergeCell ref="B1872:F1872"/>
-    <mergeCell ref="B1861:F1861"/>
-    <mergeCell ref="B1862:F1862"/>
-    <mergeCell ref="B1863:F1863"/>
-    <mergeCell ref="B1864:F1864"/>
-    <mergeCell ref="B1865:F1865"/>
-    <mergeCell ref="B1866:F1866"/>
-    <mergeCell ref="B1855:F1855"/>
-    <mergeCell ref="B1856:F1856"/>
-    <mergeCell ref="B1857:F1857"/>
-    <mergeCell ref="B1858:F1858"/>
-    <mergeCell ref="B1859:F1859"/>
-    <mergeCell ref="B1860:F1860"/>
-    <mergeCell ref="B1849:F1849"/>
-    <mergeCell ref="B1850:F1850"/>
-    <mergeCell ref="B1851:F1851"/>
-    <mergeCell ref="B1852:F1852"/>
-    <mergeCell ref="B1853:F1853"/>
-    <mergeCell ref="B1854:F1854"/>
-    <mergeCell ref="B1843:F1843"/>
-    <mergeCell ref="B1844:F1844"/>
-    <mergeCell ref="B1845:F1845"/>
-    <mergeCell ref="B1846:F1846"/>
-    <mergeCell ref="B1847:F1847"/>
-    <mergeCell ref="B1848:F1848"/>
-    <mergeCell ref="B1837:F1837"/>
-    <mergeCell ref="B1838:F1838"/>
-    <mergeCell ref="B1839:F1839"/>
-    <mergeCell ref="B1840:F1840"/>
-    <mergeCell ref="B1841:F1841"/>
-    <mergeCell ref="B1842:F1842"/>
-    <mergeCell ref="B1831:F1831"/>
-    <mergeCell ref="B1832:F1832"/>
-    <mergeCell ref="B1833:F1833"/>
-    <mergeCell ref="B1834:F1834"/>
-    <mergeCell ref="B1835:F1835"/>
-    <mergeCell ref="B1836:F1836"/>
-    <mergeCell ref="B1825:F1825"/>
-    <mergeCell ref="B1826:F1826"/>
-    <mergeCell ref="B1827:F1827"/>
-    <mergeCell ref="B1828:F1828"/>
-    <mergeCell ref="B1829:F1829"/>
-    <mergeCell ref="B1830:F1830"/>
-    <mergeCell ref="B1819:F1819"/>
-    <mergeCell ref="B1820:F1820"/>
-    <mergeCell ref="B1821:F1821"/>
-    <mergeCell ref="B1822:F1822"/>
-    <mergeCell ref="B1823:F1823"/>
-    <mergeCell ref="B1824:F1824"/>
-    <mergeCell ref="B1813:F1813"/>
-    <mergeCell ref="B1814:F1814"/>
-    <mergeCell ref="B1815:F1815"/>
-    <mergeCell ref="B1816:F1816"/>
-    <mergeCell ref="B1817:F1817"/>
-    <mergeCell ref="B1818:F1818"/>
-    <mergeCell ref="B1807:F1807"/>
-    <mergeCell ref="B1808:F1808"/>
-    <mergeCell ref="B1809:F1809"/>
-    <mergeCell ref="B1810:F1810"/>
-    <mergeCell ref="B1811:F1811"/>
-    <mergeCell ref="B1812:F1812"/>
-    <mergeCell ref="B1801:F1801"/>
-    <mergeCell ref="B1802:F1802"/>
-    <mergeCell ref="B1803:F1803"/>
-    <mergeCell ref="B1804:F1804"/>
-    <mergeCell ref="B1805:F1805"/>
-    <mergeCell ref="B1806:F1806"/>
-    <mergeCell ref="B1795:F1795"/>
-    <mergeCell ref="B1796:F1796"/>
-    <mergeCell ref="B1797:F1797"/>
-    <mergeCell ref="B1798:F1798"/>
-    <mergeCell ref="B1799:F1799"/>
-    <mergeCell ref="B1800:F1800"/>
-    <mergeCell ref="B1789:F1789"/>
-    <mergeCell ref="B1790:F1790"/>
-    <mergeCell ref="B1791:F1791"/>
-    <mergeCell ref="B1792:F1792"/>
-    <mergeCell ref="B1793:F1793"/>
-    <mergeCell ref="B1794:F1794"/>
-    <mergeCell ref="B1783:F1783"/>
-    <mergeCell ref="B1784:F1784"/>
-    <mergeCell ref="B1785:F1785"/>
-    <mergeCell ref="B1786:F1786"/>
-    <mergeCell ref="B1787:F1787"/>
-    <mergeCell ref="B1788:F1788"/>
-    <mergeCell ref="B1777:F1777"/>
-    <mergeCell ref="B1778:F1778"/>
-    <mergeCell ref="B1779:F1779"/>
-    <mergeCell ref="B1780:F1780"/>
-    <mergeCell ref="B1781:F1781"/>
-    <mergeCell ref="B1782:F1782"/>
-    <mergeCell ref="B1771:F1771"/>
-    <mergeCell ref="B1772:F1772"/>
-    <mergeCell ref="B1773:F1773"/>
-    <mergeCell ref="B1774:F1774"/>
-    <mergeCell ref="B1775:F1775"/>
-    <mergeCell ref="B1776:F1776"/>
-    <mergeCell ref="B1765:F1765"/>
-    <mergeCell ref="B1766:F1766"/>
-    <mergeCell ref="B1767:F1767"/>
-    <mergeCell ref="B1768:F1768"/>
-    <mergeCell ref="B1769:F1769"/>
-    <mergeCell ref="B1770:F1770"/>
-    <mergeCell ref="B1759:F1759"/>
-    <mergeCell ref="B1760:F1760"/>
-    <mergeCell ref="B1761:F1761"/>
-    <mergeCell ref="B1762:F1762"/>
-    <mergeCell ref="B1763:F1763"/>
-    <mergeCell ref="B1764:F1764"/>
-    <mergeCell ref="B1753:F1753"/>
-    <mergeCell ref="B1754:F1754"/>
-    <mergeCell ref="B1755:F1755"/>
-    <mergeCell ref="B1756:F1756"/>
-    <mergeCell ref="B1757:F1757"/>
-    <mergeCell ref="B1758:F1758"/>
-    <mergeCell ref="B1747:F1747"/>
-    <mergeCell ref="B1748:F1748"/>
-    <mergeCell ref="B1749:F1749"/>
-    <mergeCell ref="B1750:F1750"/>
-    <mergeCell ref="B1751:F1751"/>
-    <mergeCell ref="B1752:F1752"/>
-    <mergeCell ref="B1741:F1741"/>
-    <mergeCell ref="B1742:F1742"/>
-    <mergeCell ref="B1743:F1743"/>
-    <mergeCell ref="B1744:F1744"/>
-    <mergeCell ref="B1745:F1745"/>
-    <mergeCell ref="B1746:F1746"/>
-    <mergeCell ref="B1735:F1735"/>
-    <mergeCell ref="B1736:F1736"/>
-    <mergeCell ref="B1737:F1737"/>
-    <mergeCell ref="B1738:F1738"/>
-    <mergeCell ref="B1739:F1739"/>
-    <mergeCell ref="B1740:F1740"/>
-    <mergeCell ref="B1729:F1729"/>
-    <mergeCell ref="B1730:F1730"/>
-    <mergeCell ref="B1731:F1731"/>
-    <mergeCell ref="B1732:F1732"/>
-    <mergeCell ref="B1733:F1733"/>
-    <mergeCell ref="B1734:F1734"/>
-    <mergeCell ref="B1723:F1723"/>
-    <mergeCell ref="B1724:F1724"/>
-    <mergeCell ref="B1725:F1725"/>
-    <mergeCell ref="B1726:F1726"/>
-    <mergeCell ref="B1727:F1727"/>
-    <mergeCell ref="B1728:F1728"/>
-    <mergeCell ref="B1717:F1717"/>
-    <mergeCell ref="B1718:F1718"/>
-    <mergeCell ref="B1719:F1719"/>
-    <mergeCell ref="B1720:F1720"/>
-    <mergeCell ref="B1721:F1721"/>
-    <mergeCell ref="B1722:F1722"/>
-    <mergeCell ref="B1711:F1711"/>
-    <mergeCell ref="B1712:F1712"/>
-    <mergeCell ref="B1713:F1713"/>
-    <mergeCell ref="B1714:F1714"/>
-    <mergeCell ref="B1715:F1715"/>
-    <mergeCell ref="B1716:F1716"/>
-    <mergeCell ref="B1705:F1705"/>
-    <mergeCell ref="B1706:F1706"/>
-    <mergeCell ref="B1707:F1707"/>
-    <mergeCell ref="B1708:F1708"/>
-    <mergeCell ref="B1709:F1709"/>
-    <mergeCell ref="B1710:F1710"/>
-    <mergeCell ref="B1699:F1699"/>
-    <mergeCell ref="B1700:F1700"/>
-    <mergeCell ref="B1701:F1701"/>
-    <mergeCell ref="B1702:F1702"/>
-    <mergeCell ref="B1703:F1703"/>
-    <mergeCell ref="B1704:F1704"/>
-    <mergeCell ref="B1693:F1693"/>
-    <mergeCell ref="B1694:F1694"/>
-    <mergeCell ref="B1695:F1695"/>
-    <mergeCell ref="B1696:F1696"/>
-    <mergeCell ref="B1697:F1697"/>
-    <mergeCell ref="B1698:F1698"/>
-    <mergeCell ref="B1687:F1687"/>
-    <mergeCell ref="B1688:F1688"/>
-    <mergeCell ref="B1689:F1689"/>
-    <mergeCell ref="B1690:F1690"/>
-    <mergeCell ref="B1691:F1691"/>
-    <mergeCell ref="B1692:F1692"/>
-    <mergeCell ref="B1681:F1681"/>
-    <mergeCell ref="B1682:F1682"/>
-    <mergeCell ref="B1683:F1683"/>
-    <mergeCell ref="B1684:F1684"/>
-    <mergeCell ref="B1685:F1685"/>
-    <mergeCell ref="B1686:F1686"/>
-    <mergeCell ref="B1675:F1675"/>
-    <mergeCell ref="B1676:F1676"/>
-    <mergeCell ref="B1677:F1677"/>
-    <mergeCell ref="B1678:F1678"/>
-    <mergeCell ref="B1679:F1679"/>
-    <mergeCell ref="B1680:F1680"/>
-    <mergeCell ref="B1669:F1669"/>
-    <mergeCell ref="B1670:F1670"/>
-    <mergeCell ref="B1671:F1671"/>
-    <mergeCell ref="B1672:F1672"/>
-    <mergeCell ref="B1673:F1673"/>
-    <mergeCell ref="B1674:F1674"/>
-    <mergeCell ref="B1663:F1663"/>
-    <mergeCell ref="B1664:F1664"/>
-    <mergeCell ref="B1665:F1665"/>
-    <mergeCell ref="B1666:F1666"/>
-    <mergeCell ref="B1667:F1667"/>
-    <mergeCell ref="B1668:F1668"/>
-    <mergeCell ref="B1657:F1657"/>
-    <mergeCell ref="B1658:F1658"/>
-    <mergeCell ref="B1659:F1659"/>
-    <mergeCell ref="B1660:F1660"/>
-    <mergeCell ref="B1661:F1661"/>
-    <mergeCell ref="B1662:F1662"/>
-    <mergeCell ref="B1651:F1651"/>
-    <mergeCell ref="B1652:F1652"/>
-    <mergeCell ref="B1653:F1653"/>
-    <mergeCell ref="B1654:F1654"/>
-    <mergeCell ref="B1655:F1655"/>
-    <mergeCell ref="B1656:F1656"/>
-    <mergeCell ref="B1645:F1645"/>
-    <mergeCell ref="B1646:F1646"/>
-    <mergeCell ref="B1647:F1647"/>
-    <mergeCell ref="B1648:F1648"/>
-    <mergeCell ref="B1649:F1649"/>
-    <mergeCell ref="B1650:F1650"/>
-    <mergeCell ref="B1639:F1639"/>
-    <mergeCell ref="B1640:F1640"/>
-    <mergeCell ref="B1641:F1641"/>
-    <mergeCell ref="B1642:F1642"/>
-    <mergeCell ref="B1643:F1643"/>
-    <mergeCell ref="B1644:F1644"/>
-    <mergeCell ref="B1633:F1633"/>
-    <mergeCell ref="B1634:F1634"/>
-    <mergeCell ref="B1635:F1635"/>
-    <mergeCell ref="B1636:F1636"/>
-    <mergeCell ref="B1637:F1637"/>
-    <mergeCell ref="B1638:F1638"/>
-    <mergeCell ref="B1627:F1627"/>
-    <mergeCell ref="B1628:F1628"/>
-    <mergeCell ref="B1629:F1629"/>
-    <mergeCell ref="B1630:F1630"/>
-    <mergeCell ref="B1631:F1631"/>
-    <mergeCell ref="B1632:F1632"/>
-    <mergeCell ref="B1621:F1621"/>
-    <mergeCell ref="B1622:F1622"/>
-    <mergeCell ref="B1623:F1623"/>
-    <mergeCell ref="B1624:F1624"/>
-    <mergeCell ref="B1625:F1625"/>
-    <mergeCell ref="B1626:F1626"/>
-    <mergeCell ref="B1615:F1615"/>
-    <mergeCell ref="B1616:F1616"/>
-    <mergeCell ref="B1617:F1617"/>
-    <mergeCell ref="B1618:F1618"/>
-    <mergeCell ref="B1619:F1619"/>
-    <mergeCell ref="B1620:F1620"/>
-    <mergeCell ref="B1609:F1609"/>
-    <mergeCell ref="B1610:F1610"/>
-    <mergeCell ref="B1611:F1611"/>
-    <mergeCell ref="B1612:F1612"/>
-    <mergeCell ref="B1613:F1613"/>
-    <mergeCell ref="B1614:F1614"/>
-    <mergeCell ref="B1603:F1603"/>
-    <mergeCell ref="B1604:F1604"/>
-    <mergeCell ref="B1605:F1605"/>
-    <mergeCell ref="B1606:F1606"/>
-    <mergeCell ref="B1607:F1607"/>
-    <mergeCell ref="B1608:F1608"/>
-    <mergeCell ref="B1597:F1597"/>
-    <mergeCell ref="B1598:F1598"/>
-    <mergeCell ref="B1599:F1599"/>
-    <mergeCell ref="B1600:F1600"/>
-    <mergeCell ref="B1601:F1601"/>
-    <mergeCell ref="B1602:F1602"/>
-    <mergeCell ref="B1591:F1591"/>
-    <mergeCell ref="B1592:F1592"/>
-    <mergeCell ref="B1593:F1593"/>
-    <mergeCell ref="B1594:F1594"/>
-    <mergeCell ref="B1595:F1595"/>
-    <mergeCell ref="B1596:F1596"/>
-    <mergeCell ref="B1585:F1585"/>
-    <mergeCell ref="B1586:F1586"/>
-    <mergeCell ref="B1587:F1587"/>
-    <mergeCell ref="B1588:F1588"/>
-    <mergeCell ref="B1589:F1589"/>
-    <mergeCell ref="B1590:F1590"/>
-    <mergeCell ref="B1579:F1579"/>
-    <mergeCell ref="B1580:F1580"/>
-    <mergeCell ref="B1581:F1581"/>
-    <mergeCell ref="B1582:F1582"/>
-    <mergeCell ref="B1583:F1583"/>
-    <mergeCell ref="B1584:F1584"/>
-    <mergeCell ref="B1573:F1573"/>
-    <mergeCell ref="B1574:F1574"/>
-    <mergeCell ref="B1575:F1575"/>
-    <mergeCell ref="B1576:F1576"/>
-    <mergeCell ref="B1577:F1577"/>
-    <mergeCell ref="B1578:F1578"/>
-    <mergeCell ref="B1567:F1567"/>
-    <mergeCell ref="B1568:F1568"/>
-    <mergeCell ref="B1569:F1569"/>
-    <mergeCell ref="B1570:F1570"/>
-    <mergeCell ref="B1571:F1571"/>
-    <mergeCell ref="B1572:F1572"/>
-    <mergeCell ref="B1561:F1561"/>
-    <mergeCell ref="B1562:F1562"/>
-    <mergeCell ref="B1563:F1563"/>
-    <mergeCell ref="B1564:F1564"/>
-    <mergeCell ref="B1565:F1565"/>
-    <mergeCell ref="B1566:F1566"/>
-    <mergeCell ref="B1555:F1555"/>
-    <mergeCell ref="B1556:F1556"/>
-    <mergeCell ref="B1557:F1557"/>
-    <mergeCell ref="B1558:F1558"/>
-    <mergeCell ref="B1559:F1559"/>
-    <mergeCell ref="B1560:F1560"/>
-    <mergeCell ref="B1549:F1549"/>
-    <mergeCell ref="B1550:F1550"/>
-    <mergeCell ref="B1551:F1551"/>
-    <mergeCell ref="B1552:F1552"/>
-    <mergeCell ref="B1553:F1553"/>
-    <mergeCell ref="B1554:F1554"/>
-    <mergeCell ref="B1543:F1543"/>
-    <mergeCell ref="B1544:F1544"/>
-    <mergeCell ref="B1545:F1545"/>
-    <mergeCell ref="B1546:F1546"/>
-    <mergeCell ref="B1547:F1547"/>
-    <mergeCell ref="B1548:F1548"/>
-    <mergeCell ref="B1537:F1537"/>
-    <mergeCell ref="B1538:F1538"/>
-    <mergeCell ref="B1539:F1539"/>
-    <mergeCell ref="B1540:F1540"/>
-    <mergeCell ref="B1541:F1541"/>
-    <mergeCell ref="B1542:F1542"/>
-    <mergeCell ref="B1531:F1531"/>
-    <mergeCell ref="B1532:F1532"/>
-    <mergeCell ref="B1533:F1533"/>
-    <mergeCell ref="B1534:F1534"/>
-    <mergeCell ref="B1535:F1535"/>
-    <mergeCell ref="B1536:F1536"/>
-    <mergeCell ref="B1525:F1525"/>
-    <mergeCell ref="B1526:F1526"/>
-    <mergeCell ref="B1527:F1527"/>
-    <mergeCell ref="B1528:F1528"/>
-    <mergeCell ref="B1529:F1529"/>
-    <mergeCell ref="B1530:F1530"/>
-    <mergeCell ref="B1519:F1519"/>
-    <mergeCell ref="B1520:F1520"/>
-    <mergeCell ref="B1521:F1521"/>
-    <mergeCell ref="B1522:F1522"/>
-    <mergeCell ref="B1523:F1523"/>
-    <mergeCell ref="B1524:F1524"/>
-    <mergeCell ref="B1513:F1513"/>
-    <mergeCell ref="B1514:F1514"/>
-    <mergeCell ref="B1515:F1515"/>
-    <mergeCell ref="B1516:F1516"/>
-    <mergeCell ref="B1517:F1517"/>
-    <mergeCell ref="B1518:F1518"/>
-    <mergeCell ref="B1507:F1507"/>
-    <mergeCell ref="B1508:F1508"/>
-    <mergeCell ref="B1509:F1509"/>
-    <mergeCell ref="B1510:F1510"/>
-    <mergeCell ref="B1511:F1511"/>
-    <mergeCell ref="B1512:F1512"/>
-    <mergeCell ref="B1501:F1501"/>
-    <mergeCell ref="B1502:F1502"/>
-    <mergeCell ref="B1503:F1503"/>
-    <mergeCell ref="B1504:F1504"/>
-    <mergeCell ref="B1505:F1505"/>
-    <mergeCell ref="B1506:F1506"/>
-    <mergeCell ref="B1495:F1495"/>
-    <mergeCell ref="B1496:F1496"/>
-    <mergeCell ref="B1497:F1497"/>
-    <mergeCell ref="B1498:F1498"/>
-    <mergeCell ref="B1499:F1499"/>
-    <mergeCell ref="B1500:F1500"/>
-    <mergeCell ref="B1489:F1489"/>
-    <mergeCell ref="B1490:F1490"/>
-    <mergeCell ref="B1491:F1491"/>
-    <mergeCell ref="B1492:F1492"/>
-    <mergeCell ref="B1493:F1493"/>
-    <mergeCell ref="B1494:F1494"/>
-    <mergeCell ref="B1483:F1483"/>
-    <mergeCell ref="B1484:F1484"/>
-    <mergeCell ref="B1485:F1485"/>
-    <mergeCell ref="B1486:F1486"/>
-    <mergeCell ref="B1487:F1487"/>
-    <mergeCell ref="B1488:F1488"/>
-    <mergeCell ref="B1477:F1477"/>
-    <mergeCell ref="B1478:F1478"/>
-    <mergeCell ref="B1479:F1479"/>
-    <mergeCell ref="B1480:F1480"/>
-    <mergeCell ref="B1481:F1481"/>
-    <mergeCell ref="B1482:F1482"/>
-    <mergeCell ref="B1471:F1471"/>
-    <mergeCell ref="B1472:F1472"/>
-    <mergeCell ref="B1473:F1473"/>
-    <mergeCell ref="B1474:F1474"/>
-    <mergeCell ref="B1475:F1475"/>
-    <mergeCell ref="B1476:F1476"/>
-    <mergeCell ref="B1465:F1465"/>
-    <mergeCell ref="B1466:F1466"/>
-    <mergeCell ref="B1467:F1467"/>
-    <mergeCell ref="B1468:F1468"/>
-    <mergeCell ref="B1469:F1469"/>
-    <mergeCell ref="B1470:F1470"/>
-    <mergeCell ref="B1459:F1459"/>
-    <mergeCell ref="B1460:F1460"/>
-    <mergeCell ref="B1461:F1461"/>
-    <mergeCell ref="B1462:F1462"/>
-    <mergeCell ref="B1463:F1463"/>
-    <mergeCell ref="B1464:F1464"/>
-    <mergeCell ref="B1453:F1453"/>
-    <mergeCell ref="B1454:F1454"/>
-    <mergeCell ref="B1455:F1455"/>
-    <mergeCell ref="B1456:F1456"/>
-    <mergeCell ref="B1457:F1457"/>
-    <mergeCell ref="B1458:F1458"/>
-    <mergeCell ref="B1447:F1447"/>
-    <mergeCell ref="B1448:F1448"/>
-    <mergeCell ref="B1449:F1449"/>
-    <mergeCell ref="B1450:F1450"/>
-    <mergeCell ref="B1451:F1451"/>
-    <mergeCell ref="B1452:F1452"/>
-    <mergeCell ref="B1441:F1441"/>
-    <mergeCell ref="B1442:F1442"/>
-    <mergeCell ref="B1443:F1443"/>
-    <mergeCell ref="B1444:F1444"/>
-    <mergeCell ref="B1445:F1445"/>
-    <mergeCell ref="B1446:F1446"/>
-    <mergeCell ref="B1435:F1435"/>
-    <mergeCell ref="B1436:F1436"/>
-    <mergeCell ref="B1437:F1437"/>
-    <mergeCell ref="B1438:F1438"/>
-    <mergeCell ref="B1439:F1439"/>
-    <mergeCell ref="B1440:F1440"/>
-    <mergeCell ref="B1429:F1429"/>
-    <mergeCell ref="B1430:F1430"/>
-    <mergeCell ref="B1431:F1431"/>
-    <mergeCell ref="B1432:F1432"/>
-    <mergeCell ref="B1433:F1433"/>
-    <mergeCell ref="B1434:F1434"/>
-    <mergeCell ref="B1423:F1423"/>
-    <mergeCell ref="B1424:F1424"/>
-    <mergeCell ref="B1425:F1425"/>
-    <mergeCell ref="B1426:F1426"/>
-    <mergeCell ref="B1427:F1427"/>
-    <mergeCell ref="B1428:F1428"/>
-    <mergeCell ref="B1417:F1417"/>
-    <mergeCell ref="B1418:F1418"/>
-    <mergeCell ref="B1419:F1419"/>
-    <mergeCell ref="B1420:F1420"/>
-    <mergeCell ref="B1421:F1421"/>
-    <mergeCell ref="B1422:F1422"/>
-    <mergeCell ref="B1411:F1411"/>
-    <mergeCell ref="B1412:F1412"/>
-    <mergeCell ref="B1413:F1413"/>
-    <mergeCell ref="B1414:F1414"/>
-    <mergeCell ref="B1415:F1415"/>
-    <mergeCell ref="B1416:F1416"/>
-    <mergeCell ref="B1405:F1405"/>
-    <mergeCell ref="B1406:F1406"/>
-    <mergeCell ref="B1407:F1407"/>
-    <mergeCell ref="B1408:F1408"/>
-    <mergeCell ref="B1409:F1409"/>
-    <mergeCell ref="B1410:F1410"/>
-    <mergeCell ref="B1399:F1399"/>
-    <mergeCell ref="B1400:F1400"/>
-    <mergeCell ref="B1401:F1401"/>
-    <mergeCell ref="B1402:F1402"/>
-    <mergeCell ref="B1403:F1403"/>
-    <mergeCell ref="B1404:F1404"/>
-    <mergeCell ref="B1393:F1393"/>
-    <mergeCell ref="B1394:F1394"/>
-    <mergeCell ref="B1395:F1395"/>
-    <mergeCell ref="B1396:F1396"/>
-    <mergeCell ref="B1397:F1397"/>
-    <mergeCell ref="B1398:F1398"/>
-    <mergeCell ref="B1387:F1387"/>
-    <mergeCell ref="B1388:F1388"/>
-    <mergeCell ref="B1389:F1389"/>
-    <mergeCell ref="B1390:F1390"/>
-    <mergeCell ref="B1391:F1391"/>
-    <mergeCell ref="B1392:F1392"/>
-    <mergeCell ref="B1381:F1381"/>
-    <mergeCell ref="B1382:F1382"/>
-    <mergeCell ref="B1383:F1383"/>
-    <mergeCell ref="B1384:F1384"/>
-    <mergeCell ref="B1385:F1385"/>
-    <mergeCell ref="B1386:F1386"/>
-    <mergeCell ref="B1375:F1375"/>
-    <mergeCell ref="B1376:F1376"/>
-    <mergeCell ref="B1377:F1377"/>
-    <mergeCell ref="B1378:F1378"/>
-    <mergeCell ref="B1379:F1379"/>
-    <mergeCell ref="B1380:F1380"/>
-    <mergeCell ref="B1369:F1369"/>
-    <mergeCell ref="B1370:F1370"/>
-    <mergeCell ref="B1371:F1371"/>
-    <mergeCell ref="B1372:F1372"/>
-    <mergeCell ref="B1373:F1373"/>
-    <mergeCell ref="B1374:F1374"/>
-    <mergeCell ref="B1363:F1363"/>
-    <mergeCell ref="B1364:F1364"/>
-    <mergeCell ref="B1365:F1365"/>
-    <mergeCell ref="B1366:F1366"/>
-    <mergeCell ref="B1367:F1367"/>
-    <mergeCell ref="B1368:F1368"/>
-    <mergeCell ref="B1357:F1357"/>
-    <mergeCell ref="B1358:F1358"/>
-    <mergeCell ref="B1359:F1359"/>
-    <mergeCell ref="B1360:F1360"/>
-    <mergeCell ref="B1361:F1361"/>
-    <mergeCell ref="B1362:F1362"/>
-    <mergeCell ref="B1351:F1351"/>
-    <mergeCell ref="B1352:F1352"/>
-    <mergeCell ref="B1353:F1353"/>
-    <mergeCell ref="B1354:F1354"/>
-    <mergeCell ref="B1355:F1355"/>
-    <mergeCell ref="B1356:F1356"/>
-    <mergeCell ref="B1345:F1345"/>
-    <mergeCell ref="B1346:F1346"/>
-    <mergeCell ref="B1347:F1347"/>
-    <mergeCell ref="B1348:F1348"/>
-    <mergeCell ref="B1349:F1349"/>
-    <mergeCell ref="B1350:F1350"/>
-    <mergeCell ref="B1339:F1339"/>
-    <mergeCell ref="B1340:F1340"/>
-    <mergeCell ref="B1341:F1341"/>
-    <mergeCell ref="B1342:F1342"/>
-    <mergeCell ref="B1343:F1343"/>
-    <mergeCell ref="B1344:F1344"/>
-    <mergeCell ref="B1333:F1333"/>
-    <mergeCell ref="B1334:F1334"/>
-    <mergeCell ref="B1335:F1335"/>
-    <mergeCell ref="B1336:F1336"/>
-    <mergeCell ref="B1337:F1337"/>
-    <mergeCell ref="B1338:F1338"/>
-    <mergeCell ref="B1327:F1327"/>
-    <mergeCell ref="B1328:F1328"/>
-    <mergeCell ref="B1329:F1329"/>
-    <mergeCell ref="B1330:F1330"/>
-    <mergeCell ref="B1331:F1331"/>
-    <mergeCell ref="B1332:F1332"/>
-    <mergeCell ref="B1321:F1321"/>
-    <mergeCell ref="B1322:F1322"/>
-    <mergeCell ref="B1323:F1323"/>
-    <mergeCell ref="B1324:F1324"/>
-    <mergeCell ref="B1325:F1325"/>
-    <mergeCell ref="B1326:F1326"/>
-    <mergeCell ref="B1315:F1315"/>
-    <mergeCell ref="B1316:F1316"/>
-    <mergeCell ref="B1317:F1317"/>
-    <mergeCell ref="B1318:F1318"/>
-    <mergeCell ref="B1319:F1319"/>
-    <mergeCell ref="B1320:F1320"/>
-    <mergeCell ref="B1309:F1309"/>
-    <mergeCell ref="B1310:F1310"/>
-    <mergeCell ref="B1311:F1311"/>
-    <mergeCell ref="B1312:F1312"/>
-    <mergeCell ref="B1313:F1313"/>
-    <mergeCell ref="B1314:F1314"/>
-    <mergeCell ref="B1303:F1303"/>
-    <mergeCell ref="B1304:F1304"/>
-    <mergeCell ref="B1305:F1305"/>
-    <mergeCell ref="B1306:F1306"/>
-    <mergeCell ref="B1307:F1307"/>
-    <mergeCell ref="B1308:F1308"/>
-    <mergeCell ref="B1297:F1297"/>
-    <mergeCell ref="B1298:F1298"/>
-    <mergeCell ref="B1299:F1299"/>
-    <mergeCell ref="B1300:F1300"/>
-    <mergeCell ref="B1301:F1301"/>
-    <mergeCell ref="B1302:F1302"/>
-    <mergeCell ref="B1291:F1291"/>
-    <mergeCell ref="B1292:F1292"/>
-    <mergeCell ref="B1293:F1293"/>
-    <mergeCell ref="B1294:F1294"/>
-    <mergeCell ref="B1295:F1295"/>
-    <mergeCell ref="B1296:F1296"/>
-    <mergeCell ref="B1285:F1285"/>
-    <mergeCell ref="B1286:F1286"/>
-    <mergeCell ref="B1287:F1287"/>
-    <mergeCell ref="B1288:F1288"/>
-    <mergeCell ref="B1289:F1289"/>
-    <mergeCell ref="B1290:F1290"/>
-    <mergeCell ref="B1279:F1279"/>
-    <mergeCell ref="B1280:F1280"/>
-    <mergeCell ref="B1281:F1281"/>
-    <mergeCell ref="B1282:F1282"/>
-    <mergeCell ref="B1283:F1283"/>
-    <mergeCell ref="B1284:F1284"/>
-    <mergeCell ref="B1273:F1273"/>
-    <mergeCell ref="B1274:F1274"/>
-    <mergeCell ref="B1275:F1275"/>
-    <mergeCell ref="B1276:F1276"/>
-    <mergeCell ref="B1277:F1277"/>
-    <mergeCell ref="B1278:F1278"/>
-    <mergeCell ref="B1267:F1267"/>
-    <mergeCell ref="B1268:F1268"/>
-    <mergeCell ref="B1269:F1269"/>
-    <mergeCell ref="B1270:F1270"/>
-    <mergeCell ref="B1271:F1271"/>
-    <mergeCell ref="B1272:F1272"/>
-    <mergeCell ref="B1261:F1261"/>
-    <mergeCell ref="B1262:F1262"/>
-    <mergeCell ref="B1263:F1263"/>
-    <mergeCell ref="B1264:F1264"/>
-    <mergeCell ref="B1265:F1265"/>
-    <mergeCell ref="B1266:F1266"/>
-    <mergeCell ref="B1255:F1255"/>
-    <mergeCell ref="B1256:F1256"/>
-    <mergeCell ref="B1257:F1257"/>
-    <mergeCell ref="B1258:F1258"/>
-    <mergeCell ref="B1259:F1259"/>
-    <mergeCell ref="B1260:F1260"/>
-    <mergeCell ref="B1249:F1249"/>
-    <mergeCell ref="B1250:F1250"/>
-    <mergeCell ref="B1251:F1251"/>
-    <mergeCell ref="B1252:F1252"/>
-    <mergeCell ref="B1253:F1253"/>
-    <mergeCell ref="B1254:F1254"/>
-    <mergeCell ref="B1243:F1243"/>
-    <mergeCell ref="B1244:F1244"/>
-    <mergeCell ref="B1245:F1245"/>
-    <mergeCell ref="B1246:F1246"/>
-    <mergeCell ref="B1247:F1247"/>
-    <mergeCell ref="B1248:F1248"/>
-    <mergeCell ref="B1237:F1237"/>
-    <mergeCell ref="B1238:F1238"/>
-    <mergeCell ref="B1239:F1239"/>
-    <mergeCell ref="B1240:F1240"/>
-    <mergeCell ref="B1241:F1241"/>
-    <mergeCell ref="B1242:F1242"/>
-    <mergeCell ref="B1231:F1231"/>
-    <mergeCell ref="B1232:F1232"/>
-    <mergeCell ref="B1233:F1233"/>
-    <mergeCell ref="B1234:F1234"/>
-    <mergeCell ref="B1235:F1235"/>
-    <mergeCell ref="B1236:F1236"/>
-    <mergeCell ref="B1225:F1225"/>
-    <mergeCell ref="B1226:F1226"/>
-    <mergeCell ref="B1227:F1227"/>
-    <mergeCell ref="B1228:F1228"/>
-    <mergeCell ref="B1229:F1229"/>
-    <mergeCell ref="B1230:F1230"/>
-    <mergeCell ref="B1219:F1219"/>
-    <mergeCell ref="B1220:F1220"/>
-    <mergeCell ref="B1221:F1221"/>
-    <mergeCell ref="B1222:F1222"/>
-    <mergeCell ref="B1223:F1223"/>
-    <mergeCell ref="B1224:F1224"/>
-    <mergeCell ref="B1213:F1213"/>
-    <mergeCell ref="B1214:F1214"/>
-    <mergeCell ref="B1215:F1215"/>
-    <mergeCell ref="B1216:F1216"/>
-    <mergeCell ref="B1217:F1217"/>
-    <mergeCell ref="B1218:F1218"/>
-    <mergeCell ref="B1207:F1207"/>
-    <mergeCell ref="B1208:F1208"/>
-    <mergeCell ref="B1209:F1209"/>
-    <mergeCell ref="B1210:F1210"/>
-    <mergeCell ref="B1211:F1211"/>
-    <mergeCell ref="B1212:F1212"/>
-    <mergeCell ref="B1201:F1201"/>
-    <mergeCell ref="B1202:F1202"/>
-    <mergeCell ref="B1203:F1203"/>
-    <mergeCell ref="B1204:F1204"/>
-    <mergeCell ref="B1205:F1205"/>
-    <mergeCell ref="B1206:F1206"/>
-    <mergeCell ref="B1195:F1195"/>
-    <mergeCell ref="B1196:F1196"/>
-    <mergeCell ref="B1197:F1197"/>
-    <mergeCell ref="B1198:F1198"/>
-    <mergeCell ref="B1199:F1199"/>
-    <mergeCell ref="B1200:F1200"/>
-    <mergeCell ref="B1189:F1189"/>
-    <mergeCell ref="B1190:F1190"/>
-    <mergeCell ref="B1191:F1191"/>
-    <mergeCell ref="B1192:F1192"/>
-    <mergeCell ref="B1193:F1193"/>
-    <mergeCell ref="B1194:F1194"/>
-    <mergeCell ref="B1183:F1183"/>
-    <mergeCell ref="B1184:F1184"/>
-    <mergeCell ref="B1185:F1185"/>
-    <mergeCell ref="B1186:F1186"/>
-    <mergeCell ref="B1187:F1187"/>
-    <mergeCell ref="B1188:F1188"/>
-    <mergeCell ref="B1177:F1177"/>
-    <mergeCell ref="B1178:F1178"/>
-    <mergeCell ref="B1179:F1179"/>
-    <mergeCell ref="B1180:F1180"/>
-    <mergeCell ref="B1181:F1181"/>
-    <mergeCell ref="B1182:F1182"/>
-    <mergeCell ref="B1171:F1171"/>
-    <mergeCell ref="B1172:F1172"/>
-    <mergeCell ref="B1173:F1173"/>
-    <mergeCell ref="B1174:F1174"/>
-    <mergeCell ref="B1175:F1175"/>
-    <mergeCell ref="B1176:F1176"/>
-    <mergeCell ref="B1165:F1165"/>
-    <mergeCell ref="B1166:F1166"/>
-    <mergeCell ref="B1167:F1167"/>
-    <mergeCell ref="B1168:F1168"/>
-    <mergeCell ref="B1169:F1169"/>
-    <mergeCell ref="B1170:F1170"/>
-    <mergeCell ref="B1159:F1159"/>
-    <mergeCell ref="B1160:F1160"/>
-    <mergeCell ref="B1161:F1161"/>
-    <mergeCell ref="B1162:F1162"/>
-    <mergeCell ref="B1163:F1163"/>
-    <mergeCell ref="B1164:F1164"/>
-    <mergeCell ref="B1153:F1153"/>
-    <mergeCell ref="B1154:F1154"/>
-    <mergeCell ref="B1155:F1155"/>
-    <mergeCell ref="B1156:F1156"/>
-    <mergeCell ref="B1157:F1157"/>
-    <mergeCell ref="B1158:F1158"/>
-    <mergeCell ref="B1147:F1147"/>
-    <mergeCell ref="B1148:F1148"/>
-    <mergeCell ref="B1149:F1149"/>
-    <mergeCell ref="B1150:F1150"/>
-    <mergeCell ref="B1151:F1151"/>
-    <mergeCell ref="B1152:F1152"/>
-    <mergeCell ref="B1141:F1141"/>
-    <mergeCell ref="B1142:F1142"/>
-    <mergeCell ref="B1143:F1143"/>
-    <mergeCell ref="B1144:F1144"/>
-    <mergeCell ref="B1145:F1145"/>
-    <mergeCell ref="B1146:F1146"/>
-    <mergeCell ref="B1135:F1135"/>
-    <mergeCell ref="B1136:F1136"/>
-    <mergeCell ref="B1137:F1137"/>
-    <mergeCell ref="B1138:F1138"/>
-    <mergeCell ref="B1139:F1139"/>
-    <mergeCell ref="B1140:F1140"/>
-    <mergeCell ref="B1129:F1129"/>
-    <mergeCell ref="B1130:F1130"/>
-    <mergeCell ref="B1131:F1131"/>
-    <mergeCell ref="B1132:F1132"/>
-    <mergeCell ref="B1133:F1133"/>
-    <mergeCell ref="B1134:F1134"/>
-    <mergeCell ref="B1123:F1123"/>
-    <mergeCell ref="B1124:F1124"/>
-    <mergeCell ref="B1125:F1125"/>
-    <mergeCell ref="B1126:F1126"/>
-    <mergeCell ref="B1127:F1127"/>
-    <mergeCell ref="B1128:F1128"/>
-    <mergeCell ref="B1117:F1117"/>
-    <mergeCell ref="B1118:F1118"/>
-    <mergeCell ref="B1119:F1119"/>
-    <mergeCell ref="B1120:F1120"/>
-    <mergeCell ref="B1121:F1121"/>
-    <mergeCell ref="B1122:F1122"/>
-    <mergeCell ref="B1111:F1111"/>
-    <mergeCell ref="B1112:F1112"/>
-    <mergeCell ref="B1113:F1113"/>
-    <mergeCell ref="B1114:F1114"/>
-    <mergeCell ref="B1115:F1115"/>
-    <mergeCell ref="B1116:F1116"/>
-    <mergeCell ref="B1105:F1105"/>
-    <mergeCell ref="B1106:F1106"/>
-    <mergeCell ref="B1107:F1107"/>
-    <mergeCell ref="B1108:F1108"/>
-    <mergeCell ref="B1109:F1109"/>
-    <mergeCell ref="B1110:F1110"/>
-    <mergeCell ref="B1099:F1099"/>
-    <mergeCell ref="B1100:F1100"/>
-    <mergeCell ref="B1101:F1101"/>
-    <mergeCell ref="B1102:F1102"/>
-    <mergeCell ref="B1103:F1103"/>
-    <mergeCell ref="B1104:F1104"/>
-    <mergeCell ref="B1093:F1093"/>
-    <mergeCell ref="B1094:F1094"/>
-    <mergeCell ref="B1095:F1095"/>
-    <mergeCell ref="B1096:F1096"/>
-    <mergeCell ref="B1097:F1097"/>
-    <mergeCell ref="B1098:F1098"/>
-    <mergeCell ref="B1087:F1087"/>
-    <mergeCell ref="B1088:F1088"/>
-    <mergeCell ref="B1089:F1089"/>
-    <mergeCell ref="B1090:F1090"/>
-    <mergeCell ref="B1091:F1091"/>
-    <mergeCell ref="B1092:F1092"/>
-    <mergeCell ref="B1081:F1081"/>
-    <mergeCell ref="B1082:F1082"/>
-    <mergeCell ref="B1083:F1083"/>
-    <mergeCell ref="B1084:F1084"/>
-    <mergeCell ref="B1085:F1085"/>
-    <mergeCell ref="B1086:F1086"/>
-    <mergeCell ref="B1075:F1075"/>
-    <mergeCell ref="B1076:F1076"/>
-    <mergeCell ref="B1077:F1077"/>
-    <mergeCell ref="B1078:F1078"/>
-    <mergeCell ref="B1079:F1079"/>
-    <mergeCell ref="B1080:F1080"/>
-    <mergeCell ref="B1069:F1069"/>
-    <mergeCell ref="B1070:F1070"/>
-    <mergeCell ref="B1071:F1071"/>
-    <mergeCell ref="B1072:F1072"/>
-    <mergeCell ref="B1073:F1073"/>
-    <mergeCell ref="B1074:F1074"/>
-    <mergeCell ref="B1063:F1063"/>
-    <mergeCell ref="B1064:F1064"/>
-    <mergeCell ref="B1065:F1065"/>
-    <mergeCell ref="B1066:F1066"/>
-    <mergeCell ref="B1067:F1067"/>
-    <mergeCell ref="B1068:F1068"/>
-    <mergeCell ref="B1057:F1057"/>
-    <mergeCell ref="B1058:F1058"/>
-    <mergeCell ref="B1059:F1059"/>
-    <mergeCell ref="B1060:F1060"/>
-    <mergeCell ref="B1061:F1061"/>
-    <mergeCell ref="B1062:F1062"/>
-    <mergeCell ref="B1051:F1051"/>
-    <mergeCell ref="B1052:F1052"/>
-    <mergeCell ref="B1053:F1053"/>
-    <mergeCell ref="B1054:F1054"/>
-    <mergeCell ref="B1055:F1055"/>
-    <mergeCell ref="B1056:F1056"/>
-    <mergeCell ref="B1045:F1045"/>
-    <mergeCell ref="B1046:F1046"/>
-    <mergeCell ref="B1047:F1047"/>
-    <mergeCell ref="B1048:F1048"/>
-    <mergeCell ref="B1049:F1049"/>
-    <mergeCell ref="B1050:F1050"/>
-    <mergeCell ref="B1039:F1039"/>
-    <mergeCell ref="B1040:F1040"/>
-    <mergeCell ref="B1041:F1041"/>
-    <mergeCell ref="B1042:F1042"/>
-    <mergeCell ref="B1043:F1043"/>
-    <mergeCell ref="B1044:F1044"/>
-    <mergeCell ref="B1033:F1033"/>
-    <mergeCell ref="B1034:F1034"/>
-    <mergeCell ref="B1035:F1035"/>
-    <mergeCell ref="B1036:F1036"/>
-    <mergeCell ref="B1037:F1037"/>
-    <mergeCell ref="B1038:F1038"/>
-    <mergeCell ref="B1027:F1027"/>
-    <mergeCell ref="B1028:F1028"/>
-    <mergeCell ref="B1029:F1029"/>
-    <mergeCell ref="B1030:F1030"/>
-    <mergeCell ref="B1031:F1031"/>
-    <mergeCell ref="B1032:F1032"/>
-    <mergeCell ref="B1021:F1021"/>
-    <mergeCell ref="B1022:F1022"/>
-    <mergeCell ref="B1023:F1023"/>
-    <mergeCell ref="B1024:F1024"/>
-    <mergeCell ref="B1025:F1025"/>
-    <mergeCell ref="B1026:F1026"/>
-    <mergeCell ref="B1015:F1015"/>
-    <mergeCell ref="B1016:F1016"/>
-    <mergeCell ref="B1017:F1017"/>
-    <mergeCell ref="B1018:F1018"/>
-    <mergeCell ref="B1019:F1019"/>
-    <mergeCell ref="B1020:F1020"/>
-    <mergeCell ref="B1009:F1009"/>
-    <mergeCell ref="B1010:F1010"/>
-    <mergeCell ref="B1011:F1011"/>
-    <mergeCell ref="B1012:F1012"/>
-    <mergeCell ref="B1013:F1013"/>
-    <mergeCell ref="B1014:F1014"/>
-    <mergeCell ref="B1003:F1003"/>
-    <mergeCell ref="B1004:F1004"/>
-    <mergeCell ref="B1005:F1005"/>
-    <mergeCell ref="B1006:F1006"/>
-    <mergeCell ref="B1007:F1007"/>
-    <mergeCell ref="B1008:F1008"/>
-    <mergeCell ref="B997:F997"/>
-    <mergeCell ref="B998:F998"/>
-    <mergeCell ref="B999:F999"/>
-    <mergeCell ref="B1000:F1000"/>
-    <mergeCell ref="B1001:F1001"/>
-    <mergeCell ref="B1002:F1002"/>
-    <mergeCell ref="B991:F991"/>
-    <mergeCell ref="B992:F992"/>
-    <mergeCell ref="B993:F993"/>
-    <mergeCell ref="B994:F994"/>
-    <mergeCell ref="B995:F995"/>
-    <mergeCell ref="B996:F996"/>
-    <mergeCell ref="B985:F985"/>
-    <mergeCell ref="B986:F986"/>
-    <mergeCell ref="B987:F987"/>
-    <mergeCell ref="B988:F988"/>
-    <mergeCell ref="B989:F989"/>
-    <mergeCell ref="B990:F990"/>
-    <mergeCell ref="B979:F979"/>
-    <mergeCell ref="B980:F980"/>
-    <mergeCell ref="B981:F981"/>
-    <mergeCell ref="B982:F982"/>
-    <mergeCell ref="B983:F983"/>
-    <mergeCell ref="B984:F984"/>
-    <mergeCell ref="B973:F973"/>
-    <mergeCell ref="B974:F974"/>
-    <mergeCell ref="B975:F975"/>
-    <mergeCell ref="B976:F976"/>
-    <mergeCell ref="B977:F977"/>
-    <mergeCell ref="B978:F978"/>
-    <mergeCell ref="B967:F967"/>
-    <mergeCell ref="B968:F968"/>
-    <mergeCell ref="B969:F969"/>
-    <mergeCell ref="B970:F970"/>
-    <mergeCell ref="B971:F971"/>
-    <mergeCell ref="B972:F972"/>
-    <mergeCell ref="B961:F961"/>
-    <mergeCell ref="B962:F962"/>
-    <mergeCell ref="B963:F963"/>
-    <mergeCell ref="B964:F964"/>
-    <mergeCell ref="B965:F965"/>
-    <mergeCell ref="B966:F966"/>
-    <mergeCell ref="B955:F955"/>
-    <mergeCell ref="B956:F956"/>
-    <mergeCell ref="B957:F957"/>
-    <mergeCell ref="B958:F958"/>
-    <mergeCell ref="B959:F959"/>
-    <mergeCell ref="B960:F960"/>
-    <mergeCell ref="B949:F949"/>
-    <mergeCell ref="B950:F950"/>
-    <mergeCell ref="B951:F951"/>
-    <mergeCell ref="B952:F952"/>
-    <mergeCell ref="B953:F953"/>
-    <mergeCell ref="B954:F954"/>
-    <mergeCell ref="B943:F943"/>
-    <mergeCell ref="B944:F944"/>
-    <mergeCell ref="B945:F945"/>
-    <mergeCell ref="B946:F946"/>
-    <mergeCell ref="B947:F947"/>
-    <mergeCell ref="B948:F948"/>
-    <mergeCell ref="B937:F937"/>
-    <mergeCell ref="B938:F938"/>
-    <mergeCell ref="B939:F939"/>
-    <mergeCell ref="B940:F940"/>
-    <mergeCell ref="B941:F941"/>
-    <mergeCell ref="B942:F942"/>
-    <mergeCell ref="B931:F931"/>
-    <mergeCell ref="B932:F932"/>
-    <mergeCell ref="B933:F933"/>
-    <mergeCell ref="B934:F934"/>
-    <mergeCell ref="B935:F935"/>
-    <mergeCell ref="B936:F936"/>
-    <mergeCell ref="B925:F925"/>
-    <mergeCell ref="B926:F926"/>
-    <mergeCell ref="B927:F927"/>
-    <mergeCell ref="B928:F928"/>
-    <mergeCell ref="B929:F929"/>
-    <mergeCell ref="B930:F930"/>
-    <mergeCell ref="B919:F919"/>
-    <mergeCell ref="B920:F920"/>
-    <mergeCell ref="B921:F921"/>
-    <mergeCell ref="B922:F922"/>
-    <mergeCell ref="B923:F923"/>
-    <mergeCell ref="B924:F924"/>
-    <mergeCell ref="B913:F913"/>
-    <mergeCell ref="B914:F914"/>
-    <mergeCell ref="B915:F915"/>
-    <mergeCell ref="B916:F916"/>
-    <mergeCell ref="B917:F917"/>
-    <mergeCell ref="B918:F918"/>
-    <mergeCell ref="B907:F907"/>
-    <mergeCell ref="B908:F908"/>
-    <mergeCell ref="B909:F909"/>
-    <mergeCell ref="B910:F910"/>
-    <mergeCell ref="B911:F911"/>
-    <mergeCell ref="B912:F912"/>
-    <mergeCell ref="B901:F901"/>
-    <mergeCell ref="B902:F902"/>
-    <mergeCell ref="B903:F903"/>
-    <mergeCell ref="B904:F904"/>
-    <mergeCell ref="B905:F905"/>
-    <mergeCell ref="B906:F906"/>
-    <mergeCell ref="B895:F895"/>
-    <mergeCell ref="B896:F896"/>
-    <mergeCell ref="B897:F897"/>
-    <mergeCell ref="B898:F898"/>
-    <mergeCell ref="B899:F899"/>
-    <mergeCell ref="B900:F900"/>
-    <mergeCell ref="B889:F889"/>
-    <mergeCell ref="B890:F890"/>
-    <mergeCell ref="B891:F891"/>
-    <mergeCell ref="B892:F892"/>
-    <mergeCell ref="B893:F893"/>
-    <mergeCell ref="B894:F894"/>
-    <mergeCell ref="B883:F883"/>
-    <mergeCell ref="B884:F884"/>
-    <mergeCell ref="B885:F885"/>
-    <mergeCell ref="B886:F886"/>
-    <mergeCell ref="B887:F887"/>
-    <mergeCell ref="B888:F888"/>
-    <mergeCell ref="B877:F877"/>
-    <mergeCell ref="B878:F878"/>
-    <mergeCell ref="B879:F879"/>
-    <mergeCell ref="B880:F880"/>
-    <mergeCell ref="B881:F881"/>
-    <mergeCell ref="B882:F882"/>
-    <mergeCell ref="B871:F871"/>
-    <mergeCell ref="B872:F872"/>
-    <mergeCell ref="B873:F873"/>
-    <mergeCell ref="B874:F874"/>
-    <mergeCell ref="B875:F875"/>
-    <mergeCell ref="B876:F876"/>
-    <mergeCell ref="B865:F865"/>
-    <mergeCell ref="B866:F866"/>
-    <mergeCell ref="B867:F867"/>
-    <mergeCell ref="B868:F868"/>
-    <mergeCell ref="B869:F869"/>
-    <mergeCell ref="B870:F870"/>
-    <mergeCell ref="B859:F859"/>
-    <mergeCell ref="B860:F860"/>
-    <mergeCell ref="B861:F861"/>
-    <mergeCell ref="B862:F862"/>
-    <mergeCell ref="B863:F863"/>
-    <mergeCell ref="B864:F864"/>
-    <mergeCell ref="B853:F853"/>
-    <mergeCell ref="B854:F854"/>
-    <mergeCell ref="B855:F855"/>
-    <mergeCell ref="B856:F856"/>
-    <mergeCell ref="B857:F857"/>
-    <mergeCell ref="B858:F858"/>
-    <mergeCell ref="B847:F847"/>
-    <mergeCell ref="B848:F848"/>
-    <mergeCell ref="B849:F849"/>
-    <mergeCell ref="B850:F850"/>
-    <mergeCell ref="B851:F851"/>
-    <mergeCell ref="B852:F852"/>
-    <mergeCell ref="B841:F841"/>
-    <mergeCell ref="B842:F842"/>
-    <mergeCell ref="B843:F843"/>
-    <mergeCell ref="B844:F844"/>
-    <mergeCell ref="B845:F845"/>
-    <mergeCell ref="B846:F846"/>
-    <mergeCell ref="B835:F835"/>
-    <mergeCell ref="B836:F836"/>
-    <mergeCell ref="B837:F837"/>
-    <mergeCell ref="B838:F838"/>
-    <mergeCell ref="B839:F839"/>
-    <mergeCell ref="B840:F840"/>
-    <mergeCell ref="B829:F829"/>
-    <mergeCell ref="B830:F830"/>
-    <mergeCell ref="B831:F831"/>
-    <mergeCell ref="B832:F832"/>
-    <mergeCell ref="B833:F833"/>
-    <mergeCell ref="B834:F834"/>
-    <mergeCell ref="B823:F823"/>
-    <mergeCell ref="B824:F824"/>
-    <mergeCell ref="B825:F825"/>
-    <mergeCell ref="B826:F826"/>
-    <mergeCell ref="B827:F827"/>
-    <mergeCell ref="B828:F828"/>
-    <mergeCell ref="B817:F817"/>
-    <mergeCell ref="B818:F818"/>
-    <mergeCell ref="B819:F819"/>
-    <mergeCell ref="B820:F820"/>
-    <mergeCell ref="B821:F821"/>
-    <mergeCell ref="B822:F822"/>
-    <mergeCell ref="B811:F811"/>
-    <mergeCell ref="B812:F812"/>
-    <mergeCell ref="B813:F813"/>
-    <mergeCell ref="B814:F814"/>
-    <mergeCell ref="B815:F815"/>
-    <mergeCell ref="B816:F816"/>
-    <mergeCell ref="B805:F805"/>
-    <mergeCell ref="B806:F806"/>
-    <mergeCell ref="B807:F807"/>
-    <mergeCell ref="B808:F808"/>
-    <mergeCell ref="B809:F809"/>
-    <mergeCell ref="B810:F810"/>
-    <mergeCell ref="B799:F799"/>
-    <mergeCell ref="B800:F800"/>
-    <mergeCell ref="B801:F801"/>
-    <mergeCell ref="B802:F802"/>
-    <mergeCell ref="B803:F803"/>
-    <mergeCell ref="B804:F804"/>
-    <mergeCell ref="B793:F793"/>
-    <mergeCell ref="B794:F794"/>
-    <mergeCell ref="B795:F795"/>
-    <mergeCell ref="B796:F796"/>
-    <mergeCell ref="B797:F797"/>
-    <mergeCell ref="B798:F798"/>
-    <mergeCell ref="B787:F787"/>
-    <mergeCell ref="B788:F788"/>
-    <mergeCell ref="B789:F789"/>
-    <mergeCell ref="B790:F790"/>
-    <mergeCell ref="B791:F791"/>
-    <mergeCell ref="B792:F792"/>
-    <mergeCell ref="B781:F781"/>
-    <mergeCell ref="B782:F782"/>
-    <mergeCell ref="B783:F783"/>
-    <mergeCell ref="B784:F784"/>
-    <mergeCell ref="B785:F785"/>
-    <mergeCell ref="B786:F786"/>
-    <mergeCell ref="B775:F775"/>
-    <mergeCell ref="B776:F776"/>
-    <mergeCell ref="B777:F777"/>
-    <mergeCell ref="B778:F778"/>
-    <mergeCell ref="B779:F779"/>
-    <mergeCell ref="B780:F780"/>
-    <mergeCell ref="B769:F769"/>
-    <mergeCell ref="B770:F770"/>
-    <mergeCell ref="B771:F771"/>
-    <mergeCell ref="B772:F772"/>
-    <mergeCell ref="B773:F773"/>
-    <mergeCell ref="B774:F774"/>
-    <mergeCell ref="B763:F763"/>
-    <mergeCell ref="B764:F764"/>
-    <mergeCell ref="B765:F765"/>
-    <mergeCell ref="B766:F766"/>
-    <mergeCell ref="B767:F767"/>
-    <mergeCell ref="B768:F768"/>
-    <mergeCell ref="B757:F757"/>
-    <mergeCell ref="B758:F758"/>
-    <mergeCell ref="B759:F759"/>
-    <mergeCell ref="B760:F760"/>
-    <mergeCell ref="B761:F761"/>
-    <mergeCell ref="B762:F762"/>
-    <mergeCell ref="B751:F751"/>
-    <mergeCell ref="B752:F752"/>
-    <mergeCell ref="B753:F753"/>
-    <mergeCell ref="B754:F754"/>
-    <mergeCell ref="B755:F755"/>
-    <mergeCell ref="B756:F756"/>
-    <mergeCell ref="B745:F745"/>
-    <mergeCell ref="B746:F746"/>
-    <mergeCell ref="B747:F747"/>
-    <mergeCell ref="B748:F748"/>
-    <mergeCell ref="B749:F749"/>
-    <mergeCell ref="B750:F750"/>
-    <mergeCell ref="B739:F739"/>
-    <mergeCell ref="B740:F740"/>
-    <mergeCell ref="B741:F741"/>
-    <mergeCell ref="B742:F742"/>
-    <mergeCell ref="B743:F743"/>
-    <mergeCell ref="B744:F744"/>
-    <mergeCell ref="B733:F733"/>
-    <mergeCell ref="B734:F734"/>
-    <mergeCell ref="B735:F735"/>
-    <mergeCell ref="B736:F736"/>
-    <mergeCell ref="B737:F737"/>
-    <mergeCell ref="B738:F738"/>
-    <mergeCell ref="B727:F727"/>
-    <mergeCell ref="B728:F728"/>
-    <mergeCell ref="B729:F729"/>
-    <mergeCell ref="B730:F730"/>
-    <mergeCell ref="B731:F731"/>
-    <mergeCell ref="B732:F732"/>
-    <mergeCell ref="B721:F721"/>
-    <mergeCell ref="B722:F722"/>
-    <mergeCell ref="B723:F723"/>
-    <mergeCell ref="B724:F724"/>
-    <mergeCell ref="B725:F725"/>
-    <mergeCell ref="B726:F726"/>
-    <mergeCell ref="B715:F715"/>
-    <mergeCell ref="B716:F716"/>
-    <mergeCell ref="B717:F717"/>
-    <mergeCell ref="B718:F718"/>
-    <mergeCell ref="B719:F719"/>
-    <mergeCell ref="B720:F720"/>
-    <mergeCell ref="B709:F709"/>
-    <mergeCell ref="B710:F710"/>
-    <mergeCell ref="B711:F711"/>
-    <mergeCell ref="B712:F712"/>
-    <mergeCell ref="B713:F713"/>
-    <mergeCell ref="B714:F714"/>
-    <mergeCell ref="B703:F703"/>
-    <mergeCell ref="B704:F704"/>
-    <mergeCell ref="B705:F705"/>
-    <mergeCell ref="B706:F706"/>
-    <mergeCell ref="B707:F707"/>
-    <mergeCell ref="B708:F708"/>
-    <mergeCell ref="B697:F697"/>
-    <mergeCell ref="B698:F698"/>
-    <mergeCell ref="B699:F699"/>
-    <mergeCell ref="B700:F700"/>
-    <mergeCell ref="B701:F701"/>
-    <mergeCell ref="B702:F702"/>
-    <mergeCell ref="B691:F691"/>
-    <mergeCell ref="B692:F692"/>
-    <mergeCell ref="B693:F693"/>
-    <mergeCell ref="B694:F694"/>
-    <mergeCell ref="B695:F695"/>
-    <mergeCell ref="B696:F696"/>
-    <mergeCell ref="B685:F685"/>
-    <mergeCell ref="B686:F686"/>
-    <mergeCell ref="B687:F687"/>
-    <mergeCell ref="B688:F688"/>
-    <mergeCell ref="B689:F689"/>
-    <mergeCell ref="B690:F690"/>
-    <mergeCell ref="B679:F679"/>
-    <mergeCell ref="B680:F680"/>
-    <mergeCell ref="B681:F681"/>
-    <mergeCell ref="B682:F682"/>
-    <mergeCell ref="B683:F683"/>
-    <mergeCell ref="B684:F684"/>
-    <mergeCell ref="B673:F673"/>
-    <mergeCell ref="B674:F674"/>
-    <mergeCell ref="B675:F675"/>
-    <mergeCell ref="B676:F676"/>
-    <mergeCell ref="B677:F677"/>
-    <mergeCell ref="B678:F678"/>
-    <mergeCell ref="B667:F667"/>
-    <mergeCell ref="B668:F668"/>
-    <mergeCell ref="B669:F669"/>
-    <mergeCell ref="B670:F670"/>
-    <mergeCell ref="B671:F671"/>
-    <mergeCell ref="B672:F672"/>
-    <mergeCell ref="B661:F661"/>
-    <mergeCell ref="B662:F662"/>
-    <mergeCell ref="B663:F663"/>
-    <mergeCell ref="B664:F664"/>
-    <mergeCell ref="B665:F665"/>
-    <mergeCell ref="B666:F666"/>
-    <mergeCell ref="B655:F655"/>
-    <mergeCell ref="B656:F656"/>
-    <mergeCell ref="B657:F657"/>
-    <mergeCell ref="B658:F658"/>
-    <mergeCell ref="B659:F659"/>
-    <mergeCell ref="B660:F660"/>
-    <mergeCell ref="B649:F649"/>
-    <mergeCell ref="B650:F650"/>
-    <mergeCell ref="B651:F651"/>
-    <mergeCell ref="B652:F652"/>
-    <mergeCell ref="B653:F653"/>
-    <mergeCell ref="B654:F654"/>
-    <mergeCell ref="B643:F643"/>
-    <mergeCell ref="B644:F644"/>
-    <mergeCell ref="B645:F645"/>
-    <mergeCell ref="B646:F646"/>
-    <mergeCell ref="B647:F647"/>
-    <mergeCell ref="B648:F648"/>
-    <mergeCell ref="B637:F637"/>
-    <mergeCell ref="B638:F638"/>
-    <mergeCell ref="B639:F639"/>
-    <mergeCell ref="B640:F640"/>
-    <mergeCell ref="B641:F641"/>
-    <mergeCell ref="B642:F642"/>
-    <mergeCell ref="B631:F631"/>
-    <mergeCell ref="B632:F632"/>
-    <mergeCell ref="B633:F633"/>
-    <mergeCell ref="B634:F634"/>
-    <mergeCell ref="B635:F635"/>
-    <mergeCell ref="B636:F636"/>
-    <mergeCell ref="B625:F625"/>
-    <mergeCell ref="B626:F626"/>
-    <mergeCell ref="B627:F627"/>
-    <mergeCell ref="B628:F628"/>
-    <mergeCell ref="B629:F629"/>
-    <mergeCell ref="B630:F630"/>
-    <mergeCell ref="B619:F619"/>
-    <mergeCell ref="B620:F620"/>
-    <mergeCell ref="B621:F621"/>
-    <mergeCell ref="B622:F622"/>
-    <mergeCell ref="B623:F623"/>
-    <mergeCell ref="B624:F624"/>
-    <mergeCell ref="B613:F613"/>
-    <mergeCell ref="B614:F614"/>
-    <mergeCell ref="B615:F615"/>
-    <mergeCell ref="B616:F616"/>
-    <mergeCell ref="B617:F617"/>
-    <mergeCell ref="B618:F618"/>
-    <mergeCell ref="B607:F607"/>
-    <mergeCell ref="B608:F608"/>
-    <mergeCell ref="B609:F609"/>
-    <mergeCell ref="B610:F610"/>
-    <mergeCell ref="B611:F611"/>
-    <mergeCell ref="B612:F612"/>
-    <mergeCell ref="B601:F601"/>
-    <mergeCell ref="B602:F602"/>
-    <mergeCell ref="B603:F603"/>
-    <mergeCell ref="B604:F604"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="B606:F606"/>
-    <mergeCell ref="B595:F595"/>
-    <mergeCell ref="B596:F596"/>
-    <mergeCell ref="B597:F597"/>
-    <mergeCell ref="B598:F598"/>
-    <mergeCell ref="B599:F599"/>
-    <mergeCell ref="B600:F600"/>
-    <mergeCell ref="B589:F589"/>
-    <mergeCell ref="B590:F590"/>
-    <mergeCell ref="B591:F591"/>
-    <mergeCell ref="B592:F592"/>
-    <mergeCell ref="B593:F593"/>
-    <mergeCell ref="B594:F594"/>
-    <mergeCell ref="B583:F583"/>
-    <mergeCell ref="B584:F584"/>
-    <mergeCell ref="B585:F585"/>
-    <mergeCell ref="B586:F586"/>
-    <mergeCell ref="B587:F587"/>
-    <mergeCell ref="B588:F588"/>
-    <mergeCell ref="B577:F577"/>
-    <mergeCell ref="B578:F578"/>
-    <mergeCell ref="B579:F579"/>
-    <mergeCell ref="B580:F580"/>
-    <mergeCell ref="B581:F581"/>
-    <mergeCell ref="B582:F582"/>
-    <mergeCell ref="B571:F571"/>
-    <mergeCell ref="B572:F572"/>
-    <mergeCell ref="B573:F573"/>
-    <mergeCell ref="B574:F574"/>
-    <mergeCell ref="B575:F575"/>
-    <mergeCell ref="B576:F576"/>
-    <mergeCell ref="B565:F565"/>
-    <mergeCell ref="B566:F566"/>
-    <mergeCell ref="B567:F567"/>
-    <mergeCell ref="B568:F568"/>
-    <mergeCell ref="B569:F569"/>
-    <mergeCell ref="B570:F570"/>
-    <mergeCell ref="B559:F559"/>
-    <mergeCell ref="B560:F560"/>
-    <mergeCell ref="B561:F561"/>
-    <mergeCell ref="B562:F562"/>
-    <mergeCell ref="B563:F563"/>
-    <mergeCell ref="B564:F564"/>
-    <mergeCell ref="B553:F553"/>
-    <mergeCell ref="B554:F554"/>
-    <mergeCell ref="B555:F555"/>
-    <mergeCell ref="B556:F556"/>
-    <mergeCell ref="B557:F557"/>
-    <mergeCell ref="B558:F558"/>
-    <mergeCell ref="B547:F547"/>
-    <mergeCell ref="B548:F548"/>
-    <mergeCell ref="B549:F549"/>
-    <mergeCell ref="B550:F550"/>
-    <mergeCell ref="B551:F551"/>
-    <mergeCell ref="B552:F552"/>
-    <mergeCell ref="B541:F541"/>
-    <mergeCell ref="B542:F542"/>
-    <mergeCell ref="B543:F543"/>
-    <mergeCell ref="B544:F544"/>
-    <mergeCell ref="B545:F545"/>
-    <mergeCell ref="B546:F546"/>
-    <mergeCell ref="B535:F535"/>
-    <mergeCell ref="B536:F536"/>
-    <mergeCell ref="B537:F537"/>
-    <mergeCell ref="B538:F538"/>
-    <mergeCell ref="B539:F539"/>
-    <mergeCell ref="B540:F540"/>
-    <mergeCell ref="B529:F529"/>
-    <mergeCell ref="B530:F530"/>
-    <mergeCell ref="B531:F531"/>
-    <mergeCell ref="B532:F532"/>
-    <mergeCell ref="B533:F533"/>
-    <mergeCell ref="B534:F534"/>
-    <mergeCell ref="B523:F523"/>
-    <mergeCell ref="B524:F524"/>
-    <mergeCell ref="B525:F525"/>
-    <mergeCell ref="B526:F526"/>
-    <mergeCell ref="B527:F527"/>
-    <mergeCell ref="B528:F528"/>
-    <mergeCell ref="B517:F517"/>
-    <mergeCell ref="B518:F518"/>
-    <mergeCell ref="B519:F519"/>
-    <mergeCell ref="B520:F520"/>
-    <mergeCell ref="B521:F521"/>
-    <mergeCell ref="B522:F522"/>
-    <mergeCell ref="B511:F511"/>
-    <mergeCell ref="B512:F512"/>
-    <mergeCell ref="B513:F513"/>
-    <mergeCell ref="B514:F514"/>
-    <mergeCell ref="B515:F515"/>
-    <mergeCell ref="B516:F516"/>
-    <mergeCell ref="B505:F505"/>
-    <mergeCell ref="B506:F506"/>
-    <mergeCell ref="B507:F507"/>
-    <mergeCell ref="B508:F508"/>
-    <mergeCell ref="B509:F509"/>
-    <mergeCell ref="B510:F510"/>
-    <mergeCell ref="B499:F499"/>
-    <mergeCell ref="B500:F500"/>
-    <mergeCell ref="B501:F501"/>
-    <mergeCell ref="B502:F502"/>
-    <mergeCell ref="B503:F503"/>
-    <mergeCell ref="B504:F504"/>
-    <mergeCell ref="B493:F493"/>
-    <mergeCell ref="B494:F494"/>
-    <mergeCell ref="B495:F495"/>
-    <mergeCell ref="B496:F496"/>
-    <mergeCell ref="B497:F497"/>
-    <mergeCell ref="B498:F498"/>
-    <mergeCell ref="B487:F487"/>
-    <mergeCell ref="B488:F488"/>
-    <mergeCell ref="B489:F489"/>
-    <mergeCell ref="B490:F490"/>
-    <mergeCell ref="B491:F491"/>
-    <mergeCell ref="B492:F492"/>
-    <mergeCell ref="B481:F481"/>
-    <mergeCell ref="B482:F482"/>
-    <mergeCell ref="B483:F483"/>
-    <mergeCell ref="B484:F484"/>
-    <mergeCell ref="B485:F485"/>
-    <mergeCell ref="B486:F486"/>
-    <mergeCell ref="B475:F475"/>
-    <mergeCell ref="B476:F476"/>
-    <mergeCell ref="B477:F477"/>
-    <mergeCell ref="B478:F478"/>
-    <mergeCell ref="B479:F479"/>
-    <mergeCell ref="B480:F480"/>
-    <mergeCell ref="B469:F469"/>
-    <mergeCell ref="B470:F470"/>
-    <mergeCell ref="B471:F471"/>
-    <mergeCell ref="B472:F472"/>
-    <mergeCell ref="B473:F473"/>
-    <mergeCell ref="B474:F474"/>
-    <mergeCell ref="B463:F463"/>
-    <mergeCell ref="B464:F464"/>
-    <mergeCell ref="B465:F465"/>
-    <mergeCell ref="B466:F466"/>
-    <mergeCell ref="B467:F467"/>
-    <mergeCell ref="B468:F468"/>
-    <mergeCell ref="B457:F457"/>
-    <mergeCell ref="B458:F458"/>
-    <mergeCell ref="B459:F459"/>
-    <mergeCell ref="B460:F460"/>
-    <mergeCell ref="B461:F461"/>
-    <mergeCell ref="B462:F462"/>
-    <mergeCell ref="B451:F451"/>
-    <mergeCell ref="B452:F452"/>
-    <mergeCell ref="B453:F453"/>
-    <mergeCell ref="B454:F454"/>
-    <mergeCell ref="B455:F455"/>
-    <mergeCell ref="B456:F456"/>
-    <mergeCell ref="B445:F445"/>
-    <mergeCell ref="B446:F446"/>
-    <mergeCell ref="B447:F447"/>
-    <mergeCell ref="B448:F448"/>
-    <mergeCell ref="B449:F449"/>
-    <mergeCell ref="B450:F450"/>
-    <mergeCell ref="B439:F439"/>
-    <mergeCell ref="B440:F440"/>
-    <mergeCell ref="B441:F441"/>
-    <mergeCell ref="B442:F442"/>
-    <mergeCell ref="B443:F443"/>
-    <mergeCell ref="B444:F444"/>
-    <mergeCell ref="B433:F433"/>
-    <mergeCell ref="B434:F434"/>
-    <mergeCell ref="B435:F435"/>
-    <mergeCell ref="B436:F436"/>
-    <mergeCell ref="B437:F437"/>
-    <mergeCell ref="B438:F438"/>
-    <mergeCell ref="B427:F427"/>
-    <mergeCell ref="B428:F428"/>
-    <mergeCell ref="B429:F429"/>
-    <mergeCell ref="B430:F430"/>
-    <mergeCell ref="B431:F431"/>
-    <mergeCell ref="B432:F432"/>
-    <mergeCell ref="B421:F421"/>
-    <mergeCell ref="B422:F422"/>
-    <mergeCell ref="B423:F423"/>
-    <mergeCell ref="B424:F424"/>
-    <mergeCell ref="B425:F425"/>
-    <mergeCell ref="B426:F426"/>
-    <mergeCell ref="B415:F415"/>
-    <mergeCell ref="B416:F416"/>
-    <mergeCell ref="B417:F417"/>
-    <mergeCell ref="B418:F418"/>
-    <mergeCell ref="B419:F419"/>
-    <mergeCell ref="B420:F420"/>
-    <mergeCell ref="B409:F409"/>
-    <mergeCell ref="B410:F410"/>
-    <mergeCell ref="B411:F411"/>
-    <mergeCell ref="B412:F412"/>
-    <mergeCell ref="B413:F413"/>
-    <mergeCell ref="B414:F414"/>
-    <mergeCell ref="B403:F403"/>
-    <mergeCell ref="B404:F404"/>
-    <mergeCell ref="B405:F405"/>
-    <mergeCell ref="B406:F406"/>
-    <mergeCell ref="B407:F407"/>
-    <mergeCell ref="B408:F408"/>
-    <mergeCell ref="B397:F397"/>
-    <mergeCell ref="B398:F398"/>
-    <mergeCell ref="B399:F399"/>
-    <mergeCell ref="B400:F400"/>
-    <mergeCell ref="B401:F401"/>
-    <mergeCell ref="B402:F402"/>
-    <mergeCell ref="B391:F391"/>
-    <mergeCell ref="B392:F392"/>
-    <mergeCell ref="B393:F393"/>
-    <mergeCell ref="B394:F394"/>
-    <mergeCell ref="B395:F395"/>
-    <mergeCell ref="B396:F396"/>
-    <mergeCell ref="B385:F385"/>
-    <mergeCell ref="B386:F386"/>
-    <mergeCell ref="B387:F387"/>
-    <mergeCell ref="B388:F388"/>
-    <mergeCell ref="B389:F389"/>
-    <mergeCell ref="B390:F390"/>
-    <mergeCell ref="B379:F379"/>
-    <mergeCell ref="B380:F380"/>
-    <mergeCell ref="B381:F381"/>
-    <mergeCell ref="B382:F382"/>
-    <mergeCell ref="B383:F383"/>
-    <mergeCell ref="B384:F384"/>
-    <mergeCell ref="B373:F373"/>
-    <mergeCell ref="B374:F374"/>
-    <mergeCell ref="B375:F375"/>
-    <mergeCell ref="B376:F376"/>
-    <mergeCell ref="B377:F377"/>
-    <mergeCell ref="B378:F378"/>
-    <mergeCell ref="B367:F367"/>
-    <mergeCell ref="B368:F368"/>
-    <mergeCell ref="B369:F369"/>
-    <mergeCell ref="B370:F370"/>
-    <mergeCell ref="B371:F371"/>
-    <mergeCell ref="B372:F372"/>
-    <mergeCell ref="B361:F361"/>
-    <mergeCell ref="B362:F362"/>
-    <mergeCell ref="B363:F363"/>
-    <mergeCell ref="B364:F364"/>
-    <mergeCell ref="B365:F365"/>
-    <mergeCell ref="B366:F366"/>
-    <mergeCell ref="B355:F355"/>
-    <mergeCell ref="B356:F356"/>
-    <mergeCell ref="B357:F357"/>
-    <mergeCell ref="B358:F358"/>
-    <mergeCell ref="B359:F359"/>
-    <mergeCell ref="B360:F360"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="B350:F350"/>
-    <mergeCell ref="B351:F351"/>
-    <mergeCell ref="B352:F352"/>
-    <mergeCell ref="B353:F353"/>
-    <mergeCell ref="B354:F354"/>
-    <mergeCell ref="B343:F343"/>
-    <mergeCell ref="B344:F344"/>
-    <mergeCell ref="B345:F345"/>
-    <mergeCell ref="B346:F346"/>
-    <mergeCell ref="B347:F347"/>
-    <mergeCell ref="B348:F348"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B339:F339"/>
-    <mergeCell ref="B340:F340"/>
-    <mergeCell ref="B341:F341"/>
-    <mergeCell ref="B342:F342"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B335:F335"/>
-    <mergeCell ref="B336:F336"/>
-    <mergeCell ref="B325:F325"/>
-    <mergeCell ref="B326:F326"/>
-    <mergeCell ref="B327:F327"/>
-    <mergeCell ref="B328:F328"/>
-    <mergeCell ref="B329:F329"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B320:F320"/>
-    <mergeCell ref="B321:F321"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="B323:F323"/>
-    <mergeCell ref="B324:F324"/>
-    <mergeCell ref="B313:F313"/>
-    <mergeCell ref="B314:F314"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="B311:F311"/>
-    <mergeCell ref="B312:F312"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B306:F306"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B296:F296"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B299:F299"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="B289:F289"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B292:F292"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="B288:F288"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B282:F282"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="B275:F275"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="B265:F265"/>
-    <mergeCell ref="B266:F266"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B260:F260"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B263:F263"/>
-    <mergeCell ref="B264:F264"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B247:F247"/>
-    <mergeCell ref="B248:F248"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B242:F242"/>
-    <mergeCell ref="B243:F243"/>
-    <mergeCell ref="B244:F244"/>
-    <mergeCell ref="B245:F245"/>
-    <mergeCell ref="B246:F246"/>
-    <mergeCell ref="B235:F235"/>
-    <mergeCell ref="B236:F236"/>
-    <mergeCell ref="B237:F237"/>
-    <mergeCell ref="B238:F238"/>
-    <mergeCell ref="B239:F239"/>
-    <mergeCell ref="B240:F240"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="B230:F230"/>
-    <mergeCell ref="B231:F231"/>
-    <mergeCell ref="B232:F232"/>
-    <mergeCell ref="B233:F233"/>
-    <mergeCell ref="B234:F234"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B224:F224"/>
-    <mergeCell ref="B225:F225"/>
-    <mergeCell ref="B226:F226"/>
-    <mergeCell ref="B227:F227"/>
-    <mergeCell ref="B228:F228"/>
-    <mergeCell ref="B217:F217"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B219:F219"/>
-    <mergeCell ref="B220:F220"/>
-    <mergeCell ref="B221:F221"/>
-    <mergeCell ref="B222:F222"/>
-    <mergeCell ref="B211:F211"/>
-    <mergeCell ref="B212:F212"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B214:F214"/>
-    <mergeCell ref="B215:F215"/>
-    <mergeCell ref="B216:F216"/>
-    <mergeCell ref="B205:F205"/>
-    <mergeCell ref="B206:F206"/>
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B209:F209"/>
-    <mergeCell ref="B210:F210"/>
-    <mergeCell ref="B199:F199"/>
-    <mergeCell ref="B200:F200"/>
-    <mergeCell ref="B201:F201"/>
-    <mergeCell ref="B202:F202"/>
-    <mergeCell ref="B203:F203"/>
-    <mergeCell ref="B204:F204"/>
-    <mergeCell ref="B193:F193"/>
-    <mergeCell ref="B194:F194"/>
-    <mergeCell ref="B195:F195"/>
-    <mergeCell ref="B196:F196"/>
-    <mergeCell ref="B197:F197"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B187:F187"/>
-    <mergeCell ref="B188:F188"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B190:F190"/>
-    <mergeCell ref="B191:F191"/>
-    <mergeCell ref="B192:F192"/>
-    <mergeCell ref="B181:F181"/>
-    <mergeCell ref="B182:F182"/>
-    <mergeCell ref="B183:F183"/>
-    <mergeCell ref="B184:F184"/>
-    <mergeCell ref="B185:F185"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B175:F175"/>
-    <mergeCell ref="B176:F176"/>
-    <mergeCell ref="B177:F177"/>
-    <mergeCell ref="B178:F178"/>
-    <mergeCell ref="B179:F179"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B169:F169"/>
-    <mergeCell ref="B170:F170"/>
-    <mergeCell ref="B171:F171"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B173:F173"/>
-    <mergeCell ref="B174:F174"/>
-    <mergeCell ref="B163:F163"/>
-    <mergeCell ref="B164:F164"/>
-    <mergeCell ref="B165:F165"/>
-    <mergeCell ref="B166:F166"/>
-    <mergeCell ref="B167:F167"/>
-    <mergeCell ref="B168:F168"/>
-    <mergeCell ref="B157:F157"/>
-    <mergeCell ref="B158:F158"/>
-    <mergeCell ref="B159:F159"/>
-    <mergeCell ref="B160:F160"/>
-    <mergeCell ref="B161:F161"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B151:F151"/>
-    <mergeCell ref="B152:F152"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B154:F154"/>
-    <mergeCell ref="B155:F155"/>
-    <mergeCell ref="B156:F156"/>
-    <mergeCell ref="B145:F145"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="B147:F147"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B150:F150"/>
-    <mergeCell ref="B139:F139"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B144:F144"/>
-    <mergeCell ref="B133:F133"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B135:F135"/>
-    <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B137:F137"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B127:F127"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B130:F130"/>
-    <mergeCell ref="B131:F131"/>
-    <mergeCell ref="B132:F132"/>
-    <mergeCell ref="B121:F121"/>
-    <mergeCell ref="B122:F122"/>
-    <mergeCell ref="B123:F123"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B117:F117"/>
-    <mergeCell ref="B118:F118"/>
-    <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B109:F109"/>
-    <mergeCell ref="B110:F110"/>
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="B105:F105"/>
-    <mergeCell ref="B106:F106"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B81:F81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B77:F77"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>